<commit_message>
solucion conteo de localizacion se sigue viendo datos con cero por que???
</commit_message>
<xml_diff>
--- a/ExcelFile.xlsx
+++ b/ExcelFile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="308">
   <si>
     <t>Categoría</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Intenso /fortalecimiento</t>
   </si>
   <si>
-    <t>[{"title":"FENÓMENO EL NIÑO Y CAPTACIÓN ILEGAL DE AGUA ...","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/2313-fenomeno-el-nino-y-captacion-ilegal-..."},{"title":"Situación de la violencia feminicidia y femicida en Cúcuta ...","displayLink":"reliefweb.int","formattedUrl":"https://reliefweb.int/.../situacion-de-la-violencia-feminicidia-y-femicida-en-..."},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-63323077"},{"title":"Versión debilitada de La Niña aleja temores de pérdidas de soja y ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../granos-sudamerica-clima-idLTAKCN10722L/"},{"title":"Los caminantes venezolanos | Human Rights Watch","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/es/news/2018/09/05/los-caminantes-venezolanos"},{"title":"La OIM firme en prevenir e identificar los riesgos de explotación ...","displayLink":"colombia.iom.int","formattedUrl":"https://colombia.iom.int/.../news/la-oim-firme-en-prevenir-e-identificar-los-..."},{"title":"Heladas podrían afectar trigo de Argentina; se prevé más lluvia ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-granos-argentina-clima-idLTASI..."},{"title":"\"Aquí también hace falta ayuda\": las carencias de Cúcuta, la ciudad ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-47341759"}]</t>
+    <t>[{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"},{"title":"CIIFEN | Centro Internacional para la Investigación del Fenómeno ...","displayLink":"ciifen.org","formattedUrl":"https://ciifen.org/"},{"title":"El Niño occurrences over the past four and a half centuries - Quinn ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/10.1029/JC092iC13p14449"},{"title":"JMSE | Free Full-Text | Influence of the El Niño Phenomenon on ...","displayLink":"www.mdpi.com","formattedUrl":"https://www.mdpi.com/2077-1312/8/2/90"},{"title":"Understanding the El Niño Costero of 2017: The Definition Problem ...","displayLink":"link.springer.com","formattedUrl":"https://link.springer.com/article/10.1007/s13753-017-0151-8"},{"title":"Mapping Multi-Disease Risk during El Niño: An Ecosyndemic ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6313459/"},{"title":"Effect of extreme El Niño events on the precipitation of ... - NHESS","displayLink":"nhess.copernicus.org","formattedUrl":"https://nhess.copernicus.org/articles/23/1507/2023/"},{"title":"Root causes of recurrent catastrophe: The political ecology of El ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/pii/S2212420919302304"},{"title":"El Niño and La Niña, Explained - The New York Times","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/article/what-is-la-nina-el-nino.html"},{"title":"Frequently-(well, at least once)-asked-questions about El Niño","displayLink":"faculty.washington.edu","formattedUrl":"https://faculty.washington.edu/kessler/occasionally-asked-questions.html"}]</t>
   </si>
   <si>
     <t>[["record de temperatura","intenso "],["intenso ","record de temperatura"],["record de temperatura","fortalecimiento"],["fortalecimiento","record de temperatura"],["record de temperatura","preocupacion"],["preocupacion","record de temperatura"],["record de temperatura","agudo"],["agudo","record de temperatura"],["record de temperatura","extremo"],["extremo","record de temperatura"],["record de temperatura","aumento "],["aumento ","record de temperatura"],["record de temperatura"," aumentaria"],[" aumentaria","record de temperatura"],["record de temperatura","profundos"],["profundos","record de temperatura"],["record de temperatura","disminucion "],["disminucion ","record de temperatura"],["record de temperatura"," reduccion"],[" reduccion","record de temperatura"],["record de temperatura","grave"],["grave","record de temperatura"],["record de temperatura","emergencia"],["emergencia","record de temperatura"],["record de temperatura","crisis"],["crisis","record de temperatura"],["record de temperatura","sufrir"],["sufrir","record de temperatura"],["record de temperatura","inusual "],["inusual ","record de temperatura"],["record de temperatura","anomalo"],["anomalo","record de temperatura"],["record de temperatura","alerta"],["alerta","record de temperatura"],["record de temperatura","prolongarse"],["prolongarse","record de temperatura"],["record de temperatura","debil"],["debil","record de temperatura"],["record de temperatura","moderado"],["moderado","record de temperatura"],["record de temperatura","amenaza"],["amenaza","record de temperatura"],["record de temperatura","complejo"],["complejo","record de temperatura"],["record de temperatura","exacerbadas"],["exacerbadas","record de temperatura"],["record de temperatura","desastre"],["desastre","record de temperatura"],["alteracion ","intenso "],["intenso ","alteracion "],["alteracion ","fortalecimiento"],["fortalecimiento","alteracion "],["alteracion ","preocupacion"],["preocupacion","alteracion "],["alteracion ","agudo"],["agudo","alteracion "],["alteracion ","extremo"],["extremo","alteracion "],["alteracion ","aumento "],["aumento ","alteracion "],["alteracion "," aumentaria"],[" aumentaria","alteracion "],["alteracion ","profundos"],["profundos","alteracion "],["alteracion ","disminucion "],["disminucion ","alteracion "],["alteracion "," reduccion"],[" reduccion","alteracion "],["alteracion ","grave"],["grave","alteracion "],["alteracion ","emergencia"],["emergencia","alteracion "],["alteracion ","crisis"],["crisis","alteracion "],["alteracion ","sufrir"],["sufrir","alteracion "],["alteracion ","inusual "],["inusual ","alteracion "],["alteracion ","anomalo"],["anomalo","alteracion "],["alteracion ","alerta"],["alerta","alteracion "],["alteracion ","prolongarse"],["prolongarse","alteracion "],["alteracion ","debil"],["debil","alteracion "],["alteracion ","moderado"],["moderado","alteracion "],["alteracion ","amenaza"],["amenaza","alteracion "],["alteracion ","complejo"],["complejo","alteracion "],["alteracion ","exacerbadas"],["exacerbadas","alteracion "],["alteracion ","desastre"],["desastre","alteracion "],[" altera","intenso "],["intenso "," altera"],[" altera","fortalecimiento"],["fortalecimiento"," altera"],[" altera","preocupacion"],["preocupacion"," altera"],[" altera","agudo"],["agudo"," altera"],[" altera","extremo"],["extremo"," altera"],[" altera","aumento "],["aumento "," altera"],[" altera"," aumentaria"],[" aumentaria"," altera"],[" altera","profundos"],["profundos"," altera"],[" altera","disminucion "],["disminucion "," altera"],[" altera"," reduccion"],[" reduccion"," altera"],[" altera","grave"],["grave"," altera"],[" altera","emergencia"],["emergencia"," altera"],[" altera","crisis"],["crisis"," altera"],[" altera","sufrir"],["sufrir"," altera"],[" altera","inusual "],["inusual "," altera"],[" altera","anomalo"],["anomalo"," altera"],[" altera","alerta"],["alerta"," altera"],[" altera","prolongarse"],["prolongarse"," altera"],[" altera","debil"],["debil"," altera"],[" altera","moderado"],["moderado"," altera"],[" altera","amenaza"],["amenaza"," altera"],[" altera","complejo"],["complejo"," altera"],[" altera","exacerbadas"],["exacerbadas"," altera"],[" altera","desastre"],["desastre"," altera"],["riesgo","intenso "],["intenso ","riesgo"],["riesgo","fortalecimiento"],["fortalecimiento","riesgo"],["riesgo","preocupacion"],["preocupacion","riesgo"],["riesgo","agudo"],["agudo","riesgo"],["riesgo","extremo"],["extremo","riesgo"],["riesgo","aumento "],["aumento ","riesgo"],["riesgo"," aumentaria"],[" aumentaria","riesgo"],["riesgo","profundos"],["profundos","riesgo"],["riesgo","disminucion "],["disminucion ","riesgo"],["riesgo"," reduccion"],[" reduccion","riesgo"],["riesgo","grave"],["grave","riesgo"],["riesgo","emergencia"],["emergencia","riesgo"],["riesgo","crisis"],["crisis","riesgo"],["riesgo","sufrir"],["sufrir","riesgo"],["riesgo","inusual "],["inusual ","riesgo"],["riesgo","anomalo"],["anomalo","riesgo"],["riesgo","alerta"],["alerta","riesgo"],["riesgo","prolongarse"],["prolongarse","riesgo"],["riesgo","debil"],["debil","riesgo"],["riesgo","moderado"],["moderado","riesgo"],["riesgo","amenaza"],["amenaza","riesgo"],["riesgo","complejo"],["complejo","riesgo"],["riesgo","exacerbadas"],["exacerbadas","riesgo"],["riesgo","desastre"],["desastre","riesgo"],["caluroso","intenso "],["intenso ","caluroso"],["caluroso","fortalecimiento"],["fortalecimiento","caluroso"],["caluroso","preocupacion"],["preocupacion","caluroso"],["caluroso","agudo"],["agudo","caluroso"],["caluroso","extremo"],["extremo","caluroso"],["caluroso","aumento "],["aumento ","caluroso"],["caluroso"," aumentaria"],[" aumentaria","caluroso"],["caluroso","profundos"],["profundos","caluroso"],["caluroso","disminucion "],["disminucion ","caluroso"],["caluroso"," reduccion"],[" reduccion","caluroso"],["caluroso","grave"],["grave","caluroso"],["caluroso","emergencia"],["emergencia","caluroso"],["caluroso","crisis"],["crisis","caluroso"],["caluroso","sufrir"],["sufrir","caluroso"],["caluroso","inusual "],["inusual ","caluroso"],["caluroso","anomalo"],["anomalo","caluroso"],["caluroso","alerta"],["alerta","caluroso"],["caluroso","prolongarse"],["prolongarse","caluroso"],["caluroso","debil"],["debil","caluroso"],["caluroso","moderado"],["moderado","caluroso"],["caluroso","amenaza"],["amenaza","caluroso"],["caluroso","complejo"],["complejo","caluroso"],["caluroso","exacerbadas"],["exacerbadas","caluroso"],["caluroso","desastre"],["desastre","caluroso"],["cambios","intenso "],["intenso ","cambios"],["cambios","fortalecimiento"],["fortalecimiento","cambios"],["cambios","preocupacion"],["preocupacion","cambios"],["cambios","agudo"],["agudo","cambios"],["cambios","extremo"],["extremo","cambios"],["cambios","aumento "],["aumento ","cambios"],["cambios"," aumentaria"],[" aumentaria","cambios"],["cambios","profundos"],["profundos","cambios"],["cambios","disminucion "],["disminucion ","cambios"],["cambios"," reduccion"],[" reduccion","cambios"],["cambios","grave"],["grave","cambios"],["cambios","emergencia"],["emergencia","cambios"],["cambios","crisis"],["crisis","cambios"],["cambios","sufrir"],["sufrir","cambios"],["cambios","inusual "],["inusual ","cambios"],["cambios","anomalo"],["anomalo","cambios"],["cambios","alerta"],["alerta","cambios"],["cambios","prolongarse"],["prolongarse","cambios"],["cambios","debil"],["debil","cambios"],["cambios","moderado"],["moderado","cambios"],["cambios","amenaza"],["amenaza","cambios"],["cambios","complejo"],["complejo","cambios"],["cambios","exacerbadas"],["exacerbadas","cambios"],["cambios","desastre"],["desastre","cambios"],["efectos ","intenso "],["intenso ","efectos "],["efectos ","fortalecimiento"],["fortalecimiento","efectos "],["efectos ","preocupacion"],["preocupacion","efectos "],["efectos ","agudo"],["agudo","efectos "],["efectos ","extremo"],["extremo","efectos "],["efectos ","aumento "],["aumento ","efectos "],["efectos "," aumentaria"],[" aumentaria","efectos "],["efectos ","profundos"],["profundos","efectos "],["efectos ","disminucion "],["disminucion ","efectos "],["efectos "," reduccion"],[" reduccion","efectos "],["efectos ","grave"],["grave","efectos "],["efectos ","emergencia"],["emergencia","efectos "],["efectos ","crisis"],["crisis","efectos "],["efectos ","sufrir"],["sufrir","efectos "],["efectos ","inusual "],["inusual ","efectos "],["efectos ","anomalo"],["anomalo","efectos "],["efectos ","alerta"],["alerta","efectos "],["efectos ","prolongarse"],["prolongarse","efectos "],["efectos ","debil"],["debil","efectos "],["efectos ","moderado"],["moderado","efectos "],["efectos ","amenaza"],["amenaza","efectos "],["efectos ","complejo"],["complejo","efectos "],["efectos ","exacerbadas"],["exacerbadas","efectos "],["efectos ","desastre"],["desastre","efectos "],["efecto","intenso "],["intenso ","efecto"],["efecto","fortalecimiento"],["fortalecimiento","efecto"],["efecto","preocupacion"],["preocupacion","efecto"],["efecto","agudo"],["agudo","efecto"],["efecto","extremo"],["extremo","efecto"],["efecto","aumento "],["aumento ","efecto"],["efecto"," aumentaria"],[" aumentaria","efecto"],["efecto","profundos"],["profundos","efecto"],["efecto","disminucion "],["disminucion ","efecto"],["efecto"," reduccion"],[" reduccion","efecto"],["efecto","grave"],["grave","efecto"],["efecto","emergencia"],["emergencia","efecto"],["efecto","crisis"],["crisis","efecto"],["efecto","sufrir"],["sufrir","efecto"],["efecto","inusual "],["inusual ","efecto"],["efecto","anomalo"],["anomalo","efecto"],["efecto","alerta"],["alerta","efecto"],["efecto","prolongarse"],["prolongarse","efecto"],["efecto","debil"],["debil","efecto"],["efecto","moderado"],["moderado","efecto"],["efecto","amenaza"],["amenaza","efecto"],["efecto","complejo"],["complejo","efecto"],["efecto","exacerbadas"],["exacerbadas","efecto"],["efecto","desastre"],["desastre","efecto"],["desafio","intenso "],["intenso ","desafio"],["desafio","fortalecimiento"],["fortalecimiento","desafio"],["desafio","preocupacion"],["preocupacion","desafio"],["desafio","agudo"],["agudo","desafio"],["desafio","extremo"],["extremo","desafio"],["desafio","aumento "],["aumento ","desafio"],["desafio"," aumentaria"],[" aumentaria","desafio"],["desafio","profundos"],["profundos","desafio"],["desafio","disminucion "],["disminucion ","desafio"],["desafio"," reduccion"],[" reduccion","desafio"],["desafio","grave"],["grave","desafio"],["desafio","emergencia"],["emergencia","desafio"],["desafio","crisis"],["crisis","desafio"],["desafio","sufrir"],["sufrir","desafio"],["desafio","inusual "],["inusual ","desafio"],["desafio","anomalo"],["anomalo","desafio"],["desafio","alerta"],["alerta","desafio"],["desafio","prolongarse"],["prolongarse","desafio"],["desafio","debil"],["debil","desafio"],["desafio","moderado"],["moderado","desafio"],["desafio","amenaza"],["amenaza","desafio"],["desafio","complejo"],["complejo","desafio"],["desafio","exacerbadas"],["exacerbadas","desafio"],["desafio","desastre"],["desastre","desafio"],["verano","intenso "],["intenso ","verano"],["verano","fortalecimiento"],["fortalecimiento","verano"],["verano","preocupacion"],["preocupacion","verano"],["verano","agudo"],["agudo","verano"],["verano","extremo"],["extremo","verano"],["verano","aumento "],["aumento ","verano"],["verano"," aumentaria"],[" aumentaria","verano"],["verano","profundos"],["profundos","verano"],["verano","disminucion "],["disminucion ","verano"],["verano"," reduccion"],[" reduccion","verano"],["verano","grave"],["grave","verano"],["verano","emergencia"],["emergencia","verano"],["verano","crisis"],["crisis","verano"],["verano","sufrir"],["sufrir","verano"],["verano","inusual "],["inusual ","verano"],["verano","anomalo"],["anomalo","verano"],["verano","alerta"],["alerta","verano"],["verano","prolongarse"],["prolongarse","verano"],["verano","debil"],["debil","verano"],["verano","moderado"],["moderado","verano"],["verano","amenaza"],["amenaza","verano"],["verano","complejo"],["complejo","verano"],["verano","exacerbadas"],["exacerbadas","verano"],["verano","desastre"],["desastre","verano"],["helada","intenso "],["intenso ","helada"],["helada","fortalecimiento"],["fortalecimiento","helada"],["helada","preocupacion"],["preocupacion","helada"],["helada","agudo"],["agudo","helada"],["helada","extremo"],["extremo","helada"],["helada","aumento "],["aumento ","helada"],["helada"," aumentaria"],[" aumentaria","helada"],["helada","profundos"],["profundos","helada"],["helada","disminucion "],["disminucion ","helada"],["helada"," reduccion"],[" reduccion","helada"],["helada","grave"],["grave","helada"],["helada","emergencia"],["emergencia","helada"],["helada","crisis"],["crisis","helada"],["helada","sufrir"],["sufrir","helada"],["helada","inusual "],["inusual ","helada"],["helada","anomalo"],["anomalo","helada"],["helada","alerta"],["alerta","helada"],["helada","prolongarse"],["prolongarse","helada"],["helada","debil"],["debil","helada"],["helada","moderado"],["moderado","helada"],["helada","amenaza"],["amenaza","helada"],["helada","complejo"],["complejo","helada"],["helada","exacerbadas"],["exacerbadas","helada"],["helada","desastre"],["desastre","helada"]]</t>
@@ -82,7 +82,7 @@
     <t>preocupación</t>
   </si>
   <si>
-    <t>[{"title":"Oficina meteorológica australiana ve una La Niña más débil | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-australia-lanina-idLTASIE7..."},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"Nobel de Física recae en científicos que resolvieron elusivo misterio ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-nobel-fisica-idLTAKCN0S018Z2..."},{"title":"Índices Locales del Ciclo El Niño Oscilación del Sur para las ...","displayLink":"repositorio.unal.edu.co","formattedUrl":"https://repositorio.unal.edu.co/bitstream/.../1018421469.2021.pdf?...1...y"},{"title":"Spatio-temporal probabilistic prediction of appearance and duration ...","displayLink":"iopscience.iop.org","formattedUrl":"https://iopscience.iop.org/article/10.1088/1742-6596/1160/1/012018"},{"title":"Prisión para sujeto que explotaba sexualmente menores de edad ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../prision-para-sujeto-que-explotaba-sexualmente..."},{"title":"Ola Invernal Colombia 2010-2011","displayLink":"www.cepal.org","formattedUrl":"https://www.cepal.org/sites/.../news/.../ola_invernal_colombia_2010-2011_..."},{"title":"CIUDAD, SOSTENIBILIDAD Y POSCONFLICTO EN COLOMBIA:","displayLink":"library.fes.de","formattedUrl":"https://library.fes.de/pdf-files/bueros/kolumbien/16930-20201210.pdf"},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Notas de Población N° 111","displayLink":"repositorio.cepal.org","formattedUrl":"https://repositorio.cepal.org/server/api/core/bitstreams/...1d29.../content"}]</t>
+    <t>[{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"},{"title":"Comportamiento del Índice Oscilación del Sur (IOS) junto al ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Comportamiento-del-Indice-Oscilacion-del-..."},{"title":"A Stochastic Precipitation Generator Conditioned on ENSO Phase ...","displayLink":"journals.ametsoc.org","formattedUrl":"https://journals.ametsoc.org/.../1520-0442_2000_013_2973_aspgco_2.0.co..."},{"title":"\"Surviving Under the Reign of El Niño Southern Oscillation: An ...","displayLink":"digitalcollections.sit.edu","formattedUrl":"https://digitalcollections.sit.edu/isp_collection/3324/"},{"title":"Efecto de la Oscilación del Pacífico Sur (ENSO) sobre el ...","displayLink":"ideas.repec.org","formattedUrl":"https://ideas.repec.org/p/pra/mprapa/117109.html"},{"title":"Influencia de los períodos de “el niño oscilación del sur” en la ...","displayLink":"www.scielo.org.ar","formattedUrl":"http://www.scielo.org.ar/scielo.php?pid=S1851-23722023000200007..."},{"title":"Vista de Influencia de los períodos de “El Niño Oscilación del Sur ...","displayLink":"revistas.unc.edu.ar","formattedUrl":"https://revistas.unc.edu.ar/index.php/BSAB/article/view/38609/41653"},{"title":"EL NIÑO–SOUTHERN OSCILLATION INFLUENCES ANNUAL ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/10.1525/auk.2012.12017"},{"title":"Assessing the roles of temperature, precipitation, and enso in ...","displayLink":"www.scielo.org.mx","formattedUrl":"http://www.scielo.org.mx/scielo.php?script=sci_arttext&amp;pid=S0036..."},{"title":"Landfalling tropical cyclones on the Pacific coast of Mexico: 1850 ...","displayLink":"www.elsevier.es","formattedUrl":"https://www.elsevier.es/es-revista-atmosfera-76-articulo-landfalling-tropical..."}]</t>
   </si>
   <si>
     <t>3. Características actuales</t>
@@ -97,7 +97,7 @@
     <t>agudo</t>
   </si>
   <si>
-    <t>[{"title":"Más de 300.000 niños venezolanos en Colombia necesitan ayuda ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/04/1455081"},{"title":"Héctor Rusthenford Guerrero Flores, alias 'Niño Guerrero'","displayLink":"insightcrime.org","formattedUrl":"https://insightcrime.org/...news/hector-rusthenford-guerrero-flores-alias-nin..."},{"title":"Derechos del Niño, antibióticos... Las noticias del lunes | Noticias ONU","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/11/1465521"},{"title":"Engañoso: ¿Video de mujeres detenidas en Colombia corresponde ...","displayLink":"www.cazadoresdefakenews.info","formattedUrl":"https://www.cazadoresdefakenews.info/enganoso-video-de-mujeres-detenid..."},{"title":"Niños huyendo de Venezuela quedaron hambrientos, enfermos e ...","displayLink":"www.savannahnow.com","formattedUrl":"https://www.savannahnow.com/story/.../2018/09/.../10844076007/"},{"title":"¡Dando visibilidad a los niños refugiados de todo el mundo!","displayLink":"www.insideoutproject.net","formattedUrl":"https://www.insideoutproject.net/.../news/bringing-visibility-to-refugee-chil..."},{"title":"UNICEF: Progreso importante para los niños en los últimos 30 años ...","displayLink":"www.vaticannews.va","formattedUrl":"https://www.vaticannews.va/.../news/.../unicef-progreso-importante-ninos-ul..."},{"title":"Detienen en Cúcuta a la madre del niño abusado en Lara ...","displayLink":"maturinnews.com","formattedUrl":"https://maturinnews.com/detienen-en-cucuta-a-la-madre-del-nino-abusado-..."},{"title":"NEWS, REPORTS, COLOMBIA, FOOTWEAR-UNIVERSITY-BORN ...","displayLink":"www.serma.net","formattedUrl":"https://www.serma.net/news/reports/.../footwear-university-born-in-cucuta"},{"title":"¿Quién es El Niño Guerrero de Cúcuta? A alias “El Saúl” lo ...","displayLink":"www.eluniverso.com","formattedUrl":"https://www.eluniverso.com/.../a-alias-el-saul-lo-llaman-el-nino-guerrero-de..."}]</t>
+    <t>[{"title":"Nino Stamatovic | Davis Polk","displayLink":"www.davispolk.com","formattedUrl":"https://www.davispolk.com/lawyers/nino-stamatovic"},{"title":"Investigating El Niño: Teacher Resources | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/.../investigating-el-nino-teacher-resourc..."},{"title":"An investigation of the El Niño‐Southern Oscillation cycle With ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/abs/10.../JC092iC13p14251"},{"title":"INVESTIGATING EL NIÑO USING REAL DATA","displayLink":"www.nnvl.noaa.gov","formattedUrl":"https://www.nnvl.noaa.gov/StoryMaps/DITC/.../ElNino_TeachersGuide.pdf"},{"title":"Florida haze Canadian Smoke Matt Gaetz El Niño: News in 90","displayLink":"www.jacksonville.com","formattedUrl":"https://www.jacksonville.com/story/news/state/.../71045018007/"},{"title":"In Re Grand Jury Investigation (subpoena to Nino v. Tinari).appeal ...","displayLink":"law.justia.com","formattedUrl":"https://law.justia.com/cases/federal/appellate-courts/F2/631/17/86820/"},{"title":"Evaluating the Quality of Tuberculosis Contact Investigation in Cali ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/33617470/"},{"title":"Coping with El Nino, 1998: An investigation in the upland community ...","displayLink":"vtechworks.lib.vt.edu","formattedUrl":"https://vtechworks.lib.vt.edu/handle/10919/65550"},{"title":"what are three questions that a physical oceanographer might try to ...","displayLink":"brainly.com","formattedUrl":"https://brainly.com/question/17370380"},{"title":"El Nino - Introduction and Graph Investigation by Geo-Earth Sciences","displayLink":"www.teacherspayteachers.com","formattedUrl":"https://www.teacherspayteachers.com/.../El-Nino-Introduction-and-Graph-I..."}]</t>
   </si>
   <si>
     <t>El niño</t>
@@ -109,7 +109,7 @@
     <t>extremo</t>
   </si>
   <si>
-    <t>[{"title":"Más de 300.000 niños venezolanos en Colombia necesitan ayuda ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/04/1455081"},{"title":"Engañoso: ¿Video de mujeres detenidas en Colombia corresponde ...","displayLink":"www.cazadoresdefakenews.info","formattedUrl":"https://www.cazadoresdefakenews.info/enganoso-video-de-mujeres-detenid..."},{"title":"Derechos del Niño, antibióticos... Las noticias del lunes | Noticias ONU","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/11/1465521"},{"title":"Héctor Rusthenford Guerrero Flores, alias 'Niño Guerrero'","displayLink":"insightcrime.org","formattedUrl":"https://insightcrime.org/...news/hector-rusthenford-guerrero-flores-alias-nin..."},{"title":"Niños huyendo de Venezuela quedaron hambrientos, enfermos e ...","displayLink":"www.savannahnow.com","formattedUrl":"https://www.savannahnow.com/story/.../2018/09/.../10844076007/"},{"title":"¡Dando visibilidad a los niños refugiados de todo el mundo!","displayLink":"www.insideoutproject.net","formattedUrl":"https://www.insideoutproject.net/.../news/bringing-visibility-to-refugee-chil..."},{"title":"UNICEF: Progreso importante para los niños en los últimos 30 años ...","displayLink":"www.vaticannews.va","formattedUrl":"https://www.vaticannews.va/.../news/.../unicef-progreso-importante-ninos-ul..."},{"title":"Detienen en Cúcuta a la madre del niño abusado en Lara ...","displayLink":"maturinnews.com","formattedUrl":"https://maturinnews.com/detienen-en-cucuta-a-la-madre-del-nino-abusado-..."},{"title":"NEWS, REPORTS, COLOMBIA, FOOTWEAR-UNIVERSITY-BORN ...","displayLink":"www.serma.net","formattedUrl":"https://www.serma.net/news/reports/.../footwear-university-born-in-cucuta"},{"title":"¿Quién es El Niño Guerrero de Cúcuta? A alias “El Saúl” lo ...","displayLink":"www.eluniverso.com","formattedUrl":"https://www.eluniverso.com/.../a-alias-el-saul-lo-llaman-el-nino-guerrero-de..."}]</t>
+    <t>[{"title":"Investigating El Niño: Teacher Resources | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/el.../investigating-el-nino-teacher-resou..."},{"title":"INVESTIGATING EL NIÑO USING REAL DATA","displayLink":"www.nnvl.noaa.gov","formattedUrl":"https://www.nnvl.noaa.gov/StoryMaps/DITC/.../ElNino_TeachersGuide.pdf"},{"title":"Investigating El Niño Using Data in the Classroom | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/el.../investigating-el-nino-using-data-th..."},{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"},{"title":"An investigation of the El Niño‐Southern Oscillation cycle With ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/abs/10.../JC092iC13p14251"},{"title":"El Niño: Pacific Wind and Current Changes Bring Warm, Wild Weather","displayLink":"earthobservatory.nasa.gov","formattedUrl":"https://earthobservatory.nasa.gov/features/ElNino"},{"title":"Ocean Physics at NASA - NASA Science","displayLink":"science.nasa.gov","formattedUrl":"https://science.nasa.gov/earth-science/focus-areas/climate.../ocean-physics/"},{"title":"Coastal Sulfur Plumes off Peru During El Niño, La Niña, and Neutral ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2018GL077618"},{"title":"what are three questions that a physical oceanographer might try to ...","displayLink":"brainly.com","formattedUrl":"https://brainly.com/question/17370380"},{"title":"ENSO Information: NOAA Physical Sciences Laboratory","displayLink":"psl.noaa.gov","formattedUrl":"https://psl.noaa.gov/enso/"}]</t>
   </si>
   <si>
     <t>ENSO</t>
@@ -121,7 +121,7 @@
     <t>aumento / aumentaría</t>
   </si>
   <si>
-    <t>[{"title":"Colombia: Rains Leave 47 Dead and Over 18,000 Families Affected ...","displayLink":"www.telesurenglish.net","formattedUrl":"https://www.telesurenglish.net/news/Colombia-Rains-Leave-47-Dead-and-O..."},{"title":"Colombia reports 169 dengue deaths in 2019 - Outbreak News Today","displayLink":"outbreaknewstoday.com","formattedUrl":"https://outbreaknewstoday.com/colombia-reports-169-dengue-deaths-in-20..."},{"title":"Cez, Macquarie set for defeat on German energy market | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../cez-macquarie-set-for-defeat-on-german-energy..."},{"title":"Colombia: Dengue Outbreak Emergency Plan of Action (EPoA ...","displayLink":"reliefweb.int","formattedUrl":"https://reliefweb.int/.../colombia-dengue-outbreak-emergency-plan-action-e..."},{"title":"Spatio-temporal clusters and patterns of spread of dengue ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9439233/"},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Association of dengue infection with anti-alpha-gal antibodies, IgM ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9614307/"},{"title":"Jhan Piero Rojas Suarez1","displayLink":"pdfs.semanticscholar.org","formattedUrl":"https://pdfs.semanticscholar.org/.../62369cea0d27017150233d51e8d788f4..."},{"title":"60+ \"Edgar Rolon\" profiles | LinkedIn","displayLink":"www.linkedin.com","formattedUrl":"https://www.linkedin.com/pub/dir/Edgar/Rolon"},{"title":"DIAGNOSIS OF WATER IN THE AMERICAS","displayLink":"ianas.org","formattedUrl":"https://ianas.org/wp-content/uploads/2020/07/08-Diagnosis-of-water.pdf"}]</t>
+    <t>[{"title":"IRI – International Research Institute for Climate and Society ...","displayLink":"iri.columbia.edu","formattedUrl":"https://iri.columbia.edu/our-expertise/climate/forecasts/enso/current/"},{"title":"ENSO Information: NOAA Physical Sciences Laboratory","displayLink":"psl.noaa.gov","formattedUrl":"https://psl.noaa.gov/enso/"},{"title":"IRI – International Research Institute for Climate and Society | ENSO ...","displayLink":"iri.columbia.edu","formattedUrl":"https://iri.columbia.edu/our-expertise/climate/enso/"},{"title":"An Investigation of the Links between ENSO Flavors and Rainfall ...","displayLink":"journals.ametsoc.org","formattedUrl":"https://journals.ametsoc.org/view/journals/mwre/137/.../2009mwr3066.1.x..."},{"title":"Investigating ENSO and its teleconnections under climate ... - ESD","displayLink":"esd.copernicus.org","formattedUrl":"https://esd.copernicus.org/articles/11/267/2020/"},{"title":"Recent “Triple-Dip” La Niña upends current understanding of ENSO ...","displayLink":"research.noaa.gov","formattedUrl":"https://research.noaa.gov/.../recent-triple-dip-la-nina-upends-current-unders..."},{"title":"A model investigation of recent ENSO impacts over southern Africa ...","displayLink":"link.springer.com","formattedUrl":"https://link.springer.com/article/10.1007/s00703-005-0128-9"},{"title":"Investigating El Niño: Teacher Resources | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/.../investigating-el-nino-teacher-resourc..."},{"title":"Progress in ENSO prediction and predictability study | National ...","displayLink":"academic.oup.com","formattedUrl":"https://academic.oup.com/nsr/article/5/6/826/5123734"},{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"}]</t>
   </si>
   <si>
     <t>fenómeno meteorológico</t>
@@ -133,7 +133,7 @@
     <t>profundos</t>
   </si>
   <si>
-    <t>[{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Oficina meteorológica australiana ve una La Niña más débil | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-australia-lanina-idLTASIE7..."},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"Tormentas, inusuales tornados de invierno paralizan transporte en ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../clima-eeuu-tornados-idLTAKBN0UB0S720151..."},{"title":"Diez extrañas luces que pueden aparecer en el cielo - BBC News ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/.../151001_vert_earth_extranas_luces_cielo_y..."},{"title":"Extraño fenómeno meteorológico sorprendió en Santander, ¿De ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../extrano-fenomeno-meteorologico-sorprendio-..."},{"title":"Qué es la dispersión de Rayleigh y qué tiene que ver con que a ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-53722129"},{"title":"Relámpago del Catatumbo: tormentas sobre la misma región ...","displayLink":"www.tiempo.com","formattedUrl":"https://www.tiempo.com/.../relampago-del-catatumbo-tormentas-sobre-la-m..."},{"title":"Inundaciones amenazan a Colombia ante abandono estatal ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/inundaciones-amenazan-colombia-ante-aban..."},{"title":"Aumenta el calor en Colombia: A qué se debe y cuánto tiempo ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../aumenta-el-calor-en-colombia-a-que-se-debe-y..."}]</t>
+    <t>[{"title":"World Meteorological Organization's World Weather &amp; Climate ...","displayLink":"wmo.asu.edu","formattedUrl":"https://wmo.asu.edu/"},{"title":"Agencia meteorológica EEUU ve probabilidad de fenómeno de La ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/clima-lanina-idLTAKCN0WC21Q/"},{"title":"Weather Related Fatality and Injury Statistics","displayLink":"www.weather.gov","formattedUrl":"https://www.weather.gov/hazstat/"},{"title":"(PDF) Distribución espacial de fenómenos meteorológicos en Cuba ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../322508454_Distribucion_espacial_de_feno..."},{"title":"División de Investigación de Huracanes - NOAA/AOML","displayLink":"www.aoml.noaa.gov","formattedUrl":"https://www.aoml.noaa.gov/es/hurricane-research-division/"},{"title":"‪Giovanni Jiménez-Sánchez‬ - ‪Google Scholar‬","displayLink":"scholar.google.com","formattedUrl":"https://scholar.google.com/citations?user=QkiRrJsAAAAJ&amp;hl=en"},{"title":"Video no muestra peces alertando sobre huracán en México | AP ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/article/ap-verifica-191795492645"},{"title":"Tornados | Ready.gov","displayLink":"www.ready.gov","formattedUrl":"https://www.ready.gov/es/tornados"},{"title":"World Weather Attribution – Exploring the contribution of climate ...","displayLink":"www.worldweatherattribution.org","formattedUrl":"https://www.worldweatherattribution.org/"},{"title":"Investigación: Texas no tomó medidas contra el gas tras la crisis de ...","displayLink":"commissionshift.org","formattedUrl":"https://commissionshift.org/.../investigation-texas-failed-to-crack-down-on-..."}]</t>
   </si>
   <si>
     <t>patrón climático</t>
@@ -145,7 +145,7 @@
     <t>Disminución / reducción</t>
   </si>
   <si>
-    <t>[{"title":"The Yukpas: The Indigenous community who migrated to Colombia ...","displayLink":"www.dejusticia.org","formattedUrl":"https://www.dejusticia.org/.../the-yukpas-the-indigenous-community-who-..."},{"title":"Plan de emergencia para venezolanos, Yemen... Las noticias del ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2018/12/1448001"},{"title":"Oil trade pattern shifts as refiners go global | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../oil-trade-pattern-shifts-as-refiners-go-global-id..."},{"title":"Colombia (español) - giz.de","displayLink":"www.giz.de","formattedUrl":"https://www.giz.de/en/worldwide/29848.html"},{"title":"La migración vista como una gran oportunidad para el desarrollo","displayLink":"www.bancomundial.org","formattedUrl":"https://www.bancomundial.org/.../news/.../la-migracion-vista-como-una-gra..."},{"title":"Los cristianos colombianos predicaron la justicia... | Cristianismo hoy","displayLink":"www.christianitytoday.com","formattedUrl":"https://www.christianitytoday.com/.../colombia-inmigracion-venezuela-justi..."},{"title":"La belleza del mundo, a vuelo de drones - BBC News Mundo","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-36745733"},{"title":"Seis meses de triunfos para los derechos humanos - Amnistía ...","displayLink":"www.amnesty.org","formattedUrl":"https://www.amnesty.org/es/.../news/.../six-months-of-human-rights-success..."},{"title":"Crisis en Venezuela: en qué consiste la tarjeta de vacunación ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-49491234"},{"title":"World Drug Report 2015 - UNODC","displayLink":"www.unodc.org","formattedUrl":"https://www.unodc.org/documents/wdr2015/World_Drug_Report_2015.pdf"}]</t>
+    <t>[{"title":"¿Qué significa el patrón climático de El Niño para el invierno? | WFLA","displayLink":"www.wfla.com","formattedUrl":"https://www.wfla.com/.../que-significa-el-patron-climatico-de-el-nino-para-..."},{"title":"Catorce millones de personas, en riesgo de hambruna en el sur de ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/onu-hambruna-idESKCN0UW1BP/"},{"title":"El Niño and La Niña, Explained - The New York Times","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/article/what-is-la-nina-el-nino.html"},{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"},{"title":"NIMH » Trastorno afectivo estacional","displayLink":"www.nimh.nih.gov","formattedUrl":"https://www.nimh.nih.gov/health/publications/.../trastorno-afectivo-estacion..."},{"title":"Mapped: How climate change affects extreme weather around the ...","displayLink":"www.carbonbrief.org","formattedUrl":"https://www.carbonbrief.org/mapped-how-climate-change-affects-extreme-..."},{"title":"Causes and impacts of the 2014 warm anomaly in the NE Pacific ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/full/10.1002/2015GL063306"},{"title":"An alarming pattern: Climate disasters hit, and Spanish-language ...","displayLink":"www.nbcnews.com","formattedUrl":"https://www.nbcnews.com/.../climate-disinformation-spanish-misinformatio..."},{"title":"Climate Change Indicators: Weather and Climate | US EPA","displayLink":"www.epa.gov","formattedUrl":"https://www.epa.gov/climate-indicators/weather-climate"},{"title":"The Koch Brothers' Covert Ops | The New Yorker","displayLink":"www.newyorker.com","formattedUrl":"https://www.newyorker.com/magazine/2010/08/30/covert-operations"}]</t>
   </si>
   <si>
     <t>tormenta tropicales</t>
@@ -157,7 +157,7 @@
     <t>grave</t>
   </si>
   <si>
-    <t>[{"title":"Denuncian asesinato de hijo de líder social en Cúcuta, Colombia ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/colombia-asesinato-hijo-lider-social-cucuta-..."},{"title":"Tormenta Danny se debilita frente a costa este EEUU | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-danny-idLTASIE57P2H220..."},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"acento.com.do","formattedUrl":"https://acento.com.do/...news.../queacute-hay-detraacutes-del-insoacutelito-..."},{"title":"Cristóbal se convierte en huracán, avanza hacia Bermudas | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../portada-clima-tormenta-cristobal-idLTAKBN0G..."},{"title":"Copa Airlines anuncia vuelos hacia la ciudad colombiana de Cúcuta","displayLink":"elcapitalfinanciero.com","formattedUrl":"https://elcapitalfinanciero.com/?p=159216"},{"title":"45 Segundos Colombia (@45segundosco) • Instagram photos and ...","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/45segundosco/"},{"title":"Noticias de Copa Airlines","displayLink":"www.copaair.com","formattedUrl":"https://www.copaair.com/es-gs/noticias/"},{"title":"U.S. Sends Food, Medical Supplies to Colombia-Venezuela Border ...","displayLink":"www.sxm-talks.com","formattedUrl":"https://www.sxm-talks.com/.../u-s-sends-food-medical-supplies-to-colombia..."},{"title":"Emergencia en Santander por lluvias: más de 100 viviendas ...","displayLink":"redmas.com.co","formattedUrl":"https://redmas.com.co/.../Emergencia-en-Santander-por-lluvias-mas-de-100..."},{"title":"Ataque sicarial deja a una niña de 3 años muerta y a su madre ...","displayLink":"www.eluniversal.com.co","formattedUrl":"https://www.eluniversal.com.co/.../ataque-sicarial-deja-a-una-nina-de-3-ano..."}]</t>
+    <t>[{"title":"Presentatión de Investigation Colaborativa: Universidad de Costa ...","displayLink":"www.anticipation-hub.org","formattedUrl":"https://www.anticipation-hub.org/.../presentation-de-investigation-colaborat..."},{"title":"2005 Atlantic Hurricane Season","displayLink":"www.nhc.noaa.gov","formattedUrl":"https://www.nhc.noaa.gov/data/tcr/index.php?season=2005&amp;basin=atl"},{"title":"National Hurricane Center: Tropical Storm Bret 2023 continues path ...","displayLink":"abc11.com","formattedUrl":"https://abc11.com/bret-tropical-storm-2023-national...path.../13410211/"},{"title":"CSU Hurricane Seasonal Forecasting","displayLink":"tropical.colostate.edu","formattedUrl":"https://tropical.colostate.edu/forecasting.html"},{"title":"An Investigation of the Tropical Cyclogenesis of Arlene (2005) Using ...","displayLink":"www.tandfonline.com","formattedUrl":"https://www.tandfonline.com/doi/abs/10.1080/00330124.2014.987197"},{"title":"Tropical Storm Jose Is Absorbed by Another Storm - The New York ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/article/tropical-storm-jose-hurricane.html"},{"title":"Global Warming and Hurricanes – Geophysical Fluid Dynamics ...","displayLink":"www.gfdl.noaa.gov","formattedUrl":"https://www.gfdl.noaa.gov/global-warming-and-hurricanes/"},{"title":"Tormenta tropical Sandy se dirige a Jamaica, luego a Cuba | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-sandy-posicion-idLTASIE8..."},{"title":"Tropical Storm Idalia could threaten the Gulf Coast and Florida this ...","displayLink":"www.cnn.com","formattedUrl":"https://www.cnn.com/2023/08/27/weather/tropical...storm.../index.html"},{"title":"Tormenta Andrea se fortalece, en dirección a noroeste de Florida ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-andrea-idLTASIE95406L2..."}]</t>
   </si>
   <si>
     <t>lluvias torrenciales</t>
@@ -169,7 +169,7 @@
     <t>emergencia</t>
   </si>
   <si>
-    <t>[{"title":"Más de 300.000 niños venezolanos en Colombia necesitan ayuda ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/04/1455081"},{"title":"Nuevo atentado en Cúcuta atacaron una estación policial | Noticia ...","displayLink":"www.jambalayanews.com","formattedUrl":"https://www.jambalayanews.com/news/.../article_d708feb8-5f6b-11ec-b74d..."},{"title":"Gasolina más barata del mundo desata contrabando andino | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-venezuela-colombia-contrab-idL..."},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"acento.com.do","formattedUrl":"https://acento.com.do/...news.../queacute-hay-detraacutes-del-insoacutelito-..."},{"title":"La tormenta Imelda golpea las operaciones de energía de costa del ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/clima-imelda-energia-idLTAKBN1W434Z/"},{"title":"Emergencia en Cúcuta por fuertes lluvias: 60 barrios están afectados","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...en...lluvias.../202259/"},{"title":"Del llano venezolano a las calles de Cúcuta: la dura prueba de ...","displayLink":"migravenezuela.com","formattedUrl":"https://migravenezuela.com/.../el-migrante-de-la-calle-la-otra-realidad-del-e..."},{"title":"Los desplazamientos en masa y la crecida de los ríos incrementan ...","displayLink":"www.acnur.org","formattedUrl":"https://www.acnur.org/.../los-desplazamientos-en-masa-y-la-crecida-de-los-r..."},{"title":"ETB no prestará servicio de internet y televisión en Cúcuta: estas ...","displayLink":"es-us.finanzas.yahoo.com","formattedUrl":"https://es-us.finanzas.yahoo.com/.../etb-prestará-servicio-internet-televisión-..."},{"title":"Zona F Noticias (@zonaf_noticias) • Instagram photos and videos","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/zonaf_noticias/?hl=en"}]</t>
+    <t>[{"title":"More extreme precipitation in the world's dry and wet regions ...","displayLink":"www.nature.com","formattedUrl":"https://www.nature.com/articles/nclimate2941"},{"title":"Nine Teenagers Killed After Flash Floods Hit Israel's South ...","displayLink":"www.haaretz.com","formattedUrl":"https://www.haaretz.com/.../0000017f-ded5-df9c-a17f-feddaa940000"},{"title":"Zeta deja lluvias torrenciales al cruzar sudeste mexicano camino al ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/clima-zeta-idLTAKBN27C1IZ"},{"title":"Jeremy Schwartz — ProPublica","displayLink":"www.propublica.org","formattedUrl":"https://www.propublica.org/people/jeremy-schwartz/p2"},{"title":"Científicos prevén olas de calor y lluvias torrenciales más largas por ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../clima-temperatura-salud-idLTAKCN1V91KM/"},{"title":"La tormenta tropical Pilar azota Centroamérica con lluvias torrenciales","displayLink":"apnews.com","formattedUrl":"https://apnews.com/.../general-news-dce9b6b1835edb050e54c479ae1c7c1d"},{"title":"José Antonio Alloza's research works | University of Alicante ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/scientific.../Jose-Antonio-Alloza-21914385"},{"title":"Bajo Una Nube - CSI: Crime Scene Investigation (temporada 14 ...","displayLink":"tv.apple.com","formattedUrl":"https://tv.apple.com/pe/episode/.../umc.cmc.ml0wj6rkedrnnxnmtra9nroh"},{"title":"Pablo RUIZ SALCINES | Institute of Engineering | Research profile","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/profile/Pablo-Ruiz-Salcines"},{"title":"Lluvias torrenciales se extienden por Centroamérica a medida que ...","displayLink":"www.local10.com","formattedUrl":"https://www.local10.com/.../lluvias-torrenciales-se-extienden-por-centroame..."}]</t>
   </si>
   <si>
     <t>inundaciones</t>
@@ -178,7 +178,7 @@
     <t>Crisis</t>
   </si>
   <si>
-    <t>[{"title":"Colombia – Floods Affect 1,700 Families in Barbacoas, Nariño ...","displayLink":"floodlist.com","formattedUrl":"https://floodlist.com/america/colombia-floods-barbacoas-april-2021"},{"title":"Inundaciones afectan a 1.500 familias en Cúcuta, Colombia ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/inundaciones-riada-quebrada-cucuta-colomb..."},{"title":"El Pase De Cucuta | TikTok","displayLink":"www.tiktok.com","formattedUrl":"https://www.tiktok.com/find/el-pase-de-cucuta"},{"title":"Inundaciones amenazan a Colombia ante abandono estatal ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/inundaciones-amenazan-colombia-ante-aban..."},{"title":"Colombia: Rains Leave 47 Dead and Over 18,000 Families Affected ...","displayLink":"www.telesurenglish.net","formattedUrl":"https://www.telesurenglish.net/news/Colombia-Rains-Leave-47-Dead-and-O..."},{"title":"Presidente Obama visita Nueva Jersey tras inundaciones por Irene ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-irene-obama-idLTASIE7A7NA32..."},{"title":"BAJO EL AGUA está Cúcuta por las fuertes lluvias que dejan ríos ...","displayLink":"impactovenezuela.com","formattedUrl":"https://impactovenezuela.com/bajo-el-agua-esta-cucuta-por-las-fuertes-lluvi..."},{"title":"Al menos 24 muertos por inundaciones en Ghana | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-ghana-inundaciones-idLTASIE65..."},{"title":"Fuerte lluvia dejó graves inundaciones en Cúcuta; un vehículo ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/...inundaciones.../202312/"},{"title":"Emergencia en La Guajira por el invierno: fuertes lluvias provocaron ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../emergencia-en-la-guajira-por-el-invierno-fuert..."}]</t>
+    <t>[{"title":"Can coastal cities turn the tide on climate change flooding risk ...","displayLink":"www.mckinsey.com","formattedUrl":"https://www.mckinsey.com/.../can-coastal-cities-turn-the-tide-on-rising-floo..."},{"title":"El Paso Central Area Flood Risk Management Study","displayLink":"www.spa.usace.army.mil","formattedUrl":"https://www.spa.usace.army.mil/Missions/Civil-Works/EPCC/"},{"title":"Río Puerto Nuevo proyecto de manejo de inundaciones: Reunión ...","displayLink":"usace.contentdm.oclc.org","formattedUrl":"https://usace.contentdm.oclc.org/digital/collection/p16021coll11/id/6329/"},{"title":"Office of Professional Responsibility | FEMA.gov","displayLink":"www.fema.gov","formattedUrl":"https://www.fema.gov/es/about/offices/professional-responsibility"},{"title":"Cost of flood damage to U.S. homes will increase by 61% in 30 ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../cost-flood-damage-us-homes-will-increase-by-6..."},{"title":"Research Paper Flood monitoring and damage assessment using ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/pii/S111098231500006X"},{"title":"Fatalities in the United States from Atlantic Tropical Cyclones: New ...","displayLink":"journals.ametsoc.org","formattedUrl":"https://journals.ametsoc.org/view/journals/bams/.../bams-d-12-00074.1.xml"},{"title":"UNNATURAL COASTAL FLOODS:","displayLink":"sealevel.climatecentral.org","formattedUrl":"https://sealevel.climatecentral.org/.../Unnatural-Coastal-Floods-2016.pdf"},{"title":"Floods | Ready.gov","displayLink":"www.ready.gov","formattedUrl":"https://www.ready.gov/floods"},{"title":"Bureau of Investigation | Kings County","displayLink":"www.countyofkings.com","formattedUrl":"https://www.countyofkings.com/departments/public-safety/.../elder-abuse"}]</t>
   </si>
   <si>
     <t>sequías extremas</t>
@@ -187,7 +187,7 @@
     <t>sufrir</t>
   </si>
   <si>
-    <t>[{"title":"Versión debilitada de La Niña aleja temores de pérdidas de soja y ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../granos-sudamerica-clima-idLTAKCN10722L/"},{"title":"3 cosas que debemos hacer para que la temperatura del planeta no ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-45119084"},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Se necesitan 1.350 millones de dólares para ayudar a los ...","displayLink":"www.acnur.org","formattedUrl":"https://www.acnur.org/.../news.../se-necesitan-1350-millones-de-dolares-par..."},{"title":"News and Events","displayLink":"www.scalabrinisaintcharles.org","formattedUrl":"https://www.scalabrinisaintcharles.org/news-events"},{"title":"Bosque Seco Tropical - Ministerio de Ambiente y Desarrollo ...","displayLink":"www.minambiente.gov.co","formattedUrl":"https://www.minambiente.gov.co/direccion-de...y.../bosque-seco-tropical/"},{"title":"Advierten más de 100°F durante la primera ola de calor de la ...","displayLink":"www.univision.com","formattedUrl":"https://www.univision.com/.../ola-de-calor-100-f-incendios-sur-california"},{"title":"El cambio climático empuja a la migración en América Latina – DW ...","displayLink":"www.dw.com","formattedUrl":"https://www.dw.com/es/el-cambio-climático-también.../a-53883878"},{"title":"Ola Invernal Colombia 2010-2011","displayLink":"www.cepal.org","formattedUrl":"https://www.cepal.org/sites/.../news/.../ola_invernal_colombia_2010-2011_..."}]</t>
+    <t>[{"title":"Mortality Gradients within and among Dominant Plant Populations ...","displayLink":"conbio.onlinelibrary.wiley.com","formattedUrl":"https://conbio.onlinelibrary.wiley.com/doi/abs/.../j.1523-1739.2006.00424...."},{"title":"Extreme Weather and Real Estate: A Case Study of the Jamaican ...","displayLink":"publications.iadb.org","formattedUrl":"https://publications.iadb.org/.../extreme-weather-and-real-estate-case-study-j..."},{"title":"(PDF) El episodio de sequía extrema de 2019- 2021 en la Cuenca ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../358734930_El_episodio_de_sequia_extre..."},{"title":"Más inundaciones y sequías extremas a causa del cambio climático ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/es/.../cambio-climatico-inundaciones-sequias.html"},{"title":"Agriculture | Drought.gov","displayLink":"www.drought.gov","formattedUrl":"https://www.drought.gov/sectors/agriculture"},{"title":"Index: SPEI, The Standardised Precipitation-Evapotranspiration Index","displayLink":"spei.csic.es","formattedUrl":"https://spei.csic.es/"},{"title":"Los precedentes y las respuestas de los árboles a sequías extremas ...","displayLink":"www.revistaecosistemas.net","formattedUrl":"https://www.revistaecosistemas.net/index.php/ecosistemas/article/view/695"},{"title":"Soluciones a las sequías agravadas por el cambio climático - Union ...","displayLink":"blog.ucsusa.org","formattedUrl":"https://blog.ucsusa.org/.../soluciones-a-las-sequias-agravadas-por-el-cambio..."},{"title":"California | Drought.gov","displayLink":"www.drought.gov","formattedUrl":"https://www.drought.gov/states/california"},{"title":"Condiciones de sequía ceden levemente en Planicies EEUU ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../negocios-clima-eeuu-sequia-idLTASIE93305G..."}]</t>
   </si>
   <si>
     <t>incendios forestales</t>
@@ -196,7 +196,7 @@
     <t>inusual /anómalo</t>
   </si>
   <si>
-    <t>[{"title":"Piñera reitera decisión de viajar a Cúcuta en medio de incendios ...","displayLink":"www.eldinamo.cl","formattedUrl":"https://www.eldinamo.cl/.../pinera-reitera-decision-de-viajar-a-cucuta-en-m..."},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"DAY AHEAD-Noticias e Indicadores de América Latina (26 de ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/latam-day-ahead-idLTAL2N25M071/"},{"title":"Los Incendios Forestales un Problema Ambiental","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/563-los-incendios-forestales-un-problema-a..."},{"title":"Rusia dice fuego quemó bosques dañados por Chernobyl | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-rusia-incendios-idLTASIE67A099..."},{"title":"Controlan el nuevo incendio en Parque Isla Salamanca by Andrea ...","displayLink":"cucutagrid.com","formattedUrl":"https://cucutagrid.com/.../news/.../controlan-el-nuevo-incendio-en-parque-is..."},{"title":"Incendios forestales en Cúcuta por ola de calor - Otras Ciudades ...","displayLink":"www.eltiempo.com","formattedUrl":"https://www.eltiempo.com/.../incendios-forestales-en-cucuta-por-ola-de-cal..."},{"title":"Piñera visita La Araucanía y Los Lagos previo a su viaje a Cúcuta ...","displayLink":"cooperativa.cl","formattedUrl":"https://cooperativa.cl/.../incendios-forestales/pinera.../233640.html"},{"title":"Sebastián Piñera: “Nunca he politizado las relaciones exteriores” de ...","displayLink":"www.aa.com.tr","formattedUrl":"https://www.aa.com.tr/es/mundo/sebastián-piñera-nunca-he.../1399597"},{"title":"Capturan a mujer que robó bebé a una migrante venezolana en ...","displayLink":"venezuela-news.com","formattedUrl":"https://venezuela-news.com/capturan-mujer-robo-bebe-migrante-venezolan..."}]</t>
+    <t>[{"title":"Investigación de incendios forestales | Centro de Ciencias de la ...","displayLink":"environmentalhealth.ucdavis.edu","formattedUrl":"https://environmentalhealth.ucdavis.edu/.../incendios.../encuesta-salud-estata..."},{"title":"Español","displayLink":"www.firearson.com","formattedUrl":"https://www.firearson.com/es/"},{"title":"Forest fire research and innovation","displayLink":"research-and-innovation.ec.europa.eu","formattedUrl":"https://research-and-innovation.ec.europa.eu/.../forest-fire-research-and-inn..."},{"title":"Wildfire and Wildfire Safety","displayLink":"www.cpuc.ca.gov","formattedUrl":"https://www.cpuc.ca.gov/industries-and-topics/wildfires"},{"title":"Wildfire smoke exposure under climate change: impact on ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6743728/"},{"title":"After Action Review (AAR) – Part 1 | NWCG","displayLink":"www.nwcg.gov","formattedUrl":"https://www.nwcg.gov/committee/6mfs/aar-part1"},{"title":"International Journal of Wildland Fire - CSIRO PUBLISHING","displayLink":"www.publish.csiro.au","formattedUrl":"https://www.publish.csiro.au/wf/wf05044"},{"title":"Project – CILIFO","displayLink":"cilifo.eu","formattedUrl":"https://cilifo.eu/project"},{"title":"Incidents","displayLink":"www.fire.ca.gov","formattedUrl":"https://www.fire.ca.gov/incidents"},{"title":"Bomberos luchan contra incendios forestales en California | AP News","displayLink":"apnews.com","formattedUrl":"https://apnews.com/us.../general-news-fbc59c9523782be923bf8f63d11c8d..."}]</t>
   </si>
   <si>
     <t>condiciones meteorológicas</t>
@@ -205,7 +205,7 @@
     <t>alerta</t>
   </si>
   <si>
-    <t>[{"title":"Solicitar su cita es muy fácil | Cancillería","displayLink":"www.cancilleria.gov.co","formattedUrl":"https://www.cancilleria.gov.co/newsroom/news/solicitar-su-cita-muy-facil"},{"title":"La curiosa historia detrás de la maldición motilona por la que Boca ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../la-curiosa-historia-detras-de-la-maldicion-motil..."},{"title":"Cancillería entrega murales con componente ecológico en Cúcuta ...","displayLink":"www.cancilleria.gov.co","formattedUrl":"https://www.cancilleria.gov.co/newsroom/news/cancilleria-entrega-murales-..."},{"title":"Aeropuertos Argentina cancelan reapertura por ceniza | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-argentina-vuelos-idLTASIE75C0I..."},{"title":"Conferencia por los venezolanos, Siria, montañas... Las noticias del ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/10/1464501"},{"title":"Tormenta invernal deja decenas de muertos en Estados Unidos","displayLink":"cnnespanol.cnn.com","formattedUrl":"https://cnnespanol.cnn.com/.../prolongada-tormenta-invernal-cortes-electric..."},{"title":"El Mediterráneo se convierte en un cementerio para los niños y su ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/09/1524502"},{"title":"Qué es el estrés térmico que los científicos piden incluir en las ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-65429152"},{"title":"Noticias","displayLink":"www.aerocivil.gov.co","formattedUrl":"https://www.aerocivil.gov.co/prensa/noticias"},{"title":"Cancela, detén o cambia una suscripción en Google Play - Android ...","displayLink":"support.google.com","formattedUrl":"https://support.google.com/googlenews/answer/7018481?hl=es-419..."}]</t>
+    <t>[{"title":"Meteorological Condition - an overview | ScienceDirect Topics","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/topics/engineering/meteorological-condition"},{"title":"Extreme heat in North America, Europe and China in July 2023 ...","displayLink":"www.worldweatherattribution.org","formattedUrl":"https://www.worldweatherattribution.org/extreme-heat-in-north-america-eu..."},{"title":"Sweden and Estonia begin new investigation of 1994 Baltic ferry ...","displayLink":"www.thenomadtoday.com","formattedUrl":"https://www.thenomadtoday.com/...investigation.../2021070822430301278..."},{"title":"(PDF) Condiciones Meteorológicas y Oceanográficas en El Pacífico ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../356912546_Condiciones_Meteorologicas_..."},{"title":"National Institute Of Malaria Research Condiciones climáticas ...","displayLink":"www.aqi.in","formattedUrl":"https://www.aqi.in/weather/es/india/.../national-institute-of-malaria-research"},{"title":"Analizan las condiciones meteorológicas en el accidente mortal de ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/socedad-kobe-bryant-idESKBN1ZR10E"},{"title":"Influencia de las condiciones meteorológicas en la patología ...","displayLink":"www.apunts.org","formattedUrl":"https://www.apunts.org/es-influencia-condiciones-meteorologicas-patologia..."},{"title":"Analyzing ground ozone formation regimes using a principal axis ...","displayLink":"www.scielo.org.mx","formattedUrl":"http://www.scielo.org.mx/scielo.php?script=sci_arttext&amp;pid=S0187..."},{"title":"Inicio | Bienvenido a CICESE","displayLink":"www.cicese.edu.mx","formattedUrl":"https://www.cicese.edu.mx/"},{"title":"FireBuster: Una Herramienta Para el Manejo del Fuego","displayLink":"www.fs.usda.gov","formattedUrl":"https://www.fs.usda.gov/psw/publications/.../psw.../psw_gtr261esp_027.pdf"}]</t>
   </si>
   <si>
     <t>Aumento de la temperatura del aire</t>
@@ -214,7 +214,7 @@
     <t>prolongarse</t>
   </si>
   <si>
-    <t>[{"title":"¿Cómo saber cuál es el aire acondicionado que necesitas ...","displayLink":"news.samsung.com","formattedUrl":"https://news.samsung.com/.../como-saber-cual-es-el-aire-acondicionado-que..."},{"title":"3 cosas que debemos hacer para que la temperatura del planeta no ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-45119084"},{"title":"Cómo el clima afecta a los insectos – Insectos después de la lluvia ...","displayLink":"www.raid.com","formattedUrl":"https://www.raid.com/es-US/education/bug.../how-weather-affects-insects"},{"title":"TESTIGO-Caminando sobre un hielo Artico cada vez más ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-medioambiente-artico-idLTASIE7..."},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"Lechuza de Campanario | Audubon Field Guide","displayLink":"www.audubon.org","formattedUrl":"https://www.audubon.org/es/guia-de-aves/ave/lechuza-de-campanario"},{"title":"¿Hasta cuando irá el intenso calor en Cúcuta?, expertos revelan las ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/...temperatura/202348/"},{"title":"El tortuoso viaje a pie de madre e hija de Venezuela a Perú | AP News","displayLink":"apnews.com","formattedUrl":"https://apnews.com/general-news-72d80e607de74ba3910644c424ffcefa"},{"title":"Boletín Ambiente y Negocios Sostenibles | 25 de octubre 2023 ...","displayLink":"bu.com.co","formattedUrl":"https://bu.com.co/.../boletin-ambiente-y-negocios-sostenibles-25-de-octubre..."},{"title":"Luis Bienteveo | Audubon Field Guide","displayLink":"www.audubon.org","formattedUrl":"https://www.audubon.org/es/guia-de-aves/ave/luis-bienteveo"}]</t>
+    <t>[{"title":"Publicaciones de NIOSH - Prevención de las enfermedades ... - CDC","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/spanish/niosh/docs/wp-solutions/2013.../default.html"},{"title":"4.3 Aire acondicionado y control ambiental | International ...","displayLink":"www.iasa-web.org","formattedUrl":"https://www.iasa-web.org/tc05.../43-aire-acondicionado-y-control-ambienta..."},{"title":"Lo que los Padres Deben Saber sobre las Raves — FBI","displayLink":"www.fbi.gov","formattedUrl":"https://www.fbi.gov/news/.../lo-que-los-padres-deben-saber-sobre-las-raves"},{"title":"Evidencia | Datos – Climate Change: Vital Signs of the Planet","displayLink":"climate.nasa.gov","formattedUrl":"https://climate.nasa.gov/en-espanol/"},{"title":"Manual de Costos de Control de Contaminacion del Aire de la EPA","displayLink":"www3.epa.gov","formattedUrl":"https://www3.epa.gov/ttncatc1/cica/files/c_allchs-s.pdf"},{"title":"¿Qué es un polvo combustible?","displayLink":"www.osha.gov","formattedUrl":"https://www.osha.gov/.../riesgos_asociados_al_manejo_de_polo_combustib..."},{"title":"\"Climate Change Effects on Volcanoes in the Tropics: A review of ...","displayLink":"digitalcollections.sit.edu","formattedUrl":"https://digitalcollections.sit.edu/isp_collection/3325/"},{"title":"Algunos bosques tropicales revelan una resistencia extraordinaria ...","displayLink":"www.nationalgeographicla.com","formattedUrl":"https://www.nationalgeographicla.com/.../algunos-bosques-tropicales-revela..."},{"title":"Estudio del efecto de la geometria de un secador solar tipico/Study ...","displayLink":"go.gale.com","formattedUrl":"https://go.gale.com/ps/i.do?id...sid=googleScholar..."},{"title":"ESTUDIO BINACIONAL SOBRE OPORTUNIDADES DE ...","displayLink":"www.ibwc.gov","formattedUrl":"https://www.ibwc.gov/wp-content/uploads/2023/.../TMs_All_Portfolio.pdf"}]</t>
   </si>
   <si>
     <t>altas temperaturas</t>
@@ -223,7 +223,7 @@
     <t>debil</t>
   </si>
   <si>
-    <t>[{"title":"Autoridades de salud en Cúcuta en alerta por fuerte oleada de calor ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../autoridades-de-salud-en-cucuta-en-alerta-por-..."},{"title":"La Diócesis de Cúcuta ayuda a desplazados venezolanos - Vatican ...","displayLink":"www.vaticannews.va","formattedUrl":"https://www.vaticannews.va/.../news/.../diocesis-cucuta-colombia-ayuda-a-d..."},{"title":"Qué calor: a 37 grados estará la temperatura en Cúcuta este lunes 2 ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/que.../202330/"},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Inflación en Brasil supera meta y alcanza nivel más alto desde 2011 ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../negocios-economia-brasil-inflacion-idLTAKBN..."},{"title":"WEG suministra equipos para el proyecto de ampliación del ...","displayLink":"www.weg.net","formattedUrl":"https://www.weg.net/.../news/.../weg-suministra-equipos-para-el-proyecto-d..."},{"title":"Qué es el estrés térmico que los científicos piden incluir en las ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-65429152"},{"title":"Unos diamantes sugieren que hubo frío letal hace 12.900 años ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../oesen-ciencia-diamantes-cometas-idESMAE502..."},{"title":"Cúcuta rompe fronteras con la tecnología de Samsung Colombia ...","displayLink":"news.samsung.com","formattedUrl":"https://news.samsung.com/.../cucuta-rompe-fronteras-con-la-tecnologia-de-..."},{"title":"Recluso recibió una paliza en plena cárcel porque su familia no ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../recluso-recibio-una-paliza-de-parte-de-sus-com..."}]</t>
+    <t>[{"title":"Investigation of the Physicochemical Properties of Vegetable Oils ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8986445/"},{"title":"Death of 2,400 Australian sheep on ship to Middle East sparks ...","displayLink":"www.theguardian.com","formattedUrl":"https://www.theguardian.com/.../disgusting-death-of-2900-australian-sheep-..."},{"title":"Effects of Heat Wave on Body Temperature and Blood Pressure in ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3412201/"},{"title":"Effect of sauna-based heat acclimation on plasma volume and heart ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/25432420/"},{"title":"Monterey Bay Aquarium study finds extreme heat is the 'new normal ...","displayLink":"www.montereybayaquarium.org","formattedUrl":"https://www.montereybayaquarium.org/.../study-finds-extreme-heat-is-the-..."},{"title":"Investigación experimental del hormigón de alta resistencia ...","displayLink":"www.scielo.cl","formattedUrl":"http://www.scielo.cl/scielo.php?script=sci_arttext&amp;pid=S0718..."},{"title":"Paredes de alvenaria estrutural expostas a altas temperaturas com ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../338288171_Paredes_de_alvenaria_estrutur..."},{"title":"Estudio de las propiedades mecánicas residuales de hormigones ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/abs/pii/S0439568917300165"},{"title":"Comportamiento Térmico y Estructural del Concreto Expuesto a ...","displayLink":"revistas.uees.edu.ec","formattedUrl":"https://revistas.uees.edu.ec/index.php/IRR/article/view/560"},{"title":"Comportamento de blocos estruturais de concreto com diferentes ...","displayLink":"repositorio.ufscar.br","formattedUrl":"https://repositorio.ufscar.br/handle/ufscar/17022"}]</t>
   </si>
   <si>
     <t>Fenomenos climáticos extremos</t>
@@ -232,7 +232,7 @@
     <t>moderado</t>
   </si>
   <si>
-    <t>[{"title":"Tormentas, inusuales tornados de invierno paralizan transporte en ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../clima-eeuu-tornados-idLTAKBN0UB0S720151..."},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Versión debilitada de La Niña aleja temores de pérdidas de soja y ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../granos-sudamerica-clima-idLTAKCN10722L/"},{"title":"Los ocho obstáculos al desarrollo sostenible de América Latina ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2019/10/1463292"},{"title":"Corponor prepara a los Nortesantandereanos frente al Cambio ...","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/1521-corponor-prepara-a-los-nortesantande..."},{"title":"Qué es el estrés térmico que los científicos piden incluir en las ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-65429152"},{"title":"Ola Invernal Colombia 2010-2011","displayLink":"www.cepal.org","formattedUrl":"https://www.cepal.org/sites/.../news/.../ola_invernal_colombia_2010-2011_..."},{"title":"3 cosas que debemos hacer para que la temperatura del planeta no ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-45119084"},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"Migraciones, ambiente y cambio climático: estudios de caso en ...","displayLink":"publications.iom.int","formattedUrl":"https://publications.iom.int/.../migraciones_ambiente_y_cambio_climatico_..."}]</t>
+    <t>[{"title":"World Meteorological Organization's World Weather &amp; Climate ...","displayLink":"wmo.asu.edu","formattedUrl":"https://wmo.asu.edu/"},{"title":"World Weather Attribution – Exploring the contribution of climate ...","displayLink":"www.worldweatherattribution.org","formattedUrl":"https://www.worldweatherattribution.org/"},{"title":"Climate Change Indicators: Weather and Climate | US EPA","displayLink":"www.epa.gov","formattedUrl":"https://www.epa.gov/climate-indicators/weather-climate"},{"title":"WMO Atlas of Mortality and Economic Losses from Weather, Climate ...","displayLink":"library.wmo.int","formattedUrl":"https://library.wmo.int/.../57564-wmo-atlas-of-mortality-and-economic-loss..."},{"title":"Unlocking Green and Just Hydrogen in Latin America and the ...","displayLink":"publications.iadb.org","formattedUrl":"https://publications.iadb.org/.../unlocking-green-and-just-hydrogen-latin-a..."},{"title":"UNICEF: Millones de niños son desplazados por fenómenos ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/.../general-news-4ee2f2c0664b4d8a81ddc9bb7c4afd24"},{"title":"El calentamiento global está contribuyendo a los fenómenos ...","displayLink":"www.nationalacademies.org","formattedUrl":"https://www.nationalacademies.org/.../el-calentamiento-global-esta-contribu..."},{"title":"The Infrastructure Gap in Latin America and the Caribbean ...","displayLink":"publications.iadb.org","formattedUrl":"https://publications.iadb.org/.../infrastructure-gap-latin-america-and-caribbe..."},{"title":"Incluso la Antártida se ve golpeada por fenómenos climáticos ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/.../general-news-c96d109c7500c8fecc579b0346d58a8f"},{"title":"Mapped: How climate change affects extreme weather around the ...","displayLink":"www.carbonbrief.org","formattedUrl":"https://www.carbonbrief.org/mapped-how-climate-change-affects-extreme-..."}]</t>
   </si>
   <si>
     <t>Presente</t>
@@ -328,7 +328,7 @@
     <t>Díficil / Disminución</t>
   </si>
   <si>
-    <t>[{"title":"FENÓMENO EL NIÑO Y CAPTACIÓN ILEGAL DE AGUA ...","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/2313-fenomeno-el-nino-y-captacion-ilegal-..."},{"title":"El Niño y sequía dañan producción de café robusta, podrían subir ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../negocios-cafe-robusta-elnino-idLTAKCN0SZ1..."},{"title":"Inseguridad, venezolanos en el Darién, sequía en el Cuerno de ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2022/02/1503752"},{"title":"Heladas se suman a la sequía que castiga a trigo de Argentina ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/granos-argentina-trigo-idARL1N2FM1NL/"},{"title":"Ciclismo: Venezolano Yonder Godoy gana sexta etapa de la 58ª ...","displayLink":"spanish.news.cn","formattedUrl":"https://spanish.news.cn/20230121/.../c.html"},{"title":"¡Dando visibilidad a los niños refugiados de todo el mundo!","displayLink":"www.insideoutproject.net","formattedUrl":"https://www.insideoutproject.net/.../news/bringing-visibility-to-refugee-chil..."},{"title":"Histórico: tras 60 años de sequía, llega el agua al corregimiento de ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...tras.../202318/"},{"title":"La cifra de personas refugiadas y migrantes venezolanas alcanza ...","displayLink":"www.acnur.org","formattedUrl":"https://www.acnur.org/.../news.../la-cifra-de-personas-refugiadas-y-migrant..."},{"title":"¡Hoy juega Junior con Cúcuta!: No importa que sea por Copa, se ...","displayLink":"impactonews.co","formattedUrl":"https://impactonews.co/hoy-juega-junior-con-cucuta-no-importar-que-sea-p..."},{"title":"Refugiados y migrantes de Venezuela durante la Crisis del COVID ...","displayLink":"www.acnur.org","formattedUrl":"https://www.acnur.org/.../news.../refugiados-y-migrantes-de-venezuela-dura..."}]</t>
+    <t>[{"title":"Zanubrutinib versus bendamustine and rituximab in untreated ...","displayLink":"www.thelancet.com","formattedUrl":"https://www.thelancet.com/journals/lanonc/article/PIIS1470...5/fulltext"},{"title":"Zilingo Investigation: Sequoia Representative Leaves Board Amid ...","displayLink":"www.bloomberg.com","formattedUrl":"https://www.bloomberg.com/.../sequoia-s-singh-leaves-zilingo-board-amid-..."},{"title":"Gallagher, Krishnamoorthi Probe Sequoia's PRC High-Tech ...","displayLink":"selectcommitteeontheccp.house.gov","formattedUrl":"http://selectcommitteeontheccp.house.gov/.../gallagher-krishnamoorthi-pro..."},{"title":"TBI, FBI joined search for 4-year-old girl missing from Memphis home","displayLink":"www.actionnews5.com","formattedUrl":"https://www.actionnews5.com/.../tbi-joins-search-4-year-old-girl-missing-h..."},{"title":"SEQUOIA Clinical Trial Fact Sheet | BeiGene","displayLink":"www.beigene.com","formattedUrl":"https://www.beigene.com/wp-content/uploads/.../SEQUOIA-Fact-Sheet.pdf"},{"title":"Sequoia: A Local Privilege Escalation Vulnerability in Linux's ...","displayLink":"blog.qualys.com","formattedUrl":"https://blog.qualys.com/.../sequoia-a-local-privilege-escalation-vulnerability..."},{"title":"Sequoia under investigation by US Congressional committee over ...","displayLink":"www.firstpost.com","formattedUrl":"https://www.firstpost.com/.../sequoia-under-investigation-by-us-congression..."},{"title":"Giant Sequoia - Save the Redwoods League","displayLink":"www.savetheredwoods.org","formattedUrl":"https://www.savetheredwoods.org/redwoods/giant-sequoias/"},{"title":"Jury finds man guilty of first-degree murder after a multi-agency ...","displayLink":"www.nps.gov","formattedUrl":"https://www.nps.gov/.../jury-finds-man-guilty-of-first-degree-murder-after-..."},{"title":"Eastern District of California | Mexican National Charged for Sexual ...","displayLink":"www.justice.gov","formattedUrl":"https://www.justice.gov/.../mexican-national-charged-sexual-assault-sequoia..."}]</t>
   </si>
   <si>
     <t>[["desabastecimiento","dificil "],["dificil ","desabastecimiento"],["desabastecimiento"," disminucion"],[" disminucion","desabastecimiento"],["desabastecimiento","aumentaria "],["aumentaria ","desabastecimiento"],["desabastecimiento"," aumento "],[" aumento ","desabastecimiento"],["desabastecimiento","masivo"],["masivo","desabastecimiento"],["desabastecimiento","reduccion "],["reduccion ","desabastecimiento"],["desabastecimiento","reducidas"],["reducidas","desabastecimiento"],["desabastecimiento","mayor "],["mayor ","desabastecimiento"],["desabastecimiento"," menor"],[" menor","desabastecimiento"],["desabastecimiento","grave "],["grave ","desabastecimiento"],["desabastecimiento"," agudo"],[" agudo","desabastecimiento"],["desabastecimiento","bajo "],["bajo ","desabastecimiento"],["desabastecimiento","alto"],["alto","desabastecimiento"],["desabastecimiento","intensa "],["intensa ","desabastecimiento"],["desabastecimiento"," extrema"],[" extrema","desabastecimiento"],["desabastecimiento","moderada "],["moderada ","desabastecimiento"],["desabastecimiento","mermado"],["mermado","desabastecimiento"],["desabastecimiento","severa "],["severa ","desabastecimiento"],["desabastecimiento"," leve"],[" leve","desabastecimiento"],["desabastecimiento","magnitud"],["magnitud","desabastecimiento"],["desabastecimiento","emergencia"],["emergencia","desabastecimiento"],["desabastecimiento","debajo del promedio "],["debajo del promedio ","desabastecimiento"],["desabastecimiento"," encima del promedio"],[" encima del promedio","desabastecimiento"],["desabastecimiento","severo "],["severo ","desabastecimiento"],["desabastecimiento"," severa"],[" severa","desabastecimiento"],["desabastecimiento","significativamente"],["significativamente","desabastecimiento"],["desabastecimiento","inusual"],["inusual","desabastecimiento"],["desabastecimiento","gravedad"],["gravedad","desabastecimiento"],["desabastecimiento","irregularidad"],["irregularidad","desabastecimiento"],["desabastecimiento","inadecuado"],["inadecuado","desabastecimiento"],["desabastecimiento","secan"],["secan","desabastecimiento"],["desabastecimiento","carencia"],["carencia","desabastecimiento"],["desabastecimiento","desviacion "],["desviacion ","desabastecimiento"],["desabastecimiento"," variacion"],[" variacion","desabastecimiento"],["racionamiento ","dificil "],["dificil ","racionamiento "],["racionamiento "," disminucion"],[" disminucion","racionamiento "],["racionamiento ","aumentaria "],["aumentaria ","racionamiento "],["racionamiento "," aumento "],[" aumento ","racionamiento "],["racionamiento ","masivo"],["masivo","racionamiento "],["racionamiento ","reduccion "],["reduccion ","racionamiento "],["racionamiento ","reducidas"],["reducidas","racionamiento "],["racionamiento ","mayor "],["mayor ","racionamiento "],["racionamiento "," menor"],[" menor","racionamiento "],["racionamiento ","grave "],["grave ","racionamiento "],["racionamiento "," agudo"],[" agudo","racionamiento "],["racionamiento ","bajo "],["bajo ","racionamiento "],["racionamiento ","alto"],["alto","racionamiento "],["racionamiento ","intensa "],["intensa ","racionamiento "],["racionamiento "," extrema"],[" extrema","racionamiento "],["racionamiento ","moderada "],["moderada ","racionamiento "],["racionamiento ","mermado"],["mermado","racionamiento "],["racionamiento ","severa "],["severa ","racionamiento "],["racionamiento "," leve"],[" leve","racionamiento "],["racionamiento ","magnitud"],["magnitud","racionamiento "],["racionamiento ","emergencia"],["emergencia","racionamiento "],["racionamiento ","debajo del promedio "],["debajo del promedio ","racionamiento "],["racionamiento "," encima del promedio"],[" encima del promedio","racionamiento "],["racionamiento ","severo "],["severo ","racionamiento "],["racionamiento "," severa"],[" severa","racionamiento "],["racionamiento ","significativamente"],["significativamente","racionamiento "],["racionamiento ","inusual"],["inusual","racionamiento "],["racionamiento ","gravedad"],["gravedad","racionamiento "],["racionamiento ","irregularidad"],["irregularidad","racionamiento "],["racionamiento ","inadecuado"],["inadecuado","racionamiento "],["racionamiento ","secan"],["secan","racionamiento "],["racionamiento ","carencia"],["carencia","racionamiento "],["racionamiento ","desviacion "],["desviacion ","racionamiento "],["racionamiento "," variacion"],[" variacion","racionamiento "],["ahorro","dificil "],["dificil ","ahorro"],["ahorro"," disminucion"],[" disminucion","ahorro"],["ahorro","aumentaria "],["aumentaria ","ahorro"],["ahorro"," aumento "],[" aumento ","ahorro"],["ahorro","masivo"],["masivo","ahorro"],["ahorro","reduccion "],["reduccion ","ahorro"],["ahorro","reducidas"],["reducidas","ahorro"],["ahorro","mayor "],["mayor ","ahorro"],["ahorro"," menor"],[" menor","ahorro"],["ahorro","grave "],["grave ","ahorro"],["ahorro"," agudo"],[" agudo","ahorro"],["ahorro","bajo "],["bajo ","ahorro"],["ahorro","alto"],["alto","ahorro"],["ahorro","intensa "],["intensa ","ahorro"],["ahorro"," extrema"],[" extrema","ahorro"],["ahorro","moderada "],["moderada ","ahorro"],["ahorro","mermado"],["mermado","ahorro"],["ahorro","severa "],["severa ","ahorro"],["ahorro"," leve"],[" leve","ahorro"],["ahorro","magnitud"],["magnitud","ahorro"],["ahorro","emergencia"],["emergencia","ahorro"],["ahorro","debajo del promedio "],["debajo del promedio ","ahorro"],["ahorro"," encima del promedio"],[" encima del promedio","ahorro"],["ahorro","severo "],["severo ","ahorro"],["ahorro"," severa"],[" severa","ahorro"],["ahorro","significativamente"],["significativamente","ahorro"],["ahorro","inusual"],["inusual","ahorro"],["ahorro","gravedad"],["gravedad","ahorro"],["ahorro","irregularidad"],["irregularidad","ahorro"],["ahorro","inadecuado"],["inadecuado","ahorro"],["ahorro","secan"],["secan","ahorro"],["ahorro","carencia"],["carencia","ahorro"],["ahorro","desviacion "],["desviacion ","ahorro"],["ahorro"," variacion"],[" variacion","ahorro"],["almacenamiento","dificil "],["dificil ","almacenamiento"],["almacenamiento"," disminucion"],[" disminucion","almacenamiento"],["almacenamiento","aumentaria "],["aumentaria ","almacenamiento"],["almacenamiento"," aumento "],[" aumento ","almacenamiento"],["almacenamiento","masivo"],["masivo","almacenamiento"],["almacenamiento","reduccion "],["reduccion ","almacenamiento"],["almacenamiento","reducidas"],["reducidas","almacenamiento"],["almacenamiento","mayor "],["mayor ","almacenamiento"],["almacenamiento"," menor"],[" menor","almacenamiento"],["almacenamiento","grave "],["grave ","almacenamiento"],["almacenamiento"," agudo"],[" agudo","almacenamiento"],["almacenamiento","bajo "],["bajo ","almacenamiento"],["almacenamiento","alto"],["alto","almacenamiento"],["almacenamiento","intensa "],["intensa ","almacenamiento"],["almacenamiento"," extrema"],[" extrema","almacenamiento"],["almacenamiento","moderada "],["moderada ","almacenamiento"],["almacenamiento","mermado"],["mermado","almacenamiento"],["almacenamiento","severa "],["severa ","almacenamiento"],["almacenamiento"," leve"],[" leve","almacenamiento"],["almacenamiento","magnitud"],["magnitud","almacenamiento"],["almacenamiento","emergencia"],["emergencia","almacenamiento"],["almacenamiento","debajo del promedio "],["debajo del promedio ","almacenamiento"],["almacenamiento"," encima del promedio"],[" encima del promedio","almacenamiento"],["almacenamiento","severo "],["severo ","almacenamiento"],["almacenamiento"," severa"],[" severa","almacenamiento"],["almacenamiento","significativamente"],["significativamente","almacenamiento"],["almacenamiento","inusual"],["inusual","almacenamiento"],["almacenamiento","gravedad"],["gravedad","almacenamiento"],["almacenamiento","irregularidad"],["irregularidad","almacenamiento"],["almacenamiento","inadecuado"],["inadecuado","almacenamiento"],["almacenamiento","secan"],["secan","almacenamiento"],["almacenamiento","carencia"],["carencia","almacenamiento"],["almacenamiento","desviacion "],["desviacion ","almacenamiento"],["almacenamiento"," variacion"],[" variacion","almacenamiento"],["aprovisionamiento","dificil "],["dificil ","aprovisionamiento"],["aprovisionamiento"," disminucion"],[" disminucion","aprovisionamiento"],["aprovisionamiento","aumentaria "],["aumentaria ","aprovisionamiento"],["aprovisionamiento"," aumento "],[" aumento ","aprovisionamiento"],["aprovisionamiento","masivo"],["masivo","aprovisionamiento"],["aprovisionamiento","reduccion "],["reduccion ","aprovisionamiento"],["aprovisionamiento","reducidas"],["reducidas","aprovisionamiento"],["aprovisionamiento","mayor "],["mayor ","aprovisionamiento"],["aprovisionamiento"," menor"],[" menor","aprovisionamiento"],["aprovisionamiento","grave "],["grave ","aprovisionamiento"],["aprovisionamiento"," agudo"],[" agudo","aprovisionamiento"],["aprovisionamiento","bajo "],["bajo ","aprovisionamiento"],["aprovisionamiento","alto"],["alto","aprovisionamiento"],["aprovisionamiento","intensa "],["intensa ","aprovisionamiento"],["aprovisionamiento"," extrema"],[" extrema","aprovisionamiento"],["aprovisionamiento","moderada "],["moderada ","aprovisionamiento"],["aprovisionamiento","mermado"],["mermado","aprovisionamiento"],["aprovisionamiento","severa "],["severa ","aprovisionamiento"],["aprovisionamiento"," leve"],[" leve","aprovisionamiento"],["aprovisionamiento","magnitud"],["magnitud","aprovisionamiento"],["aprovisionamiento","emergencia"],["emergencia","aprovisionamiento"],["aprovisionamiento","debajo del promedio "],["debajo del promedio ","aprovisionamiento"],["aprovisionamiento"," encima del promedio"],[" encima del promedio","aprovisionamiento"],["aprovisionamiento","severo "],["severo ","aprovisionamiento"],["aprovisionamiento"," severa"],[" severa","aprovisionamiento"],["aprovisionamiento","significativamente"],["significativamente","aprovisionamiento"],["aprovisionamiento","inusual"],["inusual","aprovisionamiento"],["aprovisionamiento","gravedad"],["gravedad","aprovisionamiento"],["aprovisionamiento","irregularidad"],["irregularidad","aprovisionamiento"],["aprovisionamiento","inadecuado"],["inadecuado","aprovisionamiento"],["aprovisionamiento","secan"],["secan","aprovisionamiento"],["aprovisionamiento","carencia"],["carencia","aprovisionamiento"],["aprovisionamiento","desviacion "],["desviacion ","aprovisionamiento"],["aprovisionamiento"," variacion"],[" variacion","aprovisionamiento"],["promedio","dificil "],["dificil ","promedio"],["promedio"," disminucion"],[" disminucion","promedio"],["promedio","aumentaria "],["aumentaria ","promedio"],["promedio"," aumento "],[" aumento ","promedio"],["promedio","masivo"],["masivo","promedio"],["promedio","reduccion "],["reduccion ","promedio"],["promedio","reducidas"],["reducidas","promedio"],["promedio","mayor "],["mayor ","promedio"],["promedio"," menor"],[" menor","promedio"],["promedio","grave "],["grave ","promedio"],["promedio"," agudo"],[" agudo","promedio"],["promedio","bajo "],["bajo ","promedio"],["promedio","alto"],["alto","promedio"],["promedio","intensa "],["intensa ","promedio"],["promedio"," extrema"],[" extrema","promedio"],["promedio","moderada "],["moderada ","promedio"],["promedio","mermado"],["mermado","promedio"],["promedio","severa "],["severa ","promedio"],["promedio"," leve"],[" leve","promedio"],["promedio","magnitud"],["magnitud","promedio"],["promedio","emergencia"],["emergencia","promedio"],["promedio","debajo del promedio "],["debajo del promedio ","promedio"],["promedio"," encima del promedio"],[" encima del promedio","promedio"],["promedio","severo "],["severo ","promedio"],["promedio"," severa"],[" severa","promedio"],["promedio","significativamente"],["significativamente","promedio"],["promedio","inusual"],["inusual","promedio"],["promedio","gravedad"],["gravedad","promedio"],["promedio","irregularidad"],["irregularidad","promedio"],["promedio","inadecuado"],["inadecuado","promedio"],["promedio","secan"],["secan","promedio"],["promedio","carencia"],["carencia","promedio"],["promedio","desviacion "],["desviacion ","promedio"],["promedio"," variacion"],[" variacion","promedio"],["suministro","dificil "],["dificil ","suministro"],["suministro"," disminucion"],[" disminucion","suministro"],["suministro","aumentaria "],["aumentaria ","suministro"],["suministro"," aumento "],[" aumento ","suministro"],["suministro","masivo"],["masivo","suministro"],["suministro","reduccion "],["reduccion ","suministro"],["suministro","reducidas"],["reducidas","suministro"],["suministro","mayor "],["mayor ","suministro"],["suministro"," menor"],[" menor","suministro"],["suministro","grave "],["grave ","suministro"],["suministro"," agudo"],[" agudo","suministro"],["suministro","bajo "],["bajo ","suministro"],["suministro","alto"],["alto","suministro"],["suministro","intensa "],["intensa ","suministro"],["suministro"," extrema"],[" extrema","suministro"],["suministro","moderada "],["moderada ","suministro"],["suministro","mermado"],["mermado","suministro"],["suministro","severa "],["severa ","suministro"],["suministro"," leve"],[" leve","suministro"],["suministro","magnitud"],["magnitud","suministro"],["suministro","emergencia"],["emergencia","suministro"],["suministro","debajo del promedio "],["debajo del promedio ","suministro"],["suministro"," encima del promedio"],[" encima del promedio","suministro"],["suministro","severo "],["severo ","suministro"],["suministro"," severa"],[" severa","suministro"],["suministro","significativamente"],["significativamente","suministro"],["suministro","inusual"],["inusual","suministro"],["suministro","gravedad"],["gravedad","suministro"],["suministro","irregularidad"],["irregularidad","suministro"],["suministro","inadecuado"],["inadecuado","suministro"],["suministro","secan"],["secan","suministro"],["suministro","carencia"],["carencia","suministro"],["suministro","desviacion "],["desviacion ","suministro"],["suministro"," variacion"],[" variacion","suministro"],["disponibilidad","dificil "],["dificil ","disponibilidad"],["disponibilidad"," disminucion"],[" disminucion","disponibilidad"],["disponibilidad","aumentaria "],["aumentaria ","disponibilidad"],["disponibilidad"," aumento "],[" aumento ","disponibilidad"],["disponibilidad","masivo"],["masivo","disponibilidad"],["disponibilidad","reduccion "],["reduccion ","disponibilidad"],["disponibilidad","reducidas"],["reducidas","disponibilidad"],["disponibilidad","mayor "],["mayor ","disponibilidad"],["disponibilidad"," menor"],[" menor","disponibilidad"],["disponibilidad","grave "],["grave ","disponibilidad"],["disponibilidad"," agudo"],[" agudo","disponibilidad"],["disponibilidad","bajo "],["bajo ","disponibilidad"],["disponibilidad","alto"],["alto","disponibilidad"],["disponibilidad","intensa "],["intensa ","disponibilidad"],["disponibilidad"," extrema"],[" extrema","disponibilidad"],["disponibilidad","moderada "],["moderada ","disponibilidad"],["disponibilidad","mermado"],["mermado","disponibilidad"],["disponibilidad","severa "],["severa ","disponibilidad"],["disponibilidad"," leve"],[" leve","disponibilidad"],["disponibilidad","magnitud"],["magnitud","disponibilidad"],["disponibilidad","emergencia"],["emergencia","disponibilidad"],["disponibilidad","debajo del promedio "],["debajo del promedio ","disponibilidad"],["disponibilidad"," encima del promedio"],[" encima del promedio","disponibilidad"],["disponibilidad","severo "],["severo ","disponibilidad"],["disponibilidad"," severa"],[" severa","disponibilidad"],["disponibilidad","significativamente"],["significativamente","disponibilidad"],["disponibilidad","inusual"],["inusual","disponibilidad"],["disponibilidad","gravedad"],["gravedad","disponibilidad"],["disponibilidad","irregularidad"],["irregularidad","disponibilidad"],["disponibilidad","inadecuado"],["inadecuado","disponibilidad"],["disponibilidad","secan"],["secan","disponibilidad"],["disponibilidad","carencia"],["carencia","disponibilidad"],["disponibilidad","desviacion "],["desviacion ","disponibilidad"],["disponibilidad"," variacion"],[" variacion","disponibilidad"],["volumen","dificil "],["dificil ","volumen"],["volumen"," disminucion"],[" disminucion","volumen"],["volumen","aumentaria "],["aumentaria ","volumen"],["volumen"," aumento "],[" aumento ","volumen"],["volumen","masivo"],["masivo","volumen"],["volumen","reduccion "],["reduccion ","volumen"],["volumen","reducidas"],["reducidas","volumen"],["volumen","mayor "],["mayor ","volumen"],["volumen"," menor"],[" menor","volumen"],["volumen","grave "],["grave ","volumen"],["volumen"," agudo"],[" agudo","volumen"],["volumen","bajo "],["bajo ","volumen"],["volumen","alto"],["alto","volumen"],["volumen","intensa "],["intensa ","volumen"],["volumen"," extrema"],[" extrema","volumen"],["volumen","moderada "],["moderada ","volumen"],["volumen","mermado"],["mermado","volumen"],["volumen","severa "],["severa ","volumen"],["volumen"," leve"],[" leve","volumen"],["volumen","magnitud"],["magnitud","volumen"],["volumen","emergencia"],["emergencia","volumen"],["volumen","debajo del promedio "],["debajo del promedio ","volumen"],["volumen"," encima del promedio"],[" encima del promedio","volumen"],["volumen","severo "],["severo ","volumen"],["volumen"," severa"],[" severa","volumen"],["volumen","significativamente"],["significativamente","volumen"],["volumen","inusual"],["inusual","volumen"],["volumen","gravedad"],["gravedad","volumen"],["volumen","irregularidad"],["irregularidad","volumen"],["volumen","inadecuado"],["inadecuado","volumen"],["volumen","secan"],["secan","volumen"],["volumen","carencia"],["carencia","volumen"],["volumen","desviacion "],["desviacion ","volumen"],["volumen"," variacion"],[" variacion","volumen"],["estancamiento","dificil "],["dificil ","estancamiento"],["estancamiento"," disminucion"],[" disminucion","estancamiento"],["estancamiento","aumentaria "],["aumentaria ","estancamiento"],["estancamiento"," aumento "],[" aumento ","estancamiento"],["estancamiento","masivo"],["masivo","estancamiento"],["estancamiento","reduccion "],["reduccion ","estancamiento"],["estancamiento","reducidas"],["reducidas","estancamiento"],["estancamiento","mayor "],["mayor ","estancamiento"],["estancamiento"," menor"],[" menor","estancamiento"],["estancamiento","grave "],["grave ","estancamiento"],["estancamiento"," agudo"],[" agudo","estancamiento"],["estancamiento","bajo "],["bajo ","estancamiento"],["estancamiento","alto"],["alto","estancamiento"],["estancamiento","intensa "],["intensa ","estancamiento"],["estancamiento"," extrema"],[" extrema","estancamiento"],["estancamiento","moderada "],["moderada ","estancamiento"],["estancamiento","mermado"],["mermado","estancamiento"],["estancamiento","severa "],["severa ","estancamiento"],["estancamiento"," leve"],[" leve","estancamiento"],["estancamiento","magnitud"],["magnitud","estancamiento"],["estancamiento","emergencia"],["emergencia","estancamiento"],["estancamiento","debajo del promedio "],["debajo del promedio ","estancamiento"],["estancamiento"," encima del promedio"],[" encima del promedio","estancamiento"],["estancamiento","severo "],["severo ","estancamiento"],["estancamiento"," severa"],[" severa","estancamiento"],["estancamiento","significativamente"],["significativamente","estancamiento"],["estancamiento","inusual"],["inusual","estancamiento"],["estancamiento","gravedad"],["gravedad","estancamiento"],["estancamiento","irregularidad"],["irregularidad","estancamiento"],["estancamiento","inadecuado"],["inadecuado","estancamiento"],["estancamiento","secan"],["secan","estancamiento"],["estancamiento","carencia"],["carencia","estancamiento"],["estancamiento","desviacion "],["desviacion ","estancamiento"],["estancamiento"," variacion"],[" variacion","estancamiento"],["agua","dificil "],["dificil ","agua"],["agua"," disminucion"],[" disminucion","agua"],["agua","aumentaria "],["aumentaria ","agua"],["agua"," aumento "],[" aumento ","agua"],["agua","masivo"],["masivo","agua"],["agua","reduccion "],["reduccion ","agua"],["agua","reducidas"],["reducidas","agua"],["agua","mayor "],["mayor ","agua"],["agua"," menor"],[" menor","agua"],["agua","grave "],["grave ","agua"],["agua"," agudo"],[" agudo","agua"],["agua","bajo "],["bajo ","agua"],["agua","alto"],["alto","agua"],["agua","intensa "],["intensa ","agua"],["agua"," extrema"],[" extrema","agua"],["agua","moderada "],["moderada ","agua"],["agua","mermado"],["mermado","agua"],["agua","severa "],["severa ","agua"],["agua"," leve"],[" leve","agua"],["agua","magnitud"],["magnitud","agua"],["agua","emergencia"],["emergencia","agua"],["agua","debajo del promedio "],["debajo del promedio ","agua"],["agua"," encima del promedio"],[" encima del promedio","agua"],["agua","severo "],["severo ","agua"],["agua"," severa"],[" severa","agua"],["agua","significativamente"],["significativamente","agua"],["agua","inusual"],["inusual","agua"],["agua","gravedad"],["gravedad","agua"],["agua","irregularidad"],["irregularidad","agua"],["agua","inadecuado"],["inadecuado","agua"],["agua","secan"],["secan","agua"],["agua","carencia"],["carencia","agua"],["agua","desviacion "],["desviacion ","agua"],["agua"," variacion"],[" variacion","agua"],["acueductos","dificil "],["dificil ","acueductos"],["acueductos"," disminucion"],[" disminucion","acueductos"],["acueductos","aumentaria "],["aumentaria ","acueductos"],["acueductos"," aumento "],[" aumento ","acueductos"],["acueductos","masivo"],["masivo","acueductos"],["acueductos","reduccion "],["reduccion ","acueductos"],["acueductos","reducidas"],["reducidas","acueductos"],["acueductos","mayor "],["mayor ","acueductos"],["acueductos"," menor"],[" menor","acueductos"],["acueductos","grave "],["grave ","acueductos"],["acueductos"," agudo"],[" agudo","acueductos"],["acueductos","bajo "],["bajo ","acueductos"],["acueductos","alto"],["alto","acueductos"],["acueductos","intensa "],["intensa ","acueductos"],["acueductos"," extrema"],[" extrema","acueductos"],["acueductos","moderada "],["moderada ","acueductos"],["acueductos","mermado"],["mermado","acueductos"],["acueductos","severa "],["severa ","acueductos"],["acueductos"," leve"],[" leve","acueductos"],["acueductos","magnitud"],["magnitud","acueductos"],["acueductos","emergencia"],["emergencia","acueductos"],["acueductos","debajo del promedio "],["debajo del promedio ","acueductos"],["acueductos"," encima del promedio"],[" encima del promedio","acueductos"],["acueductos","severo "],["severo ","acueductos"],["acueductos"," severa"],[" severa","acueductos"],["acueductos","significativamente"],["significativamente","acueductos"],["acueductos","inusual"],["inusual","acueductos"],["acueductos","gravedad"],["gravedad","acueductos"],["acueductos","irregularidad"],["irregularidad","acueductos"],["acueductos","inadecuado"],["inadecuado","acueductos"],["acueductos","secan"],["secan","acueductos"],["acueductos","carencia"],["carencia","acueductos"],["acueductos","desviacion "],["desviacion ","acueductos"],["acueductos"," variacion"],[" variacion","acueductos"],["caudal ","dificil "],["dificil ","caudal "],["caudal "," disminucion"],[" disminucion","caudal "],["caudal ","aumentaria "],["aumentaria ","caudal "],["caudal "," aumento "],[" aumento ","caudal "],["caudal ","masivo"],["masivo","caudal "],["caudal ","reduccion "],["reduccion ","caudal "],["caudal ","reducidas"],["reducidas","caudal "],["caudal ","mayor "],["mayor ","caudal "],["caudal "," menor"],[" menor","caudal "],["caudal ","grave "],["grave ","caudal "],["caudal "," agudo"],[" agudo","caudal "],["caudal ","bajo "],["bajo ","caudal "],["caudal ","alto"],["alto","caudal "],["caudal ","intensa "],["intensa ","caudal "],["caudal "," extrema"],[" extrema","caudal "],["caudal ","moderada "],["moderada ","caudal "],["caudal ","mermado"],["mermado","caudal "],["caudal ","severa "],["severa ","caudal "],["caudal "," leve"],[" leve","caudal "],["caudal ","magnitud"],["magnitud","caudal "],["caudal ","emergencia"],["emergencia","caudal "],["caudal ","debajo del promedio "],["debajo del promedio ","caudal "],["caudal "," encima del promedio"],[" encima del promedio","caudal "],["caudal ","severo "],["severo ","caudal "],["caudal "," severa"],[" severa","caudal "],["caudal ","significativamente"],["significativamente","caudal "],["caudal ","inusual"],["inusual","caudal "],["caudal ","gravedad"],["gravedad","caudal "],["caudal ","irregularidad"],["irregularidad","caudal "],["caudal ","inadecuado"],["inadecuado","caudal "],["caudal ","secan"],["secan","caudal "],["caudal ","carencia"],["carencia","caudal "],["caudal ","desviacion "],["desviacion ","caudal "],["caudal "," variacion"],[" variacion","caudal "],["caudales","dificil "],["dificil ","caudales"],["caudales"," disminucion"],[" disminucion","caudales"],["caudales","aumentaria "],["aumentaria ","caudales"],["caudales"," aumento "],[" aumento ","caudales"],["caudales","masivo"],["masivo","caudales"],["caudales","reduccion "],["reduccion ","caudales"],["caudales","reducidas"],["reducidas","caudales"],["caudales","mayor "],["mayor ","caudales"],["caudales"," menor"],[" menor","caudales"],["caudales","grave "],["grave ","caudales"],["caudales"," agudo"],[" agudo","caudales"],["caudales","bajo "],["bajo ","caudales"],["caudales","alto"],["alto","caudales"],["caudales","intensa "],["intensa ","caudales"],["caudales"," extrema"],[" extrema","caudales"],["caudales","moderada "],["moderada ","caudales"],["caudales","mermado"],["mermado","caudales"],["caudales","severa "],["severa ","caudales"],["caudales"," leve"],[" leve","caudales"],["caudales","magnitud"],["magnitud","caudales"],["caudales","emergencia"],["emergencia","caudales"],["caudales","debajo del promedio "],["debajo del promedio ","caudales"],["caudales"," encima del promedio"],[" encima del promedio","caudales"],["caudales","severo "],["severo ","caudales"],["caudales"," severa"],[" severa","caudales"],["caudales","significativamente"],["significativamente","caudales"],["caudales","inusual"],["inusual","caudales"],["caudales","gravedad"],["gravedad","caudales"],["caudales","irregularidad"],["irregularidad","caudales"],["caudales","inadecuado"],["inadecuado","caudales"],["caudales","secan"],["secan","caudales"],["caudales","carencia"],["carencia","caudales"],["caudales","desviacion "],["desviacion ","caudales"],["caudales"," variacion"],[" variacion","caudales"],["embalses","dificil "],["dificil ","embalses"],["embalses"," disminucion"],[" disminucion","embalses"],["embalses","aumentaria "],["aumentaria ","embalses"],["embalses"," aumento "],[" aumento ","embalses"],["embalses","masivo"],["masivo","embalses"],["embalses","reduccion "],["reduccion ","embalses"],["embalses","reducidas"],["reducidas","embalses"],["embalses","mayor "],["mayor ","embalses"],["embalses"," menor"],[" menor","embalses"],["embalses","grave "],["grave ","embalses"],["embalses"," agudo"],[" agudo","embalses"],["embalses","bajo "],["bajo ","embalses"],["embalses","alto"],["alto","embalses"],["embalses","intensa "],["intensa ","embalses"],["embalses"," extrema"],[" extrema","embalses"],["embalses","moderada "],["moderada ","embalses"],["embalses","mermado"],["mermado","embalses"],["embalses","severa "],["severa ","embalses"],["embalses"," leve"],[" leve","embalses"],["embalses","magnitud"],["magnitud","embalses"],["embalses","emergencia"],["emergencia","embalses"],["embalses","debajo del promedio "],["debajo del promedio ","embalses"],["embalses"," encima del promedio"],[" encima del promedio","embalses"],["embalses","severo "],["severo ","embalses"],["embalses"," severa"],[" severa","embalses"],["embalses","significativamente"],["significativamente","embalses"],["embalses","inusual"],["inusual","embalses"],["embalses","gravedad"],["gravedad","embalses"],["embalses","irregularidad"],["irregularidad","embalses"],["embalses","inadecuado"],["inadecuado","embalses"],["embalses","secan"],["secan","embalses"],["embalses","carencia"],["carencia","embalses"],["embalses","desviacion "],["desviacion ","embalses"],["embalses"," variacion"],[" variacion","embalses"],["fuente hidrica","dificil "],["dificil ","fuente hidrica"],["fuente hidrica"," disminucion"],[" disminucion","fuente hidrica"],["fuente hidrica","aumentaria "],["aumentaria ","fuente hidrica"],["fuente hidrica"," aumento "],[" aumento ","fuente hidrica"],["fuente hidrica","masivo"],["masivo","fuente hidrica"],["fuente hidrica","reduccion "],["reduccion ","fuente hidrica"],["fuente hidrica","reducidas"],["reducidas","fuente hidrica"],["fuente hidrica","mayor "],["mayor ","fuente hidrica"],["fuente hidrica"," menor"],[" menor","fuente hidrica"],["fuente hidrica","grave "],["grave ","fuente hidrica"],["fuente hidrica"," agudo"],[" agudo","fuente hidrica"],["fuente hidrica","bajo "],["bajo ","fuente hidrica"],["fuente hidrica","alto"],["alto","fuente hidrica"],["fuente hidrica","intensa "],["intensa ","fuente hidrica"],["fuente hidrica"," extrema"],[" extrema","fuente hidrica"],["fuente hidrica","moderada "],["moderada ","fuente hidrica"],["fuente hidrica","mermado"],["mermado","fuente hidrica"],["fuente hidrica","severa "],["severa ","fuente hidrica"],["fuente hidrica"," leve"],[" leve","fuente hidrica"],["fuente hidrica","magnitud"],["magnitud","fuente hidrica"],["fuente hidrica","emergencia"],["emergencia","fuente hidrica"],["fuente hidrica","debajo del promedio "],["debajo del promedio ","fuente hidrica"],["fuente hidrica"," encima del promedio"],[" encima del promedio","fuente hidrica"],["fuente hidrica","severo "],["severo ","fuente hidrica"],["fuente hidrica"," severa"],[" severa","fuente hidrica"],["fuente hidrica","significativamente"],["significativamente","fuente hidrica"],["fuente hidrica","inusual"],["inusual","fuente hidrica"],["fuente hidrica","gravedad"],["gravedad","fuente hidrica"],["fuente hidrica","irregularidad"],["irregularidad","fuente hidrica"],["fuente hidrica","inadecuado"],["inadecuado","fuente hidrica"],["fuente hidrica","secan"],["secan","fuente hidrica"],["fuente hidrica","carencia"],["carencia","fuente hidrica"],["fuente hidrica","desviacion "],["desviacion ","fuente hidrica"],["fuente hidrica"," variacion"],[" variacion","fuente hidrica"]]</t>
@@ -346,7 +346,7 @@
     <t>aumentaría / Aumento /masivo</t>
   </si>
   <si>
-    <t>[{"title":"BAJO EL AGUA está Cúcuta por las fuertes lluvias que dejan ríos ...","displayLink":"impactovenezuela.com","formattedUrl":"https://impactovenezuela.com/bajo-el-agua-esta-cucuta-por-las-fuertes-lluvi..."},{"title":"Venezuela Rejects Any Link With an Attack on Colombian Soldiers ...","displayLink":"www.telesurenglish.net","formattedUrl":"https://www.telesurenglish.net/news/Venezuela-Rejects-Any-Link-With-an-..."},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"La violencia armada se agudiza y genera desplazamientos masivos ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2020/08/1478272"},{"title":"MeteoNews: Tiempo Cúcuta","displayLink":"meteonews.co","formattedUrl":"http://meteonews.co/es/Place/G3685533/Cúcuta"},{"title":"Fuertes lluvias generaron múltiples emergencias en Cúcuta | RCN ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../fuertes-lluvias-generaron-multiples-emergenci..."},{"title":"MeteoNews: Valores de medición Cúcuta","displayLink":"meteonews.co","formattedUrl":"http://meteonews.co/es/Measurements/M80097000/Cúcuta"},{"title":"Fuertes lluvias en Cúcuta dejan más de 100 familias afectadas ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../fuertes-lluvias-en-cucuta-dejan-mas-de-100-fa..."},{"title":"Cuatro muertos y ocho desaparecidos deja emergencia invernal en ...","displayLink":"www.elpais.com.co","formattedUrl":"https://www.elpais.com.co/.../inundacion-tras-fuertes-lluvias-en-cucuta-deja..."},{"title":"Heladas podrían afectar trigo de Argentina; se prevé más lluvia ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-granos-argentina-clima-idLTASI..."}]</t>
+    <t>[{"title":"Fuertes lluvias inundan viviendas de Massachusetts y hacen ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/us.../general-news-22c110a74c205079cab7e32a87eb3b..."},{"title":"Milímetros de agua aplicados en cada riego y precipitaciones ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-3-Milimetros-de-agua-aplicados-en-..."},{"title":"Lluvias azotan norte de Chile y dejan al menos dos muertos; minas ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../portada-clima-chile-lluvias-idLTAKBN0ML2N..."},{"title":"Promedio de precipitaciones y temperaturas 2004 -2016. Se ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-3-Promedio-de-precipitaciones-y-te..."},{"title":"Precipitation formation from orographic cloud seeding | PNAS","displayLink":"www.pnas.org","formattedUrl":"https://www.pnas.org/doi/10.1073/pnas.1716995115"},{"title":"Climate Change Is Altering Rainfall Patterns Worldwide | Scientific ...","displayLink":"www.scientificamerican.com","formattedUrl":"https://www.scientificamerican.com/.../climate-change-is-altering-rainfall-pa..."},{"title":"The Amazon rainforest is approaching a tipping point in Rio Branco ...","displayLink":"www.washingtonpost.com","formattedUrl":"https://www.washingtonpost.com/world/.../amazon-brazil-tipping-point/"},{"title":"Climate change, rainfall, and social conflict in Africa - Cullen S ...","displayLink":"journals.sagepub.com","formattedUrl":"https://journals.sagepub.com/doi/abs/10.1177/0022343311426165"},{"title":"Deforestation reduces rainfall and agricultural revenues in the ...","displayLink":"www.nature.com","formattedUrl":"https://www.nature.com/articles/s41467-021-22840-7"},{"title":"Weather Research &amp; Forecasting Model (WRF) | Mesoscale ...","displayLink":"www.mmm.ucar.edu","formattedUrl":"https://www.mmm.ucar.edu/models/wrf"}]</t>
   </si>
   <si>
     <t>3. Cantidad</t>
@@ -361,7 +361,7 @@
     <t>reducción /reducidas</t>
   </si>
   <si>
-    <t>[{"title":"Agricultores Argentina cosechan soja y maíz con rindes dispares ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../granos-argentina-gobierno-idARL1N0CE9ML2..."},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"DIAGNOSIS OF WATER IN THE AMERICAS","displayLink":"ianas.org","formattedUrl":"https://ianas.org/wp-content/uploads/2020/07/08-Diagnosis-of-water.pdf"},{"title":"AF-DIGITAL-CORREGIDO-El Agua como Derecho Humano-3.indd","displayLink":"www.corteidh.or.cr","formattedUrl":"https://www.corteidh.or.cr/docs/.../El_Agua_como_Derecho_Humano.pdf"},{"title":"Huella Ecológica del sector Textil-Confección en Colombia para el ...","displayLink":"repository.javeriana.edu.co","formattedUrl":"https://repository.javeriana.edu.co/bitstream/.../SENTENAM-TESIS.pdf?...2"},{"title":"JoomShaper: Responsive Joomla Templates &amp; Premium Themes Club","displayLink":"www.joomshaper.com","formattedUrl":"https://www.joomshaper.com/"},{"title":"Search &amp; Browse shapefile | | Page 1 of 1 | Datos Abiertos Colombia","displayLink":"colombia-mintic.data.socrata.com","formattedUrl":"https://colombia-mintic.data.socrata.com/en/browse?tags=shapefile&amp;utf8..."},{"title":"Volumen 61 • Número 1 • Enero-abril 2019 • ISSN 1794-3108 • 1 ...","displayLink":"www.policia.gov.co","formattedUrl":"https://www.policia.gov.co/sites/default/.../revista-criminalidad_61_-1_1.pd..."},{"title":"Desafíos del agua urbana en las Américas: perspectivas de las ...","displayLink":"unesdoc.unesco.org","formattedUrl":"https://unesdoc.unesco.org/ark:/48223/pf0000245202"}]</t>
+    <t>[{"title":"Dehydration markedly impairs cardiovascular function in ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/9104860/"},{"title":"Influencia del déficit hídrico sobre la producción de granos de polen ...","displayLink":"go.gale.com","formattedUrl":"https://go.gale.com/ps/i.do?id...sid=googleScholar..."},{"title":"DÉFICIT HÍDRICO E ALTAS TEMPERATURAS NO METABOLISMO ...","displayLink":"periodicoscientificos.ufmt.br","formattedUrl":"https://periodicoscientificos.ufmt.br/ojs/index.php/nativa/article/.../1855"},{"title":"Brasil - DÉFICIT HÍDRICO E OS PROCESSOS ... - SciELO","displayLink":"www.scielo.br","formattedUrl":"https://www.scielo.br/j/rbeaa/a/sptHSNGpfSCjGZ656yBJwnN/"},{"title":"-Umidade gravimétrica do solo (Ug) durante o período de déficit ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../FIGURA-1-Umidade-gravimetrica-do-solo-..."},{"title":"INFLUÊNCIA DO DÉFICIT HÍDRICO NO DESENVOLVIMENTO ...","displayLink":"revistas.fca.unesp.br","formattedUrl":"https://revistas.fca.unesp.br/index.php/irriga/article/view/196"},{"title":"(PDF) Control de la fotosíntesis en especies xerófitas durante déficit ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../272174305_Control_de_la_fotosintesis_en..."},{"title":"Vista de Déficit hídrico controlado y su efecto en el rendimiento y ...","displayLink":"cienciasagricolas.inifap.gob.mx","formattedUrl":"https://cienciasagricolas.inifap.gob.mx/index.php/agricolas/article/.../6240"},{"title":"Rizobactérias multifuncionais na mitigação do déficit hídrico e da ...","displayLink":"repositorio.bc.ufg.br","formattedUrl":"https://repositorio.bc.ufg.br/tede/handle/tede/11357"},{"title":"Aplicação exógena de tiamina em arroz de terras altas submetido ...","displayLink":"revistas.udesc.br","formattedUrl":"https://revistas.udesc.br/index.php/agroveterinaria/article/view/14751"}]</t>
   </si>
   <si>
     <t>4. Calidad</t>
@@ -376,7 +376,7 @@
     <t>mayor / menor</t>
   </si>
   <si>
-    <t>[{"title":"Tags | Postlatino","displayLink":"postlatino.com","formattedUrl":"https://postlatino.com/tags/"},{"title":"ESTUDIO DE FACTIBILIDAD PARA LA CREACIÓN DE CROKS ...","displayLink":"bibliotecadigital.univalle.edu.co","formattedUrl":"https://bibliotecadigital.univalle.edu.co/bitstream/.../CB-0586730.pdf?...1..."},{"title":"Rae - ID:5ce06b6fd99d3","displayLink":"baixardoc.com","formattedUrl":"https://baixardoc.com/documents/rae-5ce06b6fd99d3?session...id..."},{"title":"https://huggingface.co/datasets/jucadiaz/dataton_t...","displayLink":"huggingface.co","formattedUrl":"https://huggingface.co/.../b359fd18f7478830402c7ff01e1098231c3c82b5...."},{"title":"Tomo 59 by UNIVERSIDAD SIMON BOLIVAR - Issuu","displayLink":"issuu.com","formattedUrl":"https://issuu.com/universidadsimonbolivar/docs/tomo_59"},{"title":"Sin título-1","displayLink":"cojowa.edu.co","formattedUrl":"https://cojowa.edu.co/wp-content/uploads/2019/12/regiones-6.pdf"},{"title":"MONTAJE A LIBRO","displayLink":"www.centrodeestudiosaeronauticos.edu.co","formattedUrl":"http://www.centrodeestudiosaeronauticos.edu.co/.../Libro%20La%20investi..."},{"title":"Exilios y otros desarraigos. 22 años de Letralia","displayLink":"letralia.com","formattedUrl":"https://letralia.com/wp-content/uploads/editorial/22.pdf"},{"title":"Programa 06/02/23 | Sigue con la información en #ATVNoticias ...","displayLink":"www.facebook.com","formattedUrl":"https://www.facebook.com/ATVNoticias9/videos/.../1427636660974231/"}]</t>
+    <t>[{"title":"La primera Alerta de Tormenta Tropical registrada en la historia de ...","displayLink":"yaleclimateconnections.org","formattedUrl":"https://yaleclimateconnections.org/.../la-primera-alerta-de-tormenta-tropical..."},{"title":"Preparación para Emergencias. Prepárate. ¡Puede Pasar! El ...","displayLink":"www.chicago.gov","formattedUrl":"https://www.chicago.gov/content/.../AFN_GearUpGetReady-Reader_sp.pdf"},{"title":"¿Se acabó la sequía en California? Los proveedores de agua aún ...","displayLink":"calmatters.org","formattedUrl":"https://calmatters.org/.../se-acabo-la-sequia-en-california-los-proveedores-d..."},{"title":"Tormentas locales severas tropicales","displayLink":"www.meted.ucar.edu","formattedUrl":"https://www.meted.ucar.edu/tropical/synoptic/local_storms_es/print.php"},{"title":"Cumulonimbus - Wikipedia, la enciclopedia libre","displayLink":"es.wikipedia.org","formattedUrl":"https://es.wikipedia.org/wiki/Cumulonimbus"},{"title":"AMÉRICA LATINA","displayLink":"www.r4v.info","formattedUrl":"https://www.r4v.info/.../ACH-EXTERNO_Boletin-Regional_FEN-2023.pdf"},{"title":"CAPÍTULO 6 Distribución de la humedad y precipitación","displayLink":"www.meted.ucar.edu","formattedUrl":"https://www.meted.ucar.edu/tropical/textbook.../Cap6_Humedad_Precip.pd..."},{"title":"Papel del sistema inmune en la infección por el SARS-CoV-2 ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8158328/"},{"title":"Uso segurodel agua para el reúso","displayLink":"climatesmartwater.org","formattedUrl":"https://climatesmartwater.org/.../AIDIS-Uso_seguro_del_agua_26_sep.pdf"},{"title":"APÉNDICE 1. DIAGNÓSTICO","displayLink":"www.miteco.gob.es","formattedUrl":"https://www.miteco.gob.es/content/...y.../apendice1-2_tcm30-451140.pdf"}]</t>
   </si>
   <si>
     <t>4. Género</t>
@@ -391,7 +391,7 @@
     <t>grave / agudo</t>
   </si>
   <si>
-    <t>[{"title":"Colombia – Floods Affect 1,700 Families in Barbacoas, Nariño ...","displayLink":"floodlist.com","formattedUrl":"https://floodlist.com/america/colombia-floods-barbacoas-april-2021"},{"title":"Inundaciones afectan a 1.500 familias en Cúcuta, Colombia ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/inundaciones-riada-quebrada-cucuta-colomb..."},{"title":"Colombia: Rains Leave 47 Dead and Over 18,000 Families Affected ...","displayLink":"www.telesurenglish.net","formattedUrl":"https://www.telesurenglish.net/news/Colombia-Rains-Leave-47-Dead-and-O..."},{"title":"Inundaciones amenazan a Colombia ante abandono estatal ...","displayLink":"www.telesurtv.net","formattedUrl":"https://www.telesurtv.net/news/inundaciones-amenazan-colombia-ante-aban..."},{"title":"El Pase De Cucuta | TikTok","displayLink":"www.tiktok.com","formattedUrl":"https://www.tiktok.com/find/el-pase-de-cucuta"},{"title":"Presidente Obama visita Nueva Jersey tras inundaciones por Irene ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-irene-obama-idLTASIE7A7NA32..."},{"title":"BAJO EL AGUA está Cúcuta por las fuertes lluvias que dejan ríos ...","displayLink":"impactovenezuela.com","formattedUrl":"https://impactovenezuela.com/bajo-el-agua-esta-cucuta-por-las-fuertes-lluvi..."},{"title":"Gasolina más barata del mundo desata contrabando andino | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-venezuela-colombia-contrab-idL..."},{"title":"Países enteros podrían desaparecer para siempre con el aumento ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/02/1518587"},{"title":"Emergencia en La Guajira por el invierno: fuertes lluvias provocaron ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../emergencia-en-la-guajira-por-el-invierno-fuert..."}]</t>
+    <t>[{"title":"FEMA Case Study Library | FEMA.gov","displayLink":"www.fema.gov","formattedUrl":"https://www.fema.gov/es/emergency-managers/.../case-study-library"},{"title":"Flood Risk Management","displayLink":"www.usace.army.mil","formattedUrl":"https://www.usace.army.mil/Missions/Civil.../Flood-Risk-Management/"},{"title":"Office of Professional Responsibility | FEMA.gov","displayLink":"www.fema.gov","formattedUrl":"https://www.fema.gov/es/about/offices/professional-responsibility"},{"title":"Floods | Ready.gov","displayLink":"www.ready.gov","formattedUrl":"https://www.ready.gov/floods"},{"title":"Floodplain Management | FEMA.gov","displayLink":"www.fema.gov","formattedUrl":"https://www.fema.gov/es/floodplain-management"},{"title":"Health department investigating flood at Suncor | Department of ...","displayLink":"cdphe.colorado.gov","formattedUrl":"https://cdphe.colorado.gov/.../health-department-investigating-flood-at-sun..."},{"title":"What to Expect After Applying | FEMA.gov","displayLink":"www.fema.gov","formattedUrl":"https://www.fema.gov/es/careers/after-applying"},{"title":"Tabla 2. Variables estudiadas según exposición al riesgo de ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Tabla-2-Variables-estudiadas-segun-exposic..."},{"title":"La gran inundación | Smithsonian Tropical Research Institute","displayLink":"stri.si.edu","formattedUrl":"https://stri.si.edu/es/noticia/la-gran-inundacion"},{"title":"Sobreviví la gran inundación de melaza,... by Tarshis, Lauren","displayLink":"www.amazon.com","formattedUrl":"https://www.amazon.com/Sobreviví-inundación-Survived.../1338859374"}]</t>
   </si>
   <si>
     <t>Humedad</t>
@@ -403,7 +403,7 @@
     <t>bajo /alto</t>
   </si>
   <si>
-    <t>[{"title":"Crisis en Venezuela: qué tienen los kits de \"ayuda humanitaria\" que ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-47328944"},{"title":"Corponor celebró Día Mundial de la Tierra en Norte de Santander","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/2364-corponor-celebro-dia-mundial-de-la-t..."},{"title":"Qué es el estrés térmico que los científicos piden incluir en las ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-65429152"},{"title":"Heladas podrían afectar trigo de Argentina; se prevé más lluvia ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-granos-argentina-clima-idLTASI..."},{"title":"(PDF) Análisis estadístico de variables climatológicas en la ciudad ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../324825840_Analisis_estadistico_de_variabl..."},{"title":"Heladas se suman a la sequía que castiga a trigo de Argentina ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/granos-argentina-trigo-idARL1N2FM1NL/"},{"title":"Cómo el clima afecta a los insectos – Insectos después de la lluvia ...","displayLink":"www.raid.com","formattedUrl":"https://www.raid.com/es-US/education/bug.../how-weather-affects-insects"},{"title":"Economía de Cúcuta - Wikipedia, la enciclopedia libre","displayLink":"es.wikipedia.org","formattedUrl":"https://es.wikipedia.org/wiki/Economía_de_Cúcuta"},{"title":"Venezuelan refugees struggled to find healthcare in Colombia. That ...","displayLink":"www.tampabay.com","formattedUrl":"https://www.tampabay.com/.../venezuelan-refugees-struggled-to-find-health..."},{"title":"Dr. Stanley Escalante | Otorrinolaringólogo (@dr.stanleyescalante ...","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/dr.stanleyescalante/?hl=en"}]</t>
+    <t>[{"title":"Moisture retention of glycerin solutions with various concentrations ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9205919/"},{"title":"Curvas polinómicas del comportamiento de la densidad y humedad ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-2-Curvas-polinomicas-del-comporta..."},{"title":"dod instruction 8010.01 department of defense information network ...","displayLink":"www.esd.whs.mil","formattedUrl":"https://www.esd.whs.mil/Portals/54/Documents/DD/.../dodi/801001p.pdf"},{"title":"Study Finds PFAS in Most Stain- and Water-Resistant Textiles","displayLink":"www.verywellhealth.com","formattedUrl":"https://www.verywellhealth.com/pfas-water-stain-resistant-products-5217827"},{"title":"Humidity – the second pillar of climate change - Met Office","displayLink":"www.metoffice.gov.uk","formattedUrl":"https://www.metoffice.gov.uk/.../scientists-investigate-humidity---the-secon..."},{"title":"Engineer deploys research on 'mud batteries' for powering ...","displayLink":"news.ucsc.edu","formattedUrl":"https://news.ucsc.edu/2022/11/josephson-mud-batteries.html"},{"title":"Blood Flow Restriction Exercise: A Systematic Review of the Literature","displayLink":"touroscholar.touro.edu","formattedUrl":"https://touroscholar.touro.edu/cgi/viewcontent.cgi?article=1045...chhs..."},{"title":"Study of moisture absorption characteristics of cotton terry towel fabrics","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/pii/S1877705817328898"},{"title":"Mold","displayLink":"www.cdph.ca.gov","formattedUrl":"https://www.cdph.ca.gov/Programs/CCDPHP/DEODC/EHLB/.../Mold.aspx"},{"title":"Flu virus' best friend: low humidity | YaleNews","displayLink":"news.yale.edu","formattedUrl":"https://news.yale.edu/2019/05/13/flu-virus-best-friend-low-humidity"}]</t>
   </si>
   <si>
     <t>sed</t>
@@ -415,7 +415,7 @@
     <t>intensa / extrema</t>
   </si>
   <si>
-    <t>[{"title":"Keeping Hope Alive for Venezuelans in Colombia | Project HOPE","displayLink":"www.projecthope.org","formattedUrl":"https://www.projecthope.org/keeping-hope-alive-venezuelans/"},{"title":"Venezuela's Guaidó pictured with members of Colombian gang ...","displayLink":"www.theguardian.com","formattedUrl":"https://www.theguardian.com/.../juan-guaido-faces-questions-over-links-to-..."},{"title":"Politicians and Police Linked to Colombian Child Sex Ring","displayLink":"insightcrime.org","formattedUrl":"https://insightcrime.org/news/politicians-and-police-linked-to-colombian-ch..."},{"title":"Sem Cucuta","displayLink":"www.semcucuta.gov.co","formattedUrl":"https://www.semcucuta.gov.co/"},{"title":"Stream Jhoan Contreras Dj music | Listen to songs, albums, playlists ...","displayLink":"soundcloud.com","formattedUrl":"https://soundcloud.com/jhoan-contreras-74067127"},{"title":"Miami International Airport","displayLink":"www.miami-airport.com","formattedUrl":"https://www.miami-airport.com/"},{"title":"Off base","displayLink":"www.economist.com","formattedUrl":"https://www.economist.com/the-americas/2009/12/03/off-base"},{"title":"May 2020 – CIRE","displayLink":"cire-bristol.com","formattedUrl":"https://cire-bristol.com/2020/05/"},{"title":"Colombia - Y. Aponzá - Profile with news, career statistics and ...","displayLink":"us.soccerway.com","formattedUrl":"https://us.soccerway.com/players/yilber-steven-aponza-carabali/476982/"},{"title":"Sport Shop - Relojes Y Oro Cucuta","displayLink":"www.relojesyorocucuta.com","formattedUrl":"https://www.relojesyorocucuta.com/demos/shop-demos/sport-shop/"}]</t>
+    <t>[{"title":"SED Staff Wildfire Investigations","displayLink":"www.cpuc.ca.gov","formattedUrl":"https://www.cpuc.ca.gov/industries-and.../wildfires-staff-investigations"},{"title":"Survey of Earned Doctorates Field of Study Taxonomy Changes in ...","displayLink":"ncses.nsf.gov","formattedUrl":"https://ncses.nsf.gov/pubs/ncses23200"},{"title":"CALIFORNIA PUBLIC UTILITIES COMMISSION Safety and ...","displayLink":"www.cpuc.ca.gov","formattedUrl":"https://www.cpuc.ca.gov/-/.../investigations.../public-sed-investigation-repor..."},{"title":"Survey of Earned Doctorates (SED) 2022 | NSF - National Science ...","displayLink":"www.nsf.gov","formattedUrl":"https://www.nsf.gov/statistics/srvydoctorates/"},{"title":"The ED-SED Study: A Multicenter, Prospective Cohort Study of ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/31393323/"},{"title":"dnd 5e - When is Passive Investigation used? - Role-playing Games ...","displayLink":"rpg.stackexchange.com","formattedUrl":"https://rpg.stackexchange.com/questions/.../when-is-passive-investigation-us..."},{"title":"Machine Bias — ProPublica","displayLink":"www.propublica.org","formattedUrl":"https://www.propublica.org/.../machine-bias-risk-assessments-in-criminal-se..."},{"title":"SED RS 600 » Academics | Boston University","displayLink":"www.bu.edu","formattedUrl":"https://www.bu.edu/academics/wheelock/courses/sed-rs-600/"},{"title":"John and Polly Sparks Early Career Grant for Psychologists ...","displayLink":"apf.apa.org","formattedUrl":"https://apf.apa.org/funding/sparks/"},{"title":"High‐resolution synchrotron X‐ray fluorescence investigation of ...","displayLink":"onlinelibrary.wiley.com","formattedUrl":"https://onlinelibrary.wiley.com/doi/abs/10.1111/sed.12607"}]</t>
   </si>
   <si>
     <t>Recurso energético</t>
@@ -430,7 +430,7 @@
     <t>generación</t>
   </si>
   <si>
-    <t>[{"title":"Atentado en aeropuerto de Colombia; al menos tres muertos","displayLink":"www.dallasnews.com","formattedUrl":"https://www.dallasnews.com/.../explosion-aeropuerto-cucuta-colombia-poli..."},{"title":"La Opinión, Cúcuta","displayLink":"www.laopinion.com.co","formattedUrl":"https://www.laopinion.com.co/"},{"title":"Así será el gran apagón en Cúcuta contra CENS este martes 8 de ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/asi-sera.../202210/"},{"title":"Por qué cada vez hay más apagones en Cuba y cómo un vecindario ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-62187814"},{"title":"Táchira News - Táchira enfrenta ola de apagones y cortes ...","displayLink":"www.facebook.com","formattedUrl":"https://www.facebook.com/TachiraNews/...apagones...httpswwwtachiranews..."},{"title":"Prohíben a enviados del CIDH visitar Venezuela; recabarán datos ...","displayLink":"jp.reuters.com","formattedUrl":"https://jp.reuters.com/article/venezuela-cidh-idLTAKBN1ZY29X"},{"title":"Venezuela apresura importación de combustible tras fallas en ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-venezuela-petroleo-idLTAKCN0I..."},{"title":"Miles de colombianos podrían quedarse sin luz: comercializadora le ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../habra-apagon-en-colombia-dieron-ultimatum-a..."},{"title":"Boeing, Air Lease close $2.5 billion order | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/boeing-idCNN1E77E0C420110815/"},{"title":"Cuatro años después, ¿qué ha pasado con la frontera ...","displayLink":"migravenezuela.com","formattedUrl":"https://migravenezuela.com/.../cuatro-anos-despues-que-ha-pasado-con-la-f..."}]</t>
+    <t>[{"title":"Opinion | Betrayal and Blackouts in Puerto Rico - The New York Times","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/2022/09/22/.../puerto-rico-fiona-power-luma.htm..."},{"title":"California releases final root cause analysis of August rolling ...","displayLink":"www.utilitydive.com","formattedUrl":"https://www.utilitydive.com/news/california-releases-final.../593436/"},{"title":"Los apagones en India empañan la recuperación económica de ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../oesbs-india-carb-n-apagones-idESKBN0H00W..."},{"title":"Ukraine Searches For Culprit After Cyberattacks On Finance Ministry ...","displayLink":"www.rferl.org","formattedUrl":"https://www.rferl.org/a/ukraine-cyberattacks-finance.../28172004.html"},{"title":"Across Wisconsin, elderly at risk as residents wait weeks without ...","displayLink":"www.wsaw.com","formattedUrl":"https://www.wsaw.com/.../Across-Wisconsin-elderly-residents-wait-weeks-w..."},{"title":"Frozen Out in Texas: Blackouts and Inequity","displayLink":"www.rockefellerfoundation.org","formattedUrl":"https://www.rockefellerfoundation.org/.../frozen-out-in-texas-blackouts-and..."},{"title":"CAISO: Final Root Cause Analysis Mid-August 2020 Extreme Heat ...","displayLink":"www.caiso.com","formattedUrl":"http://www.caiso.com/.../Final-Root-Cause-Analysis-Mid-August-2020-Extr..."},{"title":"Winter storm blackouts plagued Texas in 2011, too ...","displayLink":"www.usatoday.com","formattedUrl":"https://www.usatoday.com/story/news/nation/2021/.../4490501001/"},{"title":"Con posibles apagones a medida que se acerca la tormenta tropical ...","displayLink":"rivcodpss.org","formattedUrl":"https://rivcodpss.org/.../con-posibles-apagones-medida-que-se-acerca-la-tor..."},{"title":"Centerpoint Outage Tracker","displayLink":"gis.centerpointenergy.com","formattedUrl":"https://gis.centerpointenergy.com/outagetracker/?WT.ac=OC_Image..."}]</t>
   </si>
   <si>
     <t>[["generacion","dificil "],["dificil ","generacion"],["generacion"," disminucion"],[" disminucion","generacion"],["generacion","aumentar "],["aumentar ","generacion"],["generacion"," aumento "],[" aumento ","generacion"],["generacion","masivo"],["masivo","generacion"],["generacion","reduccion "],["reduccion ","generacion"],["generacion","reducidas"],["reducidas","generacion"],["generacion","mayor "],["mayor ","generacion"],["generacion"," menor"],[" menor","generacion"],["generacion","grave "],["grave ","generacion"],["generacion"," agudo"],[" agudo","generacion"],["generacion","bajo "],["bajo ","generacion"],["generacion","alto"],["alto","generacion"],["generacion","intensa "],["intensa ","generacion"],["generacion"," extrema"],[" extrema","generacion"],["generacion","moderada "],["moderada ","generacion"],["generacion","mermado"],["mermado","generacion"],["generacion","severa "],["severa ","generacion"],["generacion"," leve"],[" leve","generacion"],["generacion","magnitud"],["magnitud","generacion"],["generacion","emergencia"],["emergencia","generacion"],["generacion","debajo del promedio "],["debajo del promedio ","generacion"],["generacion"," encima del promedio"],[" encima del promedio","generacion"],["generacion","severo "],["severo ","generacion"],["generacion"," severa"],[" severa","generacion"],["generacion","significativamente"],["significativamente","generacion"],["generacion","inusual"],["inusual","generacion"],["generacion","gravedad"],["gravedad","generacion"],["generacion","irregularidad"],["irregularidad","generacion"],["generacion","inadecuado"],["inadecuado","generacion"],["generacion","caido"],["caido","generacion"],["funcionamiento","dificil "],["dificil ","funcionamiento"],["funcionamiento"," disminucion"],[" disminucion","funcionamiento"],["funcionamiento","aumentar "],["aumentar ","funcionamiento"],["funcionamiento"," aumento "],[" aumento ","funcionamiento"],["funcionamiento","masivo"],["masivo","funcionamiento"],["funcionamiento","reduccion "],["reduccion ","funcionamiento"],["funcionamiento","reducidas"],["reducidas","funcionamiento"],["funcionamiento","mayor "],["mayor ","funcionamiento"],["funcionamiento"," menor"],[" menor","funcionamiento"],["funcionamiento","grave "],["grave ","funcionamiento"],["funcionamiento"," agudo"],[" agudo","funcionamiento"],["funcionamiento","bajo "],["bajo ","funcionamiento"],["funcionamiento","alto"],["alto","funcionamiento"],["funcionamiento","intensa "],["intensa ","funcionamiento"],["funcionamiento"," extrema"],[" extrema","funcionamiento"],["funcionamiento","moderada "],["moderada ","funcionamiento"],["funcionamiento","mermado"],["mermado","funcionamiento"],["funcionamiento","severa "],["severa ","funcionamiento"],["funcionamiento"," leve"],[" leve","funcionamiento"],["funcionamiento","magnitud"],["magnitud","funcionamiento"],["funcionamiento","emergencia"],["emergencia","funcionamiento"],["funcionamiento","debajo del promedio "],["debajo del promedio ","funcionamiento"],["funcionamiento"," encima del promedio"],[" encima del promedio","funcionamiento"],["funcionamiento","severo "],["severo ","funcionamiento"],["funcionamiento"," severa"],[" severa","funcionamiento"],["funcionamiento","significativamente"],["significativamente","funcionamiento"],["funcionamiento","inusual"],["inusual","funcionamiento"],["funcionamiento","gravedad"],["gravedad","funcionamiento"],["funcionamiento","irregularidad"],["irregularidad","funcionamiento"],["funcionamiento","inadecuado"],["inadecuado","funcionamiento"],["funcionamiento","caido"],["caido","funcionamiento"],["desabastecimiento","dificil "],["dificil ","desabastecimiento"],["desabastecimiento"," disminucion"],[" disminucion","desabastecimiento"],["desabastecimiento","aumentar "],["aumentar ","desabastecimiento"],["desabastecimiento"," aumento "],[" aumento ","desabastecimiento"],["desabastecimiento","masivo"],["masivo","desabastecimiento"],["desabastecimiento","reduccion "],["reduccion ","desabastecimiento"],["desabastecimiento","reducidas"],["reducidas","desabastecimiento"],["desabastecimiento","mayor "],["mayor ","desabastecimiento"],["desabastecimiento"," menor"],[" menor","desabastecimiento"],["desabastecimiento","grave "],["grave ","desabastecimiento"],["desabastecimiento"," agudo"],[" agudo","desabastecimiento"],["desabastecimiento","bajo "],["bajo ","desabastecimiento"],["desabastecimiento","alto"],["alto","desabastecimiento"],["desabastecimiento","intensa "],["intensa ","desabastecimiento"],["desabastecimiento"," extrema"],[" extrema","desabastecimiento"],["desabastecimiento","moderada "],["moderada ","desabastecimiento"],["desabastecimiento","mermado"],["mermado","desabastecimiento"],["desabastecimiento","severa "],["severa ","desabastecimiento"],["desabastecimiento"," leve"],[" leve","desabastecimiento"],["desabastecimiento","magnitud"],["magnitud","desabastecimiento"],["desabastecimiento","emergencia"],["emergencia","desabastecimiento"],["desabastecimiento","debajo del promedio "],["debajo del promedio ","desabastecimiento"],["desabastecimiento"," encima del promedio"],[" encima del promedio","desabastecimiento"],["desabastecimiento","severo "],["severo ","desabastecimiento"],["desabastecimiento"," severa"],[" severa","desabastecimiento"],["desabastecimiento","significativamente"],["significativamente","desabastecimiento"],["desabastecimiento","inusual"],["inusual","desabastecimiento"],["desabastecimiento","gravedad"],["gravedad","desabastecimiento"],["desabastecimiento","irregularidad"],["irregularidad","desabastecimiento"],["desabastecimiento","inadecuado"],["inadecuado","desabastecimiento"],["desabastecimiento","caido"],["caido","desabastecimiento"],["racionamiento ","dificil "],["dificil ","racionamiento "],["racionamiento "," disminucion"],[" disminucion","racionamiento "],["racionamiento ","aumentar "],["aumentar ","racionamiento "],["racionamiento "," aumento "],[" aumento ","racionamiento "],["racionamiento ","masivo"],["masivo","racionamiento "],["racionamiento ","reduccion "],["reduccion ","racionamiento "],["racionamiento ","reducidas"],["reducidas","racionamiento "],["racionamiento ","mayor "],["mayor ","racionamiento "],["racionamiento "," menor"],[" menor","racionamiento "],["racionamiento ","grave "],["grave ","racionamiento "],["racionamiento "," agudo"],[" agudo","racionamiento "],["racionamiento ","bajo "],["bajo ","racionamiento "],["racionamiento ","alto"],["alto","racionamiento "],["racionamiento ","intensa "],["intensa ","racionamiento "],["racionamiento "," extrema"],[" extrema","racionamiento "],["racionamiento ","moderada "],["moderada ","racionamiento "],["racionamiento ","mermado"],["mermado","racionamiento "],["racionamiento ","severa "],["severa ","racionamiento "],["racionamiento "," leve"],[" leve","racionamiento "],["racionamiento ","magnitud"],["magnitud","racionamiento "],["racionamiento ","emergencia"],["emergencia","racionamiento "],["racionamiento ","debajo del promedio "],["debajo del promedio ","racionamiento "],["racionamiento "," encima del promedio"],[" encima del promedio","racionamiento "],["racionamiento ","severo "],["severo ","racionamiento "],["racionamiento "," severa"],[" severa","racionamiento "],["racionamiento ","significativamente"],["significativamente","racionamiento "],["racionamiento ","inusual"],["inusual","racionamiento "],["racionamiento ","gravedad"],["gravedad","racionamiento "],["racionamiento ","irregularidad"],["irregularidad","racionamiento "],["racionamiento ","inadecuado"],["inadecuado","racionamiento "],["racionamiento ","caido"],["caido","racionamiento "],["ahorro","dificil "],["dificil ","ahorro"],["ahorro"," disminucion"],[" disminucion","ahorro"],["ahorro","aumentar "],["aumentar ","ahorro"],["ahorro"," aumento "],[" aumento ","ahorro"],["ahorro","masivo"],["masivo","ahorro"],["ahorro","reduccion "],["reduccion ","ahorro"],["ahorro","reducidas"],["reducidas","ahorro"],["ahorro","mayor "],["mayor ","ahorro"],["ahorro"," menor"],[" menor","ahorro"],["ahorro","grave "],["grave ","ahorro"],["ahorro"," agudo"],[" agudo","ahorro"],["ahorro","bajo "],["bajo ","ahorro"],["ahorro","alto"],["alto","ahorro"],["ahorro","intensa "],["intensa ","ahorro"],["ahorro"," extrema"],[" extrema","ahorro"],["ahorro","moderada "],["moderada ","ahorro"],["ahorro","mermado"],["mermado","ahorro"],["ahorro","severa "],["severa ","ahorro"],["ahorro"," leve"],[" leve","ahorro"],["ahorro","magnitud"],["magnitud","ahorro"],["ahorro","emergencia"],["emergencia","ahorro"],["ahorro","debajo del promedio "],["debajo del promedio ","ahorro"],["ahorro"," encima del promedio"],[" encima del promedio","ahorro"],["ahorro","severo "],["severo ","ahorro"],["ahorro"," severa"],[" severa","ahorro"],["ahorro","significativamente"],["significativamente","ahorro"],["ahorro","inusual"],["inusual","ahorro"],["ahorro","gravedad"],["gravedad","ahorro"],["ahorro","irregularidad"],["irregularidad","ahorro"],["ahorro","inadecuado"],["inadecuado","ahorro"],["ahorro","caido"],["caido","ahorro"],["almacenamiento","dificil "],["dificil ","almacenamiento"],["almacenamiento"," disminucion"],[" disminucion","almacenamiento"],["almacenamiento","aumentar "],["aumentar ","almacenamiento"],["almacenamiento"," aumento "],[" aumento ","almacenamiento"],["almacenamiento","masivo"],["masivo","almacenamiento"],["almacenamiento","reduccion "],["reduccion ","almacenamiento"],["almacenamiento","reducidas"],["reducidas","almacenamiento"],["almacenamiento","mayor "],["mayor ","almacenamiento"],["almacenamiento"," menor"],[" menor","almacenamiento"],["almacenamiento","grave "],["grave ","almacenamiento"],["almacenamiento"," agudo"],[" agudo","almacenamiento"],["almacenamiento","bajo "],["bajo ","almacenamiento"],["almacenamiento","alto"],["alto","almacenamiento"],["almacenamiento","intensa "],["intensa ","almacenamiento"],["almacenamiento"," extrema"],[" extrema","almacenamiento"],["almacenamiento","moderada "],["moderada ","almacenamiento"],["almacenamiento","mermado"],["mermado","almacenamiento"],["almacenamiento","severa "],["severa ","almacenamiento"],["almacenamiento"," leve"],[" leve","almacenamiento"],["almacenamiento","magnitud"],["magnitud","almacenamiento"],["almacenamiento","emergencia"],["emergencia","almacenamiento"],["almacenamiento","debajo del promedio "],["debajo del promedio ","almacenamiento"],["almacenamiento"," encima del promedio"],[" encima del promedio","almacenamiento"],["almacenamiento","severo "],["severo ","almacenamiento"],["almacenamiento"," severa"],[" severa","almacenamiento"],["almacenamiento","significativamente"],["significativamente","almacenamiento"],["almacenamiento","inusual"],["inusual","almacenamiento"],["almacenamiento","gravedad"],["gravedad","almacenamiento"],["almacenamiento","irregularidad"],["irregularidad","almacenamiento"],["almacenamiento","inadecuado"],["inadecuado","almacenamiento"],["almacenamiento","caido"],["caido","almacenamiento"],["aprovisionamiento","dificil "],["dificil ","aprovisionamiento"],["aprovisionamiento"," disminucion"],[" disminucion","aprovisionamiento"],["aprovisionamiento","aumentar "],["aumentar ","aprovisionamiento"],["aprovisionamiento"," aumento "],[" aumento ","aprovisionamiento"],["aprovisionamiento","masivo"],["masivo","aprovisionamiento"],["aprovisionamiento","reduccion "],["reduccion ","aprovisionamiento"],["aprovisionamiento","reducidas"],["reducidas","aprovisionamiento"],["aprovisionamiento","mayor "],["mayor ","aprovisionamiento"],["aprovisionamiento"," menor"],[" menor","aprovisionamiento"],["aprovisionamiento","grave "],["grave ","aprovisionamiento"],["aprovisionamiento"," agudo"],[" agudo","aprovisionamiento"],["aprovisionamiento","bajo "],["bajo ","aprovisionamiento"],["aprovisionamiento","alto"],["alto","aprovisionamiento"],["aprovisionamiento","intensa "],["intensa ","aprovisionamiento"],["aprovisionamiento"," extrema"],[" extrema","aprovisionamiento"],["aprovisionamiento","moderada "],["moderada ","aprovisionamiento"],["aprovisionamiento","mermado"],["mermado","aprovisionamiento"],["aprovisionamiento","severa "],["severa ","aprovisionamiento"],["aprovisionamiento"," leve"],[" leve","aprovisionamiento"],["aprovisionamiento","magnitud"],["magnitud","aprovisionamiento"],["aprovisionamiento","emergencia"],["emergencia","aprovisionamiento"],["aprovisionamiento","debajo del promedio "],["debajo del promedio ","aprovisionamiento"],["aprovisionamiento"," encima del promedio"],[" encima del promedio","aprovisionamiento"],["aprovisionamiento","severo "],["severo ","aprovisionamiento"],["aprovisionamiento"," severa"],[" severa","aprovisionamiento"],["aprovisionamiento","significativamente"],["significativamente","aprovisionamiento"],["aprovisionamiento","inusual"],["inusual","aprovisionamiento"],["aprovisionamiento","gravedad"],["gravedad","aprovisionamiento"],["aprovisionamiento","irregularidad"],["irregularidad","aprovisionamiento"],["aprovisionamiento","inadecuado"],["inadecuado","aprovisionamiento"],["aprovisionamiento","caido"],["caido","aprovisionamiento"],["promedio","dificil "],["dificil ","promedio"],["promedio"," disminucion"],[" disminucion","promedio"],["promedio","aumentar "],["aumentar ","promedio"],["promedio"," aumento "],[" aumento ","promedio"],["promedio","masivo"],["masivo","promedio"],["promedio","reduccion "],["reduccion ","promedio"],["promedio","reducidas"],["reducidas","promedio"],["promedio","mayor "],["mayor ","promedio"],["promedio"," menor"],[" menor","promedio"],["promedio","grave "],["grave ","promedio"],["promedio"," agudo"],[" agudo","promedio"],["promedio","bajo "],["bajo ","promedio"],["promedio","alto"],["alto","promedio"],["promedio","intensa "],["intensa ","promedio"],["promedio"," extrema"],[" extrema","promedio"],["promedio","moderada "],["moderada ","promedio"],["promedio","mermado"],["mermado","promedio"],["promedio","severa "],["severa ","promedio"],["promedio"," leve"],[" leve","promedio"],["promedio","magnitud"],["magnitud","promedio"],["promedio","emergencia"],["emergencia","promedio"],["promedio","debajo del promedio "],["debajo del promedio ","promedio"],["promedio"," encima del promedio"],[" encima del promedio","promedio"],["promedio","severo "],["severo ","promedio"],["promedio"," severa"],[" severa","promedio"],["promedio","significativamente"],["significativamente","promedio"],["promedio","inusual"],["inusual","promedio"],["promedio","gravedad"],["gravedad","promedio"],["promedio","irregularidad"],["irregularidad","promedio"],["promedio","inadecuado"],["inadecuado","promedio"],["promedio","caido"],["caido","promedio"],["desviacion","dificil "],["dificil ","desviacion"],["desviacion"," disminucion"],[" disminucion","desviacion"],["desviacion","aumentar "],["aumentar ","desviacion"],["desviacion"," aumento "],[" aumento ","desviacion"],["desviacion","masivo"],["masivo","desviacion"],["desviacion","reduccion "],["reduccion ","desviacion"],["desviacion","reducidas"],["reducidas","desviacion"],["desviacion","mayor "],["mayor ","desviacion"],["desviacion"," menor"],[" menor","desviacion"],["desviacion","grave "],["grave ","desviacion"],["desviacion"," agudo"],[" agudo","desviacion"],["desviacion","bajo "],["bajo ","desviacion"],["desviacion","alto"],["alto","desviacion"],["desviacion","intensa "],["intensa ","desviacion"],["desviacion"," extrema"],[" extrema","desviacion"],["desviacion","moderada "],["moderada ","desviacion"],["desviacion","mermado"],["mermado","desviacion"],["desviacion","severa "],["severa ","desviacion"],["desviacion"," leve"],[" leve","desviacion"],["desviacion","magnitud"],["magnitud","desviacion"],["desviacion","emergencia"],["emergencia","desviacion"],["desviacion","debajo del promedio "],["debajo del promedio ","desviacion"],["desviacion"," encima del promedio"],[" encima del promedio","desviacion"],["desviacion","severo "],["severo ","desviacion"],["desviacion"," severa"],[" severa","desviacion"],["desviacion","significativamente"],["significativamente","desviacion"],["desviacion","inusual"],["inusual","desviacion"],["desviacion","gravedad"],["gravedad","desviacion"],["desviacion","irregularidad"],["irregularidad","desviacion"],["desviacion","inadecuado"],["inadecuado","desviacion"],["desviacion","caido"],["caido","desviacion"],["variacion","dificil "],["dificil ","variacion"],["variacion"," disminucion"],[" disminucion","variacion"],["variacion","aumentar "],["aumentar ","variacion"],["variacion"," aumento "],[" aumento ","variacion"],["variacion","masivo"],["masivo","variacion"],["variacion","reduccion "],["reduccion ","variacion"],["variacion","reducidas"],["reducidas","variacion"],["variacion","mayor "],["mayor ","variacion"],["variacion"," menor"],[" menor","variacion"],["variacion","grave "],["grave ","variacion"],["variacion"," agudo"],[" agudo","variacion"],["variacion","bajo "],["bajo ","variacion"],["variacion","alto"],["alto","variacion"],["variacion","intensa "],["intensa ","variacion"],["variacion"," extrema"],[" extrema","variacion"],["variacion","moderada "],["moderada ","variacion"],["variacion","mermado"],["mermado","variacion"],["variacion","severa "],["severa ","variacion"],["variacion"," leve"],[" leve","variacion"],["variacion","magnitud"],["magnitud","variacion"],["variacion","emergencia"],["emergencia","variacion"],["variacion","debajo del promedio "],["debajo del promedio ","variacion"],["variacion"," encima del promedio"],[" encima del promedio","variacion"],["variacion","severo "],["severo ","variacion"],["variacion"," severa"],[" severa","variacion"],["variacion","significativamente"],["significativamente","variacion"],["variacion","inusual"],["inusual","variacion"],["variacion","gravedad"],["gravedad","variacion"],["variacion","irregularidad"],["irregularidad","variacion"],["variacion","inadecuado"],["inadecuado","variacion"],["variacion","caido"],["caido","variacion"],["carencia","dificil "],["dificil ","carencia"],["carencia"," disminucion"],[" disminucion","carencia"],["carencia","aumentar "],["aumentar ","carencia"],["carencia"," aumento "],[" aumento ","carencia"],["carencia","masivo"],["masivo","carencia"],["carencia","reduccion "],["reduccion ","carencia"],["carencia","reducidas"],["reducidas","carencia"],["carencia","mayor "],["mayor ","carencia"],["carencia"," menor"],[" menor","carencia"],["carencia","grave "],["grave ","carencia"],["carencia"," agudo"],[" agudo","carencia"],["carencia","bajo "],["bajo ","carencia"],["carencia","alto"],["alto","carencia"],["carencia","intensa "],["intensa ","carencia"],["carencia"," extrema"],[" extrema","carencia"],["carencia","moderada "],["moderada ","carencia"],["carencia","mermado"],["mermado","carencia"],["carencia","severa "],["severa ","carencia"],["carencia"," leve"],[" leve","carencia"],["carencia","magnitud"],["magnitud","carencia"],["carencia","emergencia"],["emergencia","carencia"],["carencia","debajo del promedio "],["debajo del promedio ","carencia"],["carencia"," encima del promedio"],[" encima del promedio","carencia"],["carencia","severo "],["severo ","carencia"],["carencia"," severa"],[" severa","carencia"],["carencia","significativamente"],["significativamente","carencia"],["carencia","inusual"],["inusual","carencia"],["carencia","gravedad"],["gravedad","carencia"],["carencia","irregularidad"],["irregularidad","carencia"],["carencia","inadecuado"],["inadecuado","carencia"],["carencia","caido"],["caido","carencia"],["suministro","dificil "],["dificil ","suministro"],["suministro"," disminucion"],[" disminucion","suministro"],["suministro","aumentar "],["aumentar ","suministro"],["suministro"," aumento "],[" aumento ","suministro"],["suministro","masivo"],["masivo","suministro"],["suministro","reduccion "],["reduccion ","suministro"],["suministro","reducidas"],["reducidas","suministro"],["suministro","mayor "],["mayor ","suministro"],["suministro"," menor"],[" menor","suministro"],["suministro","grave "],["grave ","suministro"],["suministro"," agudo"],[" agudo","suministro"],["suministro","bajo "],["bajo ","suministro"],["suministro","alto"],["alto","suministro"],["suministro","intensa "],["intensa ","suministro"],["suministro"," extrema"],[" extrema","suministro"],["suministro","moderada "],["moderada ","suministro"],["suministro","mermado"],["mermado","suministro"],["suministro","severa "],["severa ","suministro"],["suministro"," leve"],[" leve","suministro"],["suministro","magnitud"],["magnitud","suministro"],["suministro","emergencia"],["emergencia","suministro"],["suministro","debajo del promedio "],["debajo del promedio ","suministro"],["suministro"," encima del promedio"],[" encima del promedio","suministro"],["suministro","severo "],["severo ","suministro"],["suministro"," severa"],[" severa","suministro"],["suministro","significativamente"],["significativamente","suministro"],["suministro","inusual"],["inusual","suministro"],["suministro","gravedad"],["gravedad","suministro"],["suministro","irregularidad"],["irregularidad","suministro"],["suministro","inadecuado"],["inadecuado","suministro"],["suministro","caido"],["caido","suministro"],["disponibilidad","dificil "],["dificil ","disponibilidad"],["disponibilidad"," disminucion"],[" disminucion","disponibilidad"],["disponibilidad","aumentar "],["aumentar ","disponibilidad"],["disponibilidad"," aumento "],[" aumento ","disponibilidad"],["disponibilidad","masivo"],["masivo","disponibilidad"],["disponibilidad","reduccion "],["reduccion ","disponibilidad"],["disponibilidad","reducidas"],["reducidas","disponibilidad"],["disponibilidad","mayor "],["mayor ","disponibilidad"],["disponibilidad"," menor"],[" menor","disponibilidad"],["disponibilidad","grave "],["grave ","disponibilidad"],["disponibilidad"," agudo"],[" agudo","disponibilidad"],["disponibilidad","bajo "],["bajo ","disponibilidad"],["disponibilidad","alto"],["alto","disponibilidad"],["disponibilidad","intensa "],["intensa ","disponibilidad"],["disponibilidad"," extrema"],[" extrema","disponibilidad"],["disponibilidad","moderada "],["moderada ","disponibilidad"],["disponibilidad","mermado"],["mermado","disponibilidad"],["disponibilidad","severa "],["severa ","disponibilidad"],["disponibilidad"," leve"],[" leve","disponibilidad"],["disponibilidad","magnitud"],["magnitud","disponibilidad"],["disponibilidad","emergencia"],["emergencia","disponibilidad"],["disponibilidad","debajo del promedio "],["debajo del promedio ","disponibilidad"],["disponibilidad"," encima del promedio"],[" encima del promedio","disponibilidad"],["disponibilidad","severo "],["severo ","disponibilidad"],["disponibilidad"," severa"],[" severa","disponibilidad"],["disponibilidad","significativamente"],["significativamente","disponibilidad"],["disponibilidad","inusual"],["inusual","disponibilidad"],["disponibilidad","gravedad"],["gravedad","disponibilidad"],["disponibilidad","irregularidad"],["irregularidad","disponibilidad"],["disponibilidad","inadecuado"],["inadecuado","disponibilidad"],["disponibilidad","caido"],["caido","disponibilidad"],["energia","dificil "],["dificil ","energia"],["energia"," disminucion"],[" disminucion","energia"],["energia","aumentar "],["aumentar ","energia"],["energia"," aumento "],[" aumento ","energia"],["energia","masivo"],["masivo","energia"],["energia","reduccion "],["reduccion ","energia"],["energia","reducidas"],["reducidas","energia"],["energia","mayor "],["mayor ","energia"],["energia"," menor"],[" menor","energia"],["energia","grave "],["grave ","energia"],["energia"," agudo"],[" agudo","energia"],["energia","bajo "],["bajo ","energia"],["energia","alto"],["alto","energia"],["energia","intensa "],["intensa ","energia"],["energia"," extrema"],[" extrema","energia"],["energia","moderada "],["moderada ","energia"],["energia","mermado"],["mermado","energia"],["energia","severa "],["severa ","energia"],["energia"," leve"],[" leve","energia"],["energia","magnitud"],["magnitud","energia"],["energia","emergencia"],["emergencia","energia"],["energia","debajo del promedio "],["debajo del promedio ","energia"],["energia"," encima del promedio"],[" encima del promedio","energia"],["energia","severo "],["severo ","energia"],["energia"," severa"],[" severa","energia"],["energia","significativamente"],["significativamente","energia"],["energia","inusual"],["inusual","energia"],["energia","gravedad"],["gravedad","energia"],["energia","irregularidad"],["irregularidad","energia"],["energia","inadecuado"],["inadecuado","energia"],["energia","caido"],["caido","energia"]]</t>
@@ -448,7 +448,7 @@
     <t>aumentar / Aumento /masivo</t>
   </si>
   <si>
-    <t>[{"title":"Pilas: habrá masivo corte de luz en Cúcuta este domingo 15 y lunes ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...luz.../202333/"},{"title":"La Opinión, Cúcuta","displayLink":"www.laopinion.com.co","formattedUrl":"https://www.laopinion.com.co/"},{"title":"The collective despair of Venezuelans passing through Cúcuta ...","displayLink":"www.dejusticia.org","formattedUrl":"https://www.dejusticia.org/.../the-collective-despair-of-venezuelans-passing-..."},{"title":"Los desgarradores testimonios de familias divididas entre Colombia ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/.../150826_colombia_testimonios_familias_divididas..."},{"title":"The Yukpas: The Indigenous community who migrated to Colombia ...","displayLink":"www.dejusticia.org","formattedUrl":"https://www.dejusticia.org/.../the-yukpas-the-indigenous-community-who-..."},{"title":"Duque llega a Cúcuta para acompañar concierto y la entrega de ...","displayLink":"www.elpais.com.co","formattedUrl":"https://www.elpais.com.co/.../duque-llega-a-cucuta-para-acompanar-concier..."},{"title":"¿Quién es El Niño Guerrero de Cúcuta? A alias “El Saúl” lo ...","displayLink":"www.eluniverso.com","formattedUrl":"https://www.eluniverso.com/.../a-alias-el-saul-lo-llaman-el-nino-guerrero-de..."},{"title":"In Memoriam: Healthcare Workers Who Have Died of COVID-19","displayLink":"www.medscape.com","formattedUrl":"https://www.medscape.com/viewarticle/927976"},{"title":"Gasolina más barata del mundo desata contrabando andino | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-venezuela-colombia-contrab-idL..."},{"title":"Corte avala la extradición de alias Ciro, condenado por atentado en ...","displayLink":"www.eltiempo.com","formattedUrl":"https://www.eltiempo.com/.../cortes/corte-avala-la-extradicion-de-alias-ciro-..."}]</t>
+    <t>[{"title":"Somatic Mutations in TP53 Gene in Colombian Patients With Non ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8962838/"},{"title":"Venezuela I situation: ICC Appeals Chamber to hold hearing on ...","displayLink":"www.icc-cpi.int","formattedUrl":"https://www.icc-cpi.int/.../venezuela-i-situation-icc-appeals-chamber-hold-h..."},{"title":"Nine Indicted on Federal Drug Trafficking Conspiracy — FBI","displayLink":"www.fbi.gov","formattedUrl":"https://www.fbi.gov/.../nine-indicted-on-federal-drug-trafficking-conspirac..."},{"title":"3billion Announced the Winners of the 2nd End the Diagnostic ...","displayLink":"3billion.io","formattedUrl":"https://3billion.io/.../3billion-announced-the-winners-of-the-second-end-the..."},{"title":"World Health Organization (WHO) on X: \"Preliminary investigations ...","displayLink":"twitter.com","formattedUrl":"https://twitter.com/WHO/status/1217043229427761152"},{"title":"Sex differences in LDL-C control in a primary care population: The ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/37302923/"},{"title":"Binational Study of Water Desalination Opportunities in the Sea of ...","displayLink":"library.cap-az.com","formattedUrl":"https://library.cap-az.com/.../Binational-Desal-Study-Executive-Summary.p..."},{"title":"Phoenix Police Department Open Missing Person Cases","displayLink":"www.phoenix.gov","formattedUrl":"https://www.phoenix.gov/police/investigations/cold-case/.../opencases"},{"title":"Photos and Videos from \"Ayotzinapa Investigations\" Special Exhibit ...","displayLink":"nsarchive.gwu.edu","formattedUrl":"https://nsarchive.gwu.edu/photos-and-videos-ayotzinapa-investigations-spe..."},{"title":"ICE | U.S. Immigration and Customs Enforcement","displayLink":"www.ice.gov","formattedUrl":"https://www.ice.gov/"}]</t>
   </si>
   <si>
     <t>Costos</t>
@@ -457,7 +457,7 @@
     <t>Pobreza energética</t>
   </si>
   <si>
-    <t>[{"title":"Apple (América Latina)","displayLink":"www.apple.com","formattedUrl":"https://www.apple.com/la/"},{"title":"Latin Billboards: Juanes interpretó nueva canción | Miami.com ...","displayLink":"www.miamiherald.com","formattedUrl":"https://www.miamiherald.com/miami-com/en.../article225837495.html"},{"title":"Portal Ecopetrol","displayLink":"www.ecopetrol.com.co","formattedUrl":"https://www.ecopetrol.com.co/wps/portal/"},{"title":"Grupos militantes están reclutando menores migrantes no ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../europa-migrantes-extremistas-idLTAKBN15L2I..."},{"title":"EL PAÍS Edición América: el periódico global","displayLink":"elpais.com","formattedUrl":"https://elpais.com/america/"},{"title":"China aportará 2,000 mln dlr a fondo BID para proyectos ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../latinoamerica-finanzas-bid-china-idLTASIE92F..."},{"title":"Qué necesita Colombia para hacer realidad su plan de abandonar ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/vert-fut-63816391"},{"title":"Agenda de Grupos de Trabajo - Julio 2023 - CLACSO","displayLink":"www.clacso.org","formattedUrl":"https://www.clacso.org/en/agenda-de-grupos-de-trabajo-julio-2023/"},{"title":"ENERGÉTICO SUSTENTABLE","displayLink":"www.interacademies.org","formattedUrl":"https://www.interacademies.org/.../guide_toward_a_sustainable_future_for_..."},{"title":"DIAGNOSIS OF WATER IN THE AMERICAS","displayLink":"ianas.org","formattedUrl":"https://ianas.org/wp-content/uploads/2020/07/08-Diagnosis-of-water.pdf"}]</t>
+    <t>[{"title":"Buildings | Free Full-Text | Energy Poverty Evaluation Using a Three ...","displayLink":"www.mdpi.com","formattedUrl":"https://www.mdpi.com/2075-5309/12/8/1125"},{"title":"Understanding, recognizing, and sharing energy poverty knowledge ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/pii/S2214629621005624"},{"title":"Does energy poverty have a female face in Chile?: Tapuya: Latin ...","displayLink":"www.tandfonline.com","formattedUrl":"https://www.tandfonline.com/doi/abs/10.1080/25729861.2019.1608038"},{"title":"Impact of energy literacy on vulnerable families: Case study – The ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/abs/pii/S0301421523002355"},{"title":"Feminización de la pobreza energética en Madrid. Exposición a ...","displayLink":"oa.upm.es","formattedUrl":"https://oa.upm.es/66337/1/FEMENMAD_vONLINE_compressed.pdf"},{"title":"Capturing Multidimensional Energy Poverty in South ... - Frontiers","displayLink":"www.frontiersin.org","formattedUrl":"https://www.frontiersin.org/articles/10.3389/frsc.2021.632009"},{"title":"Energy poverty effects on policy-based PM2.5 emissions mitigation ...","displayLink":"pobrezaenergetica.cl","formattedUrl":"https://pobrezaenergetica.cl/wp-content/.../01/Energy-poverty-effects.pdf"},{"title":"(PDF) Policy Paper: Pobreza Energética. El acceso desigual a ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../339096413_Policy_Paper_Pobreza_Energe..."},{"title":"Gender perspective on access to energy in the EU | European ...","displayLink":"www.europarl.europa.eu","formattedUrl":"https://www.europarl.europa.eu/.../IPOL_STU(2017)596816_EN.pdf"},{"title":"Pobreza energética en el Uruguay: diagnóstico de brechas en el ...","displayLink":"www.gub.uy","formattedUrl":"https://www.gub.uy/agencia-uruguaya.../sites/.../S2201294_es.pdf"}]</t>
   </si>
   <si>
     <t>Seguridad alimentaria</t>
@@ -589,7 +589,7 @@
     <t>Riesgo</t>
   </si>
   <si>
-    <t>[{"title":"Risk of dengue, Zika, and chikungunya transmission in the ...","displayLink":"bmcpublichealth.biomedcentral.com","formattedUrl":"https://bmcpublichealth.biomedcentral.com/articles/10.../s12889-023-1589..."},{"title":"Travel advice and advisories for Colombia","displayLink":"travel.gc.ca","formattedUrl":"https://travel.gc.ca/destinations/colombia"},{"title":"Spatio-temporal clusters and patterns of spread of dengue ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9439233/"},{"title":"Influenza, SARS-CoV-2, RSV and other respiratory viruses situation ...","displayLink":"www.paho.org","formattedUrl":"https://www.paho.org/en/influenza-situation-report"},{"title":"'Nobody Is Immune': Bracing For Zika's First Summer In The U.S. ...","displayLink":"www.npr.org","formattedUrl":"https://www.npr.org/.../nobody-is-immune-bracing-for-zikas-first-summer-i..."},{"title":"Projections: Zika Could Infect More Than 93 Million in Americas","displayLink":"www.voanews.com","formattedUrl":"https://www.voanews.com/a/projections-show-zika.../3434386.html"},{"title":"Zika virus shadows a maternity ward in Colombia","displayLink":"www.statnews.com","formattedUrl":"https://www.statnews.com/2016/02/06/zika-colombia-pregnant-women/"},{"title":"Zika virus: more than 5,000 pregnant women infected in Colombia ...","displayLink":"www.theguardian.com","formattedUrl":"https://www.theguardian.com/.../zika-virus-more-than-5000-pregnant-wom..."},{"title":"How my assumptions about Zika got turned upside down","displayLink":"www.statnews.com","formattedUrl":"https://www.statnews.com/2016/02/16/colombia-zika-reporters-notebook/"},{"title":"Armed with tech tools, Colombian cities combat mosquito-borne ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../armed-with-tech-tools-colombian-cities-combat-..."}]</t>
+    <t>[{"title":"Chikungunya fact sheet","displayLink":"www.who.int","formattedUrl":"https://www.who.int/news-room/fact-sheets/detail/chikungunya"},{"title":"Epidemiological and genomic investigation of chikungunya virus in ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/37769008/"},{"title":"Diagnostic Testing | Chikungunya virus | CDC","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/chikungunya/hc/diagnostic.html"},{"title":"Chikungunya fever: a clinical and virological investigation of ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/23350006/"},{"title":"NIAID-Sponsored Trial of Experimental Chikungunya Vaccine ...","displayLink":"www.nih.gov","formattedUrl":"https://www.nih.gov/.../niaid-sponsored-trial-experimental-chikungunya-va..."},{"title":"Spatiotemporal dynamics and recurrence of chikungunya virus in ...","displayLink":"www.thelancet.com","formattedUrl":"https://www.thelancet.com/journals/lanmic/article/PIIS2666...2/fulltext"},{"title":"Experimental Chikungunya Vaccine is Safe and Well-Tolerated in ...","displayLink":"www.niaid.nih.gov","formattedUrl":"https://www.niaid.nih.gov/.../experimental-chikungunya-vaccine-safe-and-..."},{"title":"Entomological Investigation and Control of a Chikungunya Cluster in ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3129687/"},{"title":"Epidemiological investigation of chikungunya outbreak, West ...","displayLink":"www.sciencedirect.com","formattedUrl":"https://www.sciencedirect.com/science/article/pii/S2213398419301435"},{"title":"Human and entomologic investigations of chikungunya outbreak in ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6181335/"}]</t>
   </si>
   <si>
     <t>[["plaga","riesgo"],["riesgo","plaga"],["plaga","aumento"],["aumento","plaga"],["plaga","incremento"],["incremento","plaga"],["plaga","incrementaria"],["incrementaria","plaga"],["plaga","incidencia"],["incidencia","plaga"],["plaga","grave"],["grave","plaga"],["plaga","agudo"],["agudo","plaga"],["plaga","aguda"],["aguda","plaga"],["plaga","inusual"],["inusual","plaga"],["plaga","amenaza"],["amenaza","plaga"],["plaga","muerte "],["muerte ","plaga"],["plaga"," muertes "],[" muertes ","plaga"],["plaga"," defunciones"],[" defunciones","plaga"],["plaga","colapsar"],["colapsar","plaga"],["plaga","inadecuado"],["inadecuado","plaga"],["plaga","incapacidad"],["incapacidad","plaga"],["epidemia","riesgo"],["riesgo","epidemia"],["epidemia","aumento"],["aumento","epidemia"],["epidemia","incremento"],["incremento","epidemia"],["epidemia","incrementaria"],["incrementaria","epidemia"],["epidemia","incidencia"],["incidencia","epidemia"],["epidemia","grave"],["grave","epidemia"],["epidemia","agudo"],["agudo","epidemia"],["epidemia","aguda"],["aguda","epidemia"],["epidemia","inusual"],["inusual","epidemia"],["epidemia","amenaza"],["amenaza","epidemia"],["epidemia","muerte "],["muerte ","epidemia"],["epidemia"," muertes "],[" muertes ","epidemia"],["epidemia"," defunciones"],[" defunciones","epidemia"],["epidemia","colapsar"],["colapsar","epidemia"],["epidemia","inadecuado"],["inadecuado","epidemia"],["epidemia","incapacidad"],["incapacidad","epidemia"],["virica","riesgo"],["riesgo","virica"],["virica","aumento"],["aumento","virica"],["virica","incremento"],["incremento","virica"],["virica","incrementaria"],["incrementaria","virica"],["virica","incidencia"],["incidencia","virica"],["virica","grave"],["grave","virica"],["virica","agudo"],["agudo","virica"],["virica","aguda"],["aguda","virica"],["virica","inusual"],["inusual","virica"],["virica","amenaza"],["amenaza","virica"],["virica","muerte "],["muerte ","virica"],["virica"," muertes "],[" muertes ","virica"],["virica"," defunciones"],[" defunciones","virica"],["virica","colapsar"],["colapsar","virica"],["virica","inadecuado"],["inadecuado","virica"],["virica","incapacidad"],["incapacidad","virica"],["virus","riesgo"],["riesgo","virus"],["virus","aumento"],["aumento","virus"],["virus","incremento"],["incremento","virus"],["virus","incrementaria"],["incrementaria","virus"],["virus","incidencia"],["incidencia","virus"],["virus","grave"],["grave","virus"],["virus","agudo"],["agudo","virus"],["virus","aguda"],["aguda","virus"],["virus","inusual"],["inusual","virus"],["virus","amenaza"],["amenaza","virus"],["virus","muerte "],["muerte ","virus"],["virus"," muertes "],[" muertes ","virus"],["virus"," defunciones"],[" defunciones","virus"],["virus","colapsar"],["colapsar","virus"],["virus","inadecuado"],["inadecuado","virus"],["virus","incapacidad"],["incapacidad","virus"],["picadura","riesgo"],["riesgo","picadura"],["picadura","aumento"],["aumento","picadura"],["picadura","incremento"],["incremento","picadura"],["picadura","incrementaria"],["incrementaria","picadura"],["picadura","incidencia"],["incidencia","picadura"],["picadura","grave"],["grave","picadura"],["picadura","agudo"],["agudo","picadura"],["picadura","aguda"],["aguda","picadura"],["picadura","inusual"],["inusual","picadura"],["picadura","amenaza"],["amenaza","picadura"],["picadura","muerte "],["muerte ","picadura"],["picadura"," muertes "],[" muertes ","picadura"],["picadura"," defunciones"],[" defunciones","picadura"],["picadura","colapsar"],["colapsar","picadura"],["picadura","inadecuado"],["inadecuado","picadura"],["picadura","incapacidad"],["incapacidad","picadura"],["transmitida","riesgo"],["riesgo","transmitida"],["transmitida","aumento"],["aumento","transmitida"],["transmitida","incremento"],["incremento","transmitida"],["transmitida","incrementaria"],["incrementaria","transmitida"],["transmitida","incidencia"],["incidencia","transmitida"],["transmitida","grave"],["grave","transmitida"],["transmitida","agudo"],["agudo","transmitida"],["transmitida","aguda"],["aguda","transmitida"],["transmitida","inusual"],["inusual","transmitida"],["transmitida","amenaza"],["amenaza","transmitida"],["transmitida","muerte "],["muerte ","transmitida"],["transmitida"," muertes "],[" muertes ","transmitida"],["transmitida"," defunciones"],[" defunciones","transmitida"],["transmitida","colapsar"],["colapsar","transmitida"],["transmitida","inadecuado"],["inadecuado","transmitida"],["transmitida","incapacidad"],["incapacidad","transmitida"],["transmision","riesgo"],["riesgo","transmision"],["transmision","aumento"],["aumento","transmision"],["transmision","incremento"],["incremento","transmision"],["transmision","incrementaria"],["incrementaria","transmision"],["transmision","incidencia"],["incidencia","transmision"],["transmision","grave"],["grave","transmision"],["transmision","agudo"],["agudo","transmision"],["transmision","aguda"],["aguda","transmision"],["transmision","inusual"],["inusual","transmision"],["transmision","amenaza"],["amenaza","transmision"],["transmision","muerte "],["muerte ","transmision"],["transmision"," muertes "],[" muertes ","transmision"],["transmision"," defunciones"],[" defunciones","transmision"],["transmision","colapsar"],["colapsar","transmision"],["transmision","inadecuado"],["inadecuado","transmision"],["transmision","incapacidad"],["incapacidad","transmision"],["brote","riesgo"],["riesgo","brote"],["brote","aumento"],["aumento","brote"],["brote","incremento"],["incremento","brote"],["brote","incrementaria"],["incrementaria","brote"],["brote","incidencia"],["incidencia","brote"],["brote","grave"],["grave","brote"],["brote","agudo"],["agudo","brote"],["brote","aguda"],["aguda","brote"],["brote","inusual"],["inusual","brote"],["brote","amenaza"],["amenaza","brote"],["brote","muerte "],["muerte ","brote"],["brote"," muertes "],[" muertes ","brote"],["brote"," defunciones"],[" defunciones","brote"],["brote","colapsar"],["colapsar","brote"],["brote","inadecuado"],["inadecuado","brote"],["brote","incapacidad"],["incapacidad","brote"],["proliferacion","riesgo"],["riesgo","proliferacion"],["proliferacion","aumento"],["aumento","proliferacion"],["proliferacion","incremento"],["incremento","proliferacion"],["proliferacion","incrementaria"],["incrementaria","proliferacion"],["proliferacion","incidencia"],["incidencia","proliferacion"],["proliferacion","grave"],["grave","proliferacion"],["proliferacion","agudo"],["agudo","proliferacion"],["proliferacion","aguda"],["aguda","proliferacion"],["proliferacion","inusual"],["inusual","proliferacion"],["proliferacion","amenaza"],["amenaza","proliferacion"],["proliferacion","muerte "],["muerte ","proliferacion"],["proliferacion"," muertes "],[" muertes ","proliferacion"],["proliferacion"," defunciones"],[" defunciones","proliferacion"],["proliferacion","colapsar"],["colapsar","proliferacion"],["proliferacion","inadecuado"],["inadecuado","proliferacion"],["proliferacion","incapacidad"],["incapacidad","proliferacion"],["prevalencia","riesgo"],["riesgo","prevalencia"],["prevalencia","aumento"],["aumento","prevalencia"],["prevalencia","incremento"],["incremento","prevalencia"],["prevalencia","incrementaria"],["incrementaria","prevalencia"],["prevalencia","incidencia"],["incidencia","prevalencia"],["prevalencia","grave"],["grave","prevalencia"],["prevalencia","agudo"],["agudo","prevalencia"],["prevalencia","aguda"],["aguda","prevalencia"],["prevalencia","inusual"],["inusual","prevalencia"],["prevalencia","amenaza"],["amenaza","prevalencia"],["prevalencia","muerte "],["muerte ","prevalencia"],["prevalencia"," muertes "],[" muertes ","prevalencia"],["prevalencia"," defunciones"],[" defunciones","prevalencia"],["prevalencia","colapsar"],["colapsar","prevalencia"],["prevalencia","inadecuado"],["inadecuado","prevalencia"],["prevalencia","incapacidad"],["incapacidad","prevalencia"]]</t>
@@ -607,7 +607,7 @@
     <t>aumento</t>
   </si>
   <si>
-    <t>[{"title":"Risk of dengue, Zika, and chikungunya transmission in the ...","displayLink":"bmcpublichealth.biomedcentral.com","formattedUrl":"https://bmcpublichealth.biomedcentral.com/articles/10.../s12889-023-1589..."},{"title":"Colombia border hospitals struggle with Venezuelan migrant influx ...","displayLink":"www.aljazeera.com","formattedUrl":"https://www.aljazeera.com/news/.../colombia-border-hospitals-struggle-with..."},{"title":"Kenya Health Officials Issue Alert Over Dengue Fever Outbreak","displayLink":"www.voanews.com","formattedUrl":"https://www.voanews.com/a/kenya-health...alert-dengue.../3843040.html"},{"title":"Colombia: Dengue Outbreak Emergency Plan of Action (EPoA ...","displayLink":"reliefweb.int","formattedUrl":"https://reliefweb.int/.../colombia-dengue-outbreak-emergency-plan-action-e..."},{"title":"New App Identifies Mosquitoes by Buzzing Sound","displayLink":"www.voanews.com","formattedUrl":"https://www.voanews.com/a/science-health_new-app.../6198441.html"},{"title":"Travel advice and advisories for Colombia","displayLink":"travel.gc.ca","formattedUrl":"https://travel.gc.ca/destinations/colombia"},{"title":"Our Work in Colombia | Project HOPE","displayLink":"www.projecthope.org","formattedUrl":"https://www.projecthope.org/country/colombia/"},{"title":"Laboratory Findings in Patients with Probable Dengue Diagnosis ...","displayLink":"www.mdpi.com","formattedUrl":"https://www.mdpi.com/1999-4915/13/7/1401"},{"title":"Armed with tech tools, Colombian cities combat mosquito-borne ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../armed-with-tech-tools-colombian-cities-combat-..."},{"title":"Association of dengue infection with anti-alpha-gal antibodies, IgM ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9614307/"}]</t>
+    <t>[{"title":"Diagnosis | Dengue | CDC","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/dengue/healthcare-providers/diagnosis.html"},{"title":"LABORATORY DIAGNOSIS AND DIAGNOSTIC TESTS - Dengue ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/books/NBK143156/"},{"title":"Epidemiological, Entomological, and Climatological Investigation of ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/36421969/"},{"title":"Dengue Fever Outbreak Investigation in Werder Town, Dollo Zone ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9741851/"},{"title":"Investigation of Dengue Infection in Asymptomatic Individuals during ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/36992451/"},{"title":"Genomic investigation of a dengue virus outbreak in Thiès, Senegal ...","displayLink":"www.nature.com","formattedUrl":"https://www.nature.com/articles/s41598-021-89070-1"},{"title":"Epidemiological and hematological investigation of dengue virus ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/35769047/"},{"title":"Dengue Case Investigation Form","displayLink":"www.dshs.texas.gov","formattedUrl":"https://www.dshs.texas.gov/.../Dengue-Case-Investigation-Form-0722-Filla..."},{"title":"Investigation Into an Outbreak of Dengue-like Illness in Pernambuco ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/27015222/"},{"title":"Dengue Outbreak Toolbox","displayLink":"www.who.int","formattedUrl":"https://www.who.int/emergencies/outbreak.../dengue-outbreak-toolbox"}]</t>
   </si>
   <si>
     <t>Género</t>
@@ -622,7 +622,7 @@
     <t>incremento</t>
   </si>
   <si>
-    <t>[{"title":"Colombia border hospitals struggle with Venezuelan migrant influx ...","displayLink":"www.aljazeera.com","formattedUrl":"https://www.aljazeera.com/news/.../colombia-border-hospitals-struggle-with..."},{"title":"New App Identifies Mosquitoes by Buzzing Sound","displayLink":"www.voanews.com","formattedUrl":"https://www.voanews.com/a/science-health_new-app.../6198441.html"},{"title":"Our Work in Colombia | Project HOPE","displayLink":"www.projecthope.org","formattedUrl":"https://www.projecthope.org/country/colombia/"},{"title":"Venezuela crisis: Facts, FAQs, and how to help | World Vision","displayLink":"www.worldvision.org","formattedUrl":"https://www.worldvision.org/disaster-relief-news.../venezuela-crisis-facts"},{"title":"Travel advice and advisories for Colombia","displayLink":"travel.gc.ca","formattedUrl":"https://travel.gc.ca/destinations/colombia"},{"title":"Venezuela: UN Should Lead Full-Scale Emergency Response ...","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/news/.../venezuela-un-should-lead-full-scale-emergenc..."},{"title":"Shaping the future through dialogue in Colombia - giz.de","displayLink":"www.giz.de","formattedUrl":"https://www.giz.de/en/ourservices/55910.html"},{"title":"Colombia | International Rescue Committee (IRC)","displayLink":"www.rescue.org","formattedUrl":"https://www.rescue.org/country/colombia"},{"title":"Hungry, sick and increasingly desperate, thousands of Venezuelans ...","displayLink":"www.latimes.com","formattedUrl":"https://www.latimes.com/.../la-fg-venezuela-colombia-20180513-story.html"},{"title":"Trading in Venezuela's pain: Border vendors do brisk business in ...","displayLink":"www.france24.com","formattedUrl":"https://www.france24.com/.../20190210-trading-venezuelas-pain-border-ve..."}]</t>
+    <t>[{"title":"Malaria - Diagnosis &amp; Treatment (United States) - Diagnosis ... - CDC","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/malaria/diagnosis_treatment/diagnosis.html"},{"title":"Malaria Case Investigation Form","displayLink":"www.dshs.texas.gov","formattedUrl":"https://www.dshs.texas.gov/.../Malaria-Case-Investigation-Form3-2022Filla..."},{"title":"Malaria case investigation with reactive focal testing and treatment ...","displayLink":"malariajournal.biomedcentral.com","formattedUrl":"https://malariajournal.biomedcentral.com/articles/10.../s12936-018-2587-8"},{"title":"Locally Acquired Mosquito-Transmitted Malaria: A Guide for ...","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/mmwr/preview/mmwrhtml/rr5513a1.htm"},{"title":"Malaria outbreak investigation and contracting factors in Simada ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6525450/"},{"title":"Correction: Molecular investigation of malaria-infected patients in ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/37254163/"},{"title":"A comparative study of epidemiological investigations of malaria ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5848391/"},{"title":"A Molecular Investigation of Malaria Infections From High ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/34925255/"},{"title":"Malaria - Diagnosis &amp; treatment - Mayo Clinic","displayLink":"www.mayoclinic.org","formattedUrl":"https://www.mayoclinic.org/diseases-conditions/malaria/.../drc-20351190"},{"title":"Malaria surveillance, outbreak investigation, response and its ...","displayLink":"www.nature.com","formattedUrl":"https://www.nature.com/articles/s41598-023-36918-3"}]</t>
   </si>
   <si>
     <t>zika</t>
@@ -634,7 +634,7 @@
     <t>incrementaría</t>
   </si>
   <si>
-    <t>[{"title":"'Nobody Is Immune': Bracing For Zika's First Summer In The U.S. ...","displayLink":"www.npr.org","formattedUrl":"https://www.npr.org/.../nobody-is-immune-bracing-for-zikas-first-summer-i..."},{"title":"Colombia: A nation concerned over Zika - BBC News","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/news/health-35552340"},{"title":"Zika virus shadows a maternity ward in Colombia","displayLink":"www.statnews.com","formattedUrl":"https://www.statnews.com/2016/02/06/zika-colombia-pregnant-women/"},{"title":"Zika virus: more than 5,000 pregnant women infected in Colombia ...","displayLink":"www.theguardian.com","formattedUrl":"https://www.theguardian.com/.../zika-virus-more-than-5000-pregnant-wom..."},{"title":"Risk of dengue, Zika, and chikungunya transmission in the ...","displayLink":"bmcpublichealth.biomedcentral.com","formattedUrl":"https://bmcpublichealth.biomedcentral.com/articles/10.../s12889-023-1589..."},{"title":"Zika Virus in Colombia Presents Complicated Choice About ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/.../zika-virus-in-colombia-presents-complicated-c..."},{"title":"New Evidence Supports Biological Link Between Zika Infection ...","displayLink":"www.hopkinsmedicine.org","formattedUrl":"https://www.hopkinsmedicine.org/News/.../new_evidence_supports_biologi..."},{"title":"Zika Virus - The New York Times","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/news-event/zika-virus"},{"title":"Projections: Zika Could Infect More Than 93 Million in Americas","displayLink":"www.voanews.com","formattedUrl":"https://www.voanews.com/a/projections-show-zika.../3434386.html"},{"title":"Doctors: Upsurge in paralysis condition accompanies Zika","displayLink":"www.fox5atlanta.com","formattedUrl":"https://www.fox5atlanta.com/news/doctors-upsurge-in-paralysis-condition-a..."}]</t>
+    <t>[{"title":"Epidemiologic Investigation Toolkit for Investigating Possible Local ...","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/zika/public.../epidemiologic-investigation-toolkit.html"},{"title":"Investigation of Zika virus methyl transferase inhibitors using steered ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/37325855/"},{"title":"Preliminary Findings from an Investigation of Zika Virus Infection in a ...","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/mmwr/volumes/65/wr/mm6536e4.htm"},{"title":"Zika virus","displayLink":"www.who.int","formattedUrl":"https://www.who.int/news-room/fact-sheets/detail/zika-virus"},{"title":"Congenital Zika virus syndrome in Brazil: a case series of the first ...","displayLink":"www.thelancet.com","formattedUrl":"https://www.thelancet.com/journals/lancet/article/PIIS0140...3/fulltext"},{"title":"NIH launches large study of pregnant women in areas affected by ...","displayLink":"www.nih.gov","formattedUrl":"https://www.nih.gov/.../nih-launches-large-study-pregnant-women-areas-aff..."},{"title":"Experimental Assessment of Zika Virus Mechanical Transmission by ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6723193/"},{"title":"Emergence of the Asian lineage of Zika virus in Angola: an outbreak ...","displayLink":"www.thelancet.com","formattedUrl":"https://www.thelancet.com/journals/laninf/article/PIIS1473...2/fulltext"},{"title":"Study to examine effects of Zika infection in Guatemalan infants and ...","displayLink":"www.nih.gov","formattedUrl":"https://www.nih.gov/.../study-examine-effects-zika-infection-guatemalan-in..."},{"title":"Zika Virus Vaccines | NIH: National Institute of Allergy and Infectious ...","displayLink":"www.niaid.nih.gov","formattedUrl":"https://www.niaid.nih.gov/diseases-conditions/zika-vaccines"}]</t>
   </si>
   <si>
     <t>enfermedades diarreicas infecciones respiratorias</t>
@@ -646,7 +646,7 @@
     <t>incidencia</t>
   </si>
   <si>
-    <t>[{"title":"Comportamiento epidemiológico de la enfermedad diarreica aguda ...","displayLink":"www.ins.gov.co","formattedUrl":"https://www.ins.gov.co/.../2022_Boletín_epidemiologico_semana_19.pdf"},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"La emergencia humanitaria en Venezuela: Se requiere una ...","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/es/.../04/.../se-requiere-una-respuesta-gran-escala-de"},{"title":"BOLETÍN EPIDEMIOLÓGICO DEL PERÚ","displayLink":"www.dge.gob.pe","formattedUrl":"https://www.dge.gob.pe/portal/docs/vigilancia/boletines/2018/52.pdf"},{"title":"Cerca de 2.000 millones de personas usan agua contaminada con ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-salud-agua-contaminacion-idLTA..."},{"title":"Análisis de Situación de Salud Norte de Santander 2022","displayLink":"ids.gov.co","formattedUrl":"https://ids.gov.co/.../ASIS_DEPARTAMENTAL_NORTE%20DE_SANTA..."},{"title":"Desigualdades en salud de la población migrante y refugiada ...","displayLink":"s3.amazonaws.com","formattedUrl":"https://s3.amazonaws.com/semanaruralvzla/carpeta.../OFDA_13Mayo.pdf"},{"title":"Conocimientos y prácticas sobre enfermedad diarreica aguda en ...","displayLink":"revistas.ufps.edu.co","formattedUrl":"https://revistas.ufps.edu.co/index.php/cienciaycuidado/article/view/2230"},{"title":"Boletín técnico","displayLink":"www.dane.gov.co","formattedUrl":"https://www.dane.gov.co/files/.../bol-EEVV-Defunciones-ITrim2023.pdf"},{"title":"Conocimientos y prácticas sobre enfermedad diarreica aguda en ...","displayLink":"revistas.ufps.edu.co","formattedUrl":"https://revistas.ufps.edu.co/index.php/cienciaycuidado/article/.../13130"}]</t>
+    <t>[{"title":"Burden of disease from inadequate water, sanitation and hygiene for ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6593152/"},{"title":"Enfermedades Diarréicas - American College of Gastroenterology","displayLink":"gi.org","formattedUrl":"https://gi.org/patients/recursos-en-espanol/enfermedades-diarreicas/"},{"title":"El lavado de las manos en la comunidad: Las manos limpias salvan ...","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/handwashing/esp/index.html"},{"title":"Life expectancy, death, and disability in Haiti, 1990- 2017: a ...","displayLink":"iris.paho.org","formattedUrl":"https://iris.paho.org/handle/10665.2/52938"},{"title":"Muéstreme los fundamentos científicos: ¿Por qué lavarse las manos ...","displayLink":"www.cdc.gov","formattedUrl":"https://www.cdc.gov/handwashing/esp/why-handwashing.html"},{"title":"Prevalencia de infecciones respiratorias y enfermedades diarreicas ...","displayLink":"pesquisa.bvsalud.org","formattedUrl":"https://pesquisa.bvsalud.org/portal/resource/pt/biblio-959734"},{"title":"Enfermedades diarreicas, infecciones respiratorias y características ...","displayLink":"www.scielo.org.pe","formattedUrl":"http://www.scielo.org.pe/scielo.php?script=sci_arttext&amp;pid=S1726..."},{"title":"Encuesta Nacional de Salud y Nutrición 2018. ENSANUT. Informe ...","displayLink":"www.inegi.org.mx","formattedUrl":"https://www.inegi.org.mx/.../2018/.../ensanut_2018_diseno_conceptual.pdf"},{"title":"Norma Oficial Mexicana NOM-031-SSA2-1999, Para la atención a la ...","displayLink":"www.cndh.org.mx","formattedUrl":"https://www.cndh.org.mx/DocTR/2016/JUR/.../JUR-20170331-NOR12.pdf"},{"title":"Life expectancy, death, and disability in Haiti, 1990-2017: a ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/33165413/"}]</t>
   </si>
   <si>
     <t>Enfermedades tropicales</t>
@@ -655,7 +655,7 @@
     <t>transmitida</t>
   </si>
   <si>
-    <t>[{"title":"Influenza, SARS-CoV-2, RSV and other respiratory viruses situation ...","displayLink":"www.paho.org","formattedUrl":"https://www.paho.org/en/influenza-situation-report"},{"title":"“28 días”, una campaña para mejorar la salud de los recién nacidos ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2022/02/1503432"},{"title":"Escasez de medicinas deja a Venezuela vulnerable ante zika | AP ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/article/d3a6b53b7a4c46cab1ecfabdf86203b5"},{"title":"Depresión tropical Harvey se debilita sobre México | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../portada-clima-harvey-idLTASIE7A76S620110..."},{"title":"El zika presenta un dilema en Colombia, donde el aborto es legal ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/es/2016/.../zika-dilema-colombia-aborto-legal.ht..."},{"title":"Molecular surveillance of resistance to pyrethroids insecticides in ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8735628/"},{"title":"Latin Billboards: Juanes interpretó nueva canción | Miami.com ...","displayLink":"www.miamiherald.com","formattedUrl":"https://www.miamiherald.com/miami-com/en.../article225837495.html"},{"title":"Venezuela: Las cifras evidencian una crisis de salud | Human ...","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/.../news/.../venezuela-las-cifras-evidencian-una-crisis-d..."},{"title":"ABC News fails to keep 'pink slime' lawsuit in federal court | ロイター","displayLink":"jp.reuters.com","formattedUrl":"https://jp.reuters.com/.../us-usa-media-abc-bpi-idUSBRE95C00J20130613"},{"title":"Estas son las plantas más venenosas del mundo - BBC News Mundo","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/.../150819_ciencia_vert_earth_plantas_venenosas_lv"}]</t>
+    <t>[{"title":"Tropical Disease Priority Review Voucher Program | FDA","displayLink":"www.fda.gov","formattedUrl":"https://www.fda.gov/.../tropical-disease-priority-review-voucher-program"},{"title":"Neuromuscular Effects of Common Krait (Bungarus caeruleus ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4734751/"},{"title":"A Digital Tool to Improve Patient Recruitment and Retention in ...","displayLink":"link.springer.com","formattedUrl":"https://link.springer.com/chapter/10.1007/978-3-030-47994-7_24"},{"title":"Reappraisal of Leishmanin Skin Test (LST) in the management of ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5645152/"},{"title":"Epidemiological investigations of diarrhea in children in Praia city ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/36619987/"},{"title":"Author Info | PLOS Neglected Tropical Diseases","displayLink":"journals.plos.org","formattedUrl":"https://journals.plos.org/plosntds/article/authors?id=10.1371/journal..."},{"title":"The Aotus nancymaae erythrocyte proteome and its importance for ...","displayLink":"pubmed.ncbi.nlm.nih.gov","formattedUrl":"https://pubmed.ncbi.nlm.nih.gov/27989940/"},{"title":"Author Info | PLOS Neglected Tropical Diseases","displayLink":"journals.plos.org","formattedUrl":"https://journals.plos.org/plosntds/article/authors?id=10.1371/journal..."},{"title":"Vector Research Laboratory | Centro de Investigación ...","displayLink":"ciet.ucr.ac.cr","formattedUrl":"http://ciet.ucr.ac.cr/en/lines-of-investigation/vector-research-laboratory"},{"title":"Prioritizing diseases for research and development in emergency ...","displayLink":"www.who.int","formattedUrl":"https://www.who.int/.../prioritizing-diseases-for-research-and-development-..."}]</t>
   </si>
   <si>
     <t>Calor</t>
@@ -667,7 +667,7 @@
     <t>agudo/aguda</t>
   </si>
   <si>
-    <t>[{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"Autoridades de salud en Cúcuta en alerta por fuerte oleada de calor ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../autoridades-de-salud-en-cucuta-en-alerta-por-..."},{"title":"Where to Go in Norte de Santander, Colombia | Moon Travel Guides","displayLink":"www.moon.com","formattedUrl":"https://www.moon.com/travel/.../where-to-go-norte-de-santander-colombia/"},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-63323077"},{"title":"Insoportable: así estará el intenso calor en Cúcuta este martes, 26 ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...calor-en.../202335/"},{"title":"ACTUALIZA 2-EEUU envía alimentos y medicinas a Colombia, en ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/venezuela-idARL1N20011P/"},{"title":"Qué calor: Así será la temperatura máxima en Cúcuta este jueves ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...calor.../202323/"},{"title":"Incendios forestales en Cúcuta por ola de calor - Otras Ciudades ...","displayLink":"www.eltiempo.com","formattedUrl":"https://www.eltiempo.com/.../incendios-forestales-en-cucuta-por-ola-de-cal..."},{"title":"Leonardo Peña Ocariz (@lasnoticiasdeleonardopena) • Instagram ...","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/lasnoticiasdeleonardopena/"},{"title":"Maternidad sin nacionalidad: así promueven la lactancia con ...","displayLink":"migravenezuela.com","formattedUrl":"https://migravenezuela.com/.../maternidad-sin-nacionalidad-asi-promueven-..."}]</t>
+    <t>[{"title":"Intermittent DMARC/SPF failures to MessageLabs hosted MX ...","displayLink":"community.broadcom.com","formattedUrl":"https://community.broadcom.com/...home/.../viewthread?..."},{"title":"Investigation of soft segments of thermoplastic polyurethane by NMR ...","displayLink":"www.itmc.rwth-aachen.de","formattedUrl":"https://www.itmc.rwth-aachen.de/cms/ITMC/Forschung/.../Details/?file..."},{"title":"Chemotherapy for isolated locoregional recurrence of breast cancer ...","displayLink":"europepmc.org","formattedUrl":"https://europepmc.org/article/med/24439313"},{"title":"Mastitis in the Lactating Mink Female (Mustela vison S.) and the ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7996420/"},{"title":"Revealed: hundreds of migrant workers dying of heat stress in Qatar ...","displayLink":"www.theguardian.com","formattedUrl":"https://www.theguardian.com/.../revealed-hundreds-of-migrant-workers-dyi..."},{"title":"InSight Crime, Author at InSight Crime - Page 12 of 22","displayLink":"insightcrime.org","formattedUrl":"https://insightcrime.org/author/insight-crime/page/12/"},{"title":"Critical care after lung resection: CALoR 1, a single‐centre pilot ...","displayLink":"associationofanaesthetists-publications.onlinelibrary.wiley.com","formattedUrl":"https://associationofanaesthetists-publications.onlinelibrary.wiley.com/.../an..."},{"title":"William Frievogel, Author at Investigate Midwest","displayLink":"investigatemidwest.org","formattedUrl":"https://investigatemidwest.org/author/william-frievogel/"},{"title":"Author Info | PLOS ONE","displayLink":"journals.plos.org","formattedUrl":"https://journals.plos.org/plosone/article/authors?id=10.1371/journal..."},{"title":"The National Archives","displayLink":"webarchive.nationalarchives.gov.uk","formattedUrl":"https://webarchive.nationalarchives.gov.uk/.../insights-issed03-art03.html"}]</t>
   </si>
   <si>
     <t>Deshidratación / sed</t>
@@ -679,7 +679,7 @@
     <t>inusual</t>
   </si>
   <si>
-    <t>[{"title":"Huelga de hambre en Guantánamo se debe a frustración de presos ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-eeuu-guantanamo-idLTASIE92J0..."},{"title":"Presidente Petro reabre la puerta comercial con Venezuela | Fotos ...","displayLink":"sputniknews.lat","formattedUrl":"https://sputniknews.lat/.../presidente-petro-reabre-la-puerta-comercial-con-v..."},{"title":"Qué es la ameba \"come cerebros\" y cómo puedes evitar que te ...","displayLink":"www.bbc.com","formattedUrl":"http://www.bbc.com/mundo/noticias-45863292"},{"title":"Ola de calor en Colombia: Ideam advirtió temperaturas que podrían ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../ola-de-calor-en-colombia-ideam-advirtio-temp..."},{"title":"El libertador No. 23 by Universidad Simón Bolívar Cúcuta - Issuu","displayLink":"issuu.com","formattedUrl":"https://issuu.com/usimon/docs/el_libertador_23-2014-2"},{"title":"DIRECTIVOS Revista Nodo Norte de Santander Periodicidad : anual","displayLink":"www.fesc.edu.co","formattedUrl":"https://www.fesc.edu.co/portal/archivos/.../Revista_Nodo_NdS-Vol1.pdf"},{"title":"CICL O 5","displayLink":"www.redacademica.edu.co","formattedUrl":"https://www.redacademica.edu.co/sites/default/files/.../05Libro_Ciclo5.pdf"},{"title":"La travesía de 24 caminantes que se perdieron en el cerro La Judía ...","displayLink":"www.eluniversal.com.co","formattedUrl":"https://www.eluniversal.com.co/.../la-travesia-de-24-caminantes-que-se-per..."},{"title":"INFORME DE CLASIFICACIÒN NUTRICIONAL POR ...","displayLink":"repositoriodspace.unipamplona.edu.co","formattedUrl":"http://repositoriodspace.unipamplona.edu.co/jspui/.../Pérez_2020_TG.pdf"},{"title":"EXPERIENCIAS POSOPERATORIO CIRUGIA CARDIOVASCULAR ...","displayLink":"repository.javeriana.edu.co","formattedUrl":"https://repository.javeriana.edu.co/.../Trabajo%20ajustes%20jurados%20%2..."}]</t>
+    <t>[{"title":"Staphylococcus aureus and Staphylococcal Food-Borne Disease ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3988705/"},{"title":"Todo lo que sabemos sobre la sal podría estar equivocado - The ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/.../todo-lo-que-sabemos-sobre-la-sal-podria-estar-..."},{"title":"Real-life study of the effectiveness of a high calorie and high protein ...","displayLink":"www.elsevier.es","formattedUrl":"https://www.elsevier.es/en-revista-endocrinologia-diabetes-nutricion-english..."},{"title":"Exercise fluid replacement: is thirst enough? | Semantic Scholar","displayLink":"www.semanticscholar.org","formattedUrl":"https://www.semanticscholar.org/.../3e9df12751ffdc19ec6df73ea862dd640..."},{"title":"| Thirst and mood scales means, SDs, and F ratios by water ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Thirst-and-mood-scales-means-SDs-and-F-r..."},{"title":"Aliviar la sed con bebidas azucaradas puede deshidratar y causar ...","displayLink":"www.chicagotribune.com","formattedUrl":"https://www.chicagotribune.com/efe-3651664-14295388-20180616-story...."},{"title":"(PDF) Culture media used in the proliferation of edible mushrooms ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../367136576_Culture_media_used_in_the_p..."},{"title":"10 signos de diabetes no controlada","displayLink":"www.medicalnewstoday.com","formattedUrl":"https://www.medicalnewstoday.com/.../es/signos-de-diabetes-incontrolados"},{"title":"If I Had Given Him Just One Bottle, He Would Still Be Alive. - Fed Is ...","displayLink":"fedisbest.org","formattedUrl":"https://fedisbest.org/2017/02/given-just-one-bottle-still-alive/"},{"title":"Amanecer con migraña: Causas, tratamientos y prevención","displayLink":"www.medicalnewstoday.com","formattedUrl":"https://www.medicalnewstoday.com/articles/es/despertar-con-migrana"}]</t>
   </si>
   <si>
     <t>Golpe de calor</t>
@@ -688,7 +688,7 @@
     <t>proliferación</t>
   </si>
   <si>
-    <t>[{"title":"Autoridades de salud en Cúcuta en alerta por fuerte oleada de calor ...","displayLink":"www.rcnradio.com","formattedUrl":"https://www.rcnradio.com/.../autoridades-de-salud-en-cucuta-en-alerta-por-..."},{"title":"Ola de calor en Cúcuta: estos efectos podrían generarse en los ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/ola...calor.../202332/"},{"title":"Qué es el estrés térmico que los científicos piden incluir en las ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-65429152"},{"title":"Insoportable: así estará el intenso calor en Cúcuta este martes, 26 ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...calor-en.../202335/"},{"title":"El cambio climático podría llevar la malaria hasta Inglaterra | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../internacional-clima-malaria-inglaterra-s-idLTA..."},{"title":"Qué calor: a 37 grados estará la temperatura en Cúcuta este lunes 2 ...","displayLink":"www.semana.com","formattedUrl":"https://www.semana.com/nacion/cucuta/articulo/...calor.../202330/"},{"title":"El éxodo venezolano: 200 kilómetros a pie por los Andes - The New ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/es/2019/02/.../venezuela-migrantes-cucuta.html"},{"title":"Ola de calor en Colombia: consejos para cuidar a su perro o gato de ...","displayLink":"www.eltiempo.com","formattedUrl":"https://www.eltiempo.com/.../ola-de-calor-en-colombia-consejos-para-cuida..."},{"title":"Fue hallado muerto motociclista desaparecido mientras competía en ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../fue-hallado-muerto-motociclista-desaparecido-..."},{"title":"¿Cómo reconocer si sufres un golpe de calor o una insolación ...","displayLink":"www.univision.com","formattedUrl":"https://www.univision.com/local/fresno.../reconocer-golpe-calor-insolacion"}]</t>
+    <t>[{"title":"Heatstroke in dogs and cats - prevention, symptoms and first aid tips ...","displayLink":"www.rvc.ac.uk","formattedUrl":"https://www.rvc.ac.uk/small-animal-vet/.../heatstroke-in-dogs-and-cats"},{"title":"Heat Stroke - StatPearls - NCBI Bookshelf","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/books/NBK537135/"},{"title":"Heatstroke - Symptoms and causes - Mayo Clinic","displayLink":"www.mayoclinic.org","formattedUrl":"https://www.mayoclinic.org/diseases-conditions/heat.../syc-20353581"},{"title":"Comparison between the Bouchama and Japanese Association for ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6765926/"},{"title":"Las deficientes salvaguardias normativas dejan a los trabajadores ...","displayLink":"investigatemidwest.org","formattedUrl":"https://investigatemidwest.org/.../las-deficientes-salvaguardias-normativas-d..."},{"title":"Heat exposure in the U.S. has led to hundreds of worker deaths ...","displayLink":"www.npr.org","formattedUrl":"https://www.npr.org/.../hundreds-of-workers-have-died-from-heat-in-the-la..."},{"title":"Rhabdomyolysis and Acute Kidney Injury due to Severe Heat Stroke","displayLink":"www.hindawi.com","formattedUrl":"https://www.hindawi.com/journals/cricc/2011/951719/"},{"title":"Incidence and risk factors for heat-related illness (heatstroke) in UK ...","displayLink":"www.nature.com","formattedUrl":"https://www.nature.com/articles/s41598-020-66015-8"},{"title":"Northern India Endures Heat Wave, and a Wave of Deaths - The ...","displayLink":"www.nytimes.com","formattedUrl":"https://www.nytimes.com/2023/06/18/world/asia/india-heat-death.html"},{"title":"Death of adopted Russian child in U.S. spurs anger in Moscow - The ...","displayLink":"www.washingtonpost.com","formattedUrl":"https://www.washingtonpost.com/.../493b3862-7aa0-11e2-9a75-dab02016..."}]</t>
   </si>
   <si>
     <t>escorpiones</t>
@@ -700,7 +700,7 @@
     <t>muerte / muertes / defunciones</t>
   </si>
   <si>
-    <t>[{"title":"Colombia Begins 2021 with Alarming Records of Violence","displayLink":"www.wola.org","formattedUrl":"https://www.wola.org/.../colombia-begins-2021-alarming-records-violence-..."},{"title":"Héctor Mancilla - Manager profile | Transfermarkt","displayLink":"www.transfermarkt.us","formattedUrl":"https://www.transfermarkt.us/hector-mancilla/profil/trainer/103773"},{"title":"Cómo el clima afecta a los insectos – Insectos después de la lluvia ...","displayLink":"www.raid.com","formattedUrl":"https://www.raid.com/es-US/education/bug.../how-weather-affects-insects"},{"title":"Murder Page 21","displayLink":"theync.com","formattedUrl":"https://theync.com/channels/11/murder/page21.html"},{"title":"NotiFrontera Cúcuta","displayLink":"www.facebook.com","formattedUrl":"https://www.facebook.com/NOTIFRONTERACUCUTAA/"},{"title":"yo me inventé “El escorpión” rene higuita","displayLink":"www.soho.co","formattedUrl":"https://www.soho.co/historias/articulo/yo-me-invente-el...rene.../61362/"},{"title":"La Legión (@legion_tica) • Instagram photos and videos","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/legion_tica/?hl=en"},{"title":"Barranquilla FC vs Cúcuta Deportivo Predicción, cuotas y consejos ...","displayLink":"betimate.com","formattedUrl":"https://betimate.com/.../news/.../barranquilla-fc-vs-cucuta-deportivo-predicti..."},{"title":"Acta Toxicológica Argentina","displayLink":"www.toxicologia.org.ar","formattedUrl":"https://www.toxicologia.org.ar/wp-content/.../01/acta-25-1-2017-alta.pdf"},{"title":"Héctor Mancilla - Wikipedia","displayLink":"it.wikipedia.org","formattedUrl":"https://it.wikipedia.org/wiki/Héctor_Mancilla"}]</t>
+    <t>[{"title":"Everything we know about the kidnapping of 4 Americans in Mexico ...","displayLink":"abcnews.go.com","formattedUrl":"https://abcnews.go.com/International/kidnapping-4-americans.../story?id..."},{"title":"Cyclones, Scorpions and Old School Killers - The War for Tamaulipas","displayLink":"insightcrime.org","formattedUrl":"https://insightcrime.org/.../cyclones-scorpions-old-school-killers-war-tamaul..."},{"title":"Gulf cartel apologizes after Americans are kidnapped and killed in ...","displayLink":"www.nbcnews.com","formattedUrl":"https://www.nbcnews.com/.../gulf-cartel-apologizes-americans-are-kidnapp..."},{"title":"\"El Lobista\" La rana y el Escorpion (TV Episode 2018) - IMDb","displayLink":"www.imdb.com","formattedUrl":"https://www.imdb.com/title/tt11186722/"},{"title":"Escorpiones del estado de Ceará, Brasil: distribución y comentarios ...","displayLink":"www.scielo.org.pe","formattedUrl":"http://www.scielo.org.pe/scielo.php?script=sci_arttext&amp;pid=S1727..."},{"title":"RANCHO EL ESCORPION LIME KILN El Escorpion Park, between ...","displayLink":"planning.lacity.org","formattedUrl":"https://planning.lacity.org/.../5.../RanchoElEscorpionLimeKiln_FINAL.pdf"},{"title":"Escorpion Mandíbulas | Ask A Biologist","displayLink":"askabiologist.asu.edu","formattedUrl":"https://askabiologist.asu.edu/escorpion-quijadas"},{"title":"(PDF) Estudio monográfico de los escorpiones de la República ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../291997537_Estudio_monografico_de_los_..."},{"title":"AllPolitics - Congress Probes Passport 900 Telephone Number ...","displayLink":"www.cnn.com","formattedUrl":"http://www.cnn.com/ALLPOLITICS/1997/05/13/email/900/"},{"title":"Toxicological and epidemiological studies of scorpion sting cases ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6479097/"}]</t>
   </si>
   <si>
     <t>accidente ofídico</t>
@@ -709,7 +709,7 @@
     <t>colapsar</t>
   </si>
   <si>
-    <t>[{"title":"Accidente Ofídico y Leishmaniasis, un desafío en Enfermedades ...","displayLink":"www.ins.gov.co","formattedUrl":"https://www.ins.gov.co/.../2021_Boletin_epidemiologico_semana_12.pdf"},{"title":"Análisis de Situación de Salud (ASIS) Colombia, 2021 Dirección de ...","displayLink":"www.minsalud.gov.co","formattedUrl":"https://www.minsalud.gov.co/.../analisis-situacion-salud-colombia-2021.pdf"},{"title":"Accidente Ofídico","displayLink":"www.ins.gov.co","formattedUrl":"https://www.ins.gov.co/.../2022_Boletín_epidemiologico_semana_27.pdf"},{"title":"Análisis de Situación de Salud Norte de Santander 2022","displayLink":"ids.gov.co","formattedUrl":"https://ids.gov.co/.../ASIS_DEPARTAMENTAL_NORTE%20DE_SANTA..."},{"title":"Revista del Instituto Nacional de Salud","displayLink":"revistabiomedica.org","formattedUrl":"https://revistabiomedica.org/index.php/biomedica/issue/download/176/74"},{"title":"cartilla rutas","displayLink":"www.yumpu.com","formattedUrl":"https://www.yumpu.com/es/document/view/65652127/cartilla-rutas"},{"title":"2023-boletin-epidemiologico-semana-8.pdf","displayLink":"www.ins.gov.co","formattedUrl":"http://www.ins.gov.co/.../2023-boletin-epidemiologico-semana-8.pdf"},{"title":"CARACTERIZACION DE LA OFIDIOTOXICOSIS Y SU ...","displayLink":"repositoriodspace.unipamplona.edu.co","formattedUrl":"http://repositoriodspace.unipamplona.edu.co/.../Blanco_Camayo_Álvarez_2..."},{"title":"Acta Toxicológica Argentina","displayLink":"www.toxicologia.org.ar","formattedUrl":"https://www.toxicologia.org.ar/wp-content/.../01/acta-25-1-2017-alta.pdf"},{"title":"Revisión de estrategias de turismo de salud e identificación de ...","displayLink":"revistas.unab.edu.co","formattedUrl":"https://revistas.unab.edu.co/index.php/medunab/article/view/2582"}]</t>
+    <t>[{"title":"Agente causal del accidente ofídico y notificaciones atribuidas a los ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-4-Agente-causal-del-accidente-ofidi..."},{"title":"Poor efficacy of preemptive amoxicillin clavulanate for preventing ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5519217/"},{"title":"(PDF) Primer registro de accidentes ofídicos por mordedura de ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../357313426_Primer_registro_de_accidentes..."},{"title":"A generalized framework for estimating snakebite underreporting ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9934346/"},{"title":"Descripción de los eventos por Envenenamiento Ofídico en ...","displayLink":"repositorio.una.ac.cr","formattedUrl":"https://repositorio.una.ac.cr/handle/11056/12892"},{"title":"Comportamiento epidemiológico del accidente ofídico en el ...","displayLink":"revistas.urosario.edu.co","formattedUrl":"https://revistas.urosario.edu.co/index.php/revsalud/article/view/4938"},{"title":"Clinical characteristics and use of antibiotics in a group of patients ...","displayLink":"journals.sagepub.com","formattedUrl":"https://journals.sagepub.com/doi/abs/10.1177/20499361231210400"},{"title":"UNIVERSIDAD LAICA \"ELOY ALFARO\" DE MANABI: Accidente ...","displayLink":"repositorio.uleam.edu.ec","formattedUrl":"https://repositorio.uleam.edu.ec/handle/123456789/4536?mode=full"},{"title":"Clinical characteristics and use of antibiotics in a group of patients ...","displayLink":"journals.sagepub.com","formattedUrl":"https://journals.sagepub.com/doi/10.1177/20499361231210400"},{"title":"Accidente Ofídico y Leishmaniasis, un desafío en Enfermedades ...","displayLink":"www.ins.gov.co","formattedUrl":"https://www.ins.gov.co/.../2021_Boletin_epidemiologico_semana_12.pdf"}]</t>
   </si>
   <si>
     <t>Causa</t>
@@ -862,19 +862,19 @@
     <t>sequ?as extremas</t>
   </si>
   <si>
-    <t>[{"title":"Immigration news in the Global South: A comparative analysis of ...","displayLink":"conservancy.umn.edu","formattedUrl":"https://conservancy.umn.edu/.../Severino_umn_0130E_21659.pdf?sequenc..."},{"title":"Iglesia Centro Cristiano abre congregação em Nova York - CPAD ...","displayLink":"www.cpadnews.com.br","formattedUrl":"https://www.cpadnews.com.br/iglesia-centro-cristiano-abre-congregacao-e..."},{"title":"Haitianos são enviados de volta a um país em caos | Human Rights ...","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/pt/news/2022/.../haitians-being-returned-country-chao..."},{"title":"Trump amenaza a Universidad de California en Berkeley tras ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/eeuu-trump-berkeley-idLTAKBN15H2JK/"},{"title":"Perceptions and attitudes of young university students about ...","displayLink":"files.eric.ed.gov","formattedUrl":"https://files.eric.ed.gov/fulltext/EJ1379508.pdf"},{"title":"Health services inequalities affecting the Venezuelan migrant and ...","displayLink":"profamilia.org.co","formattedUrl":"https://profamilia.org.co/.../Health-services-inequalities-affecting-the-Venez..."},{"title":"CYC16-3 SEP-DIC2019.indd","displayLink":"dialnet.unirioja.es","formattedUrl":"https://dialnet.unirioja.es/descarga/articulo/7490911.pdf"},{"title":"Viewing Subject: Latin American Studies - JSTOR","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/subject/latinamericanstudies"},{"title":"Capítulo 3 El trabajo sexual una de las múltiples violencias a la ...","displayLink":"bonga.unisimon.edu.co","formattedUrl":"https://bonga.unisimon.edu.co/.../Cap_3_TrabajoSexual.pdf?sequence..."},{"title":"El desprecio como narrativa prototípica: análisis del cubrimiento ...","displayLink":"repositorio.unal.edu.co","formattedUrl":"https://repositorio.unal.edu.co/bitstream/.../33376949.2022.pdf?sequence..."}]</t>
+    <t>[{"title":"Local extrema in random permutations and the structure of longest ...","displayLink":"www.math.ucdavis.edu","formattedUrl":"https://www.math.ucdavis.edu/~romik/data/uploads/.../alter-revised.pdf"},{"title":"Getting the maximum / minimum value of a shifting sequence - Stack ...","displayLink":"stackoverflow.com","formattedUrl":"https://stackoverflow.com/.../getting-the-maximum-minimum-value-of-a-sh..."},{"title":"Calculus I - Finding Absolute Extrema","displayLink":"tutorial.math.lamar.edu","formattedUrl":"https://tutorial.math.lamar.edu/classes/calci/absextrema.aspx"},{"title":"python - Finding local maxima/minima with Numpy in a 1D numpy ...","displayLink":"stackoverflow.com","formattedUrl":"https://stackoverflow.com/.../finding-local-maxima-minima-with-numpy-in..."},{"title":"LE-DTA: Local Extrema Convolution for Drug Target Affinity ...","displayLink":"ieeexplore.ieee.org","formattedUrl":"https://ieeexplore.ieee.org/document/10096347"},{"title":"How to Estimate a VAR after March 2020 | NBER","displayLink":"www.nber.org","formattedUrl":"https://www.nber.org/papers/w27771"},{"title":"On special extrema of polynomials with applications to Diophantine ...","displayLink":"link.springer.com","formattedUrl":"https://link.springer.com/article/10.1007/s40993-019-0178-6"},{"title":"El Niño–Southern Oscillation extrema in the Holocene and Last ...","displayLink":"agupubs.onlinelibrary.wiley.com","formattedUrl":"https://agupubs.onlinelibrary.wiley.com/doi/10.1029/2012PA002378"},{"title":"Algebra 2 Curriculum | Fairfax County Public Schools","displayLink":"www.fcps.edu","formattedUrl":"https://www.fcps.edu/academics/high-school-grades-9-12/.../algebra-2"},{"title":"Press release: The Nobel Prize in Physiology or Medicine 2022 ...","displayLink":"www.nobelprize.org","formattedUrl":"https://www.nobelprize.org/prizes/medicine/2022/press-release/"}]</t>
   </si>
   <si>
     <t>condiciones meteorol�gicas</t>
   </si>
   <si>
-    <t>[{"title":"César Pérez Vivas (@cesarperezvivas) • Instagram photos and videos","displayLink":"www.instagram.com","formattedUrl":"https://www.instagram.com/cesarperezvivas/"},{"title":"Corporación Educativa SinFronteras: Inicio","displayLink":"corposinfronteras.edu.co","formattedUrl":"https://corposinfronteras.edu.co/"},{"title":"https://huggingface.co/ixa-ehu/ixambert-base-cased...","displayLink":"huggingface.co","formattedUrl":"https://huggingface.co/ixa-ehu/ixambert-base-cased/resolve/.../vocab.txt"},{"title":"Periodismo, “noticias falsas” &amp; desinformación: manual de ...","displayLink":"unesdoc.unesco.org","formattedUrl":"https://unesdoc.unesco.org/ark:/48223/pf0000373349"},{"title":"Caracol Radio | Noticias, deportes y opinión en Colombia | Caracol ...","displayLink":"caracol.com.co","formattedUrl":"https://caracol.com.co/"},{"title":"Acta Toxicológica Argentina","displayLink":"www.toxicologia.org.ar","formattedUrl":"https://www.toxicologia.org.ar/wp-content/.../01/acta-25-1-2017-alta.pdf"},{"title":"Revista Colombiana de Ciencias","displayLink":"revistas.uptc.edu.co","formattedUrl":"https://revistas.uptc.edu.co/index.../RCCH%2013%282%29%2C%202019"},{"title":"venezolanos en New Jersey, | Facebook","displayLink":"www.facebook.com","formattedUrl":"https://www.facebook.com/groups/568574393563638/"},{"title":"\"La llegada masiva de venezolanos me llevó a pensar en lo ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-55724714"},{"title":"Venezuelan women hi-res stock photography and images - Alamy","displayLink":"www.alamy.com","formattedUrl":"https://www.alamy.com/stock-photo/venezuelan-women.html"}]</t>
+    <t>[{"title":"oficial para licencias de conducir de florida","displayLink":"www.flhsmv.gov","formattedUrl":"https://www.flhsmv.gov/pdf/handbooks/spanishdriverhandbook.pdf"},{"title":"Geographic location of the study area in the southwest of the Sierra ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Geographic-location-of-the-study-area-in-t..."},{"title":"Research Estimating mortality, morbidity and disability due to ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2557714/.../10516785.pdf"},{"title":"Ubicaci?n de estaciones: hidrom?trica y meteorol?gicas, vectores ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-1-Ubicacin-de-estaciones-hidromtric..."},{"title":"Research Note Weather Variables Affecting Oklahoma Wildfires","displayLink":"journals.uair.arizona.edu","formattedUrl":"https://journals.uair.arizona.edu/index.php/jrm/article/download/.../19691"},{"title":"JAIC , Volume 39, Number 2, Article 6 (pp. to )","displayLink":"cool.culturalheritage.org","formattedUrl":"https://cool.culturalheritage.org/jaic/articles/jaic39-02-006.html"},{"title":"Vista de Bancos de Germoplasma para salvaguardar las ...","displayLink":"dominiodelasciencias.com","formattedUrl":"https://dominiodelasciencias.com/ojs/index.php/es/article/view/1258/html"},{"title":"E1 Nifo Occurrences Over the Past Four and a Half Centuries","displayLink":"rainbow.ldeo.columbia.edu","formattedUrl":"http://rainbow.ldeo.columbia.edu/~alexeyk/Papers/Quinn_etal1987.pdf"},{"title":"trayectorias de misiles bal?sticos - intercontinentales: implicaciones ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/27755685"},{"title":"DECLARATORIA de vigencia de las normas mexicanas NMX-AA ...","displayLink":"www.dof.gob.mx","formattedUrl":"https://www.dof.gob.mx/nota_detalle_popup.php?codigo=5312875"}]</t>
   </si>
   <si>
     <t>Fenomenos clim?ticos extremos</t>
   </si>
   <si>
-    <t>[{"title":"Índice de vulnerabilidad y adaptación al cambio climático en la ...","displayLink":"scioteca.caf.com","formattedUrl":"https://scioteca.caf.com/.../caf-indice-vulnerabilidad-cambio-climatico.pdf"},{"title":"Migraciones, ambiente y cambio climático: estudios de caso en ...","displayLink":"publications.iom.int","formattedUrl":"https://publications.iom.int/.../migraciones_ambiente_y_cambio_climatico_..."},{"title":"Ola Invernal Colombia 2010-2011","displayLink":"www.cepal.org","formattedUrl":"https://www.cepal.org/sites/.../news/.../ola_invernal_colombia_2010-2011_..."},{"title":"Violencia Política contra las mujeres","displayLink":"mlkrook.org","formattedUrl":"http://mlkrook.org/pdf/VPCM_20.pdf"},{"title":"Informe Mundial sobre Desplazamiento Interno","displayLink":"www.internal-displacement.org","formattedUrl":"https://www.internal-displacement.org/sites/.../2019-IDMC-GRID-sp.pdf"},{"title":"AF-DIGITAL-CORREGIDO-El Agua como Derecho Humano-3.indd","displayLink":"www.corteidh.or.cr","formattedUrl":"https://www.corteidh.or.cr/docs/.../El_Agua_como_Derecho_Humano.pdf"},{"title":"(PDF) Cambio climático y variabilidad climática para el periodo ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../273773968_Cambio_climatico_y_variabili..."},{"title":"EXTREMOS POLÍTICOS","displayLink":"www.kas.de","formattedUrl":"https://www.kas.de/...1.../a465f0e9-e8f3-9c4c-d3ab-658697b6ba08?..."},{"title":"Calidad del aire: ¡Es el momento de actuar! | UNICEF","displayLink":"www.unicef.org","formattedUrl":"https://www.unicef.org/lac/.../Calidad-del-aire-es-el-momento-de-actuar.pdf"},{"title":"Aumenta el calor en Colombia: A qué se debe y cuánto tiempo ...","displayLink":"www.infobae.com","formattedUrl":"https://www.infobae.com/.../aumenta-el-calor-en-colombia-a-que-se-debe-y..."}]</t>
+    <t>[{"title":"Atlas de la OMM sobre mortalidad y pérdidas económicas debidas a ...","displayLink":"library.wmo.int","formattedUrl":"https://library.wmo.int/.../28270-atlas-de-la-omm-sobre-mortalidad-y-perdi..."},{"title":"Extreme weather events and high Colombian food prices: A non","displayLink":"repositorio.banrep.gov.co","formattedUrl":"https://repositorio.banrep.gov.co/bitstream/handle/20.../be_1189.pdf?..."},{"title":"¿Cuál es la diferencia entre el calentamiento global y el cambio ...","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/.../climate.../¿cuál-es-la-diferencia-entre-el-calentam..."},{"title":"Frecuencia (%) de eventos clim?ticos-meteorol?gicos extremos en ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-2-Frecuencia-de-eventos-climticos-..."},{"title":"La Temporada de Peligros climáticos está aquí. ¿Qué puede ...","displayLink":"blog.ucsusa.org","formattedUrl":"https://blog.ucsusa.org/.../la-temporada-de-peligros-climaticos-esta-aqui-qu..."},{"title":"(PDF) Fenómenos climáticos extremos y sus efectos en el Caribe ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../326092848_Fenomenos_climaticos_extrem..."},{"title":"Projects gallery 2022-2023 – Climate detectives","displayLink":"climatedetectives.esa.int","formattedUrl":"https://climatedetectives.esa.int/projects-gallery-2022-2023/entry/59301/"},{"title":"Evidencia | Datos – Climate Change: Vital Signs of the Planet","displayLink":"climate.nasa.gov","formattedUrl":"https://climate.nasa.gov/en-espanol/"},{"title":"Early warning system on extreme weather events for disaster risk ...","displayLink":"link.gale.com","formattedUrl":"https://link.gale.com/apps/doc/A600269433/IFME?u=googlescholar..."},{"title":"Desarrollo resiliente al clima de los servicios de agua, saneamiento ...","displayLink":"www.gwp.org","formattedUrl":"https://www.gwp.org/.../global/.../gwp_unicef_strategic_framework_es.pdf"}]</t>
   </si>
   <si>
     <t>producci�n de informaci�n</t>
@@ -886,28 +886,34 @@
     <t>Articulaci�n</t>
   </si>
   <si>
-    <t>[{"title":"FENÓMENO EL NIÑO Y CAPTACIÓN ILEGAL DE AGUA ...","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/2313-fenomeno-el-nino-y-captacion-ilegal-..."},{"title":"Los caminantes venezolanos | Human Rights Watch","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/es/news/2018/09/05/los-caminantes-venezolanos"},{"title":"Temperaturas máximas de 40 grados Han bordeado a Cúcuta.","displayLink":"corponor.gov.co","formattedUrl":"https://corponor.gov.co/...news/429-temperaturas-maximas-de-40-grados-h..."},{"title":"La posible vuelta del fenómeno El Niño amenaza con batir récords ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2023/03/1518967"},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-63323077"},{"title":"Pacto Mundial sobre Migración: ¿a qué obliga y qué beneficios ...","displayLink":"news.un.org","formattedUrl":"https://news.un.org/es/story/2018/12/1447231"},{"title":"Versión debilitada de La Niña aleja temores de pérdidas de soja y ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../granos-sudamerica-clima-idLTAKCN10722L/"},{"title":"La migración vista como una gran oportunidad para el desarrollo","displayLink":"www.bancomundial.org","formattedUrl":"https://www.bancomundial.org/.../news/.../la-migracion-vista-como-una-gra..."},{"title":"Huir para ver la luz: el éxodo de las embarazadas venezolanas ...","displayLink":"www.amnesty.org","formattedUrl":"https://www.amnesty.org/.../news/.../huir-para-ver-la-luz-el-exodo-de-las-e..."},{"title":"Frontera Colombo-Venezolana. Iglesia preocupada por trata y ...","displayLink":"www.vaticannews.va","formattedUrl":"https://www.vaticannews.va/.../news/.../frontera-colombo-venezolana-preoc..."}]</t>
+    <t>[{"title":"El Niño and Variations in Climate: Large-scale interactions between ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/27853159"},{"title":"In situ construction of porous hierarchical (Ni3-xFex)FeN/Ni ...","displayLink":"link.springer.com","formattedUrl":"https://link.springer.com/article/10.1007/s12274-020-2649-4"},{"title":"Comprehensive Cancer Information - NCI","displayLink":"www.cancer.gov","formattedUrl":"https://www.cancer.gov/"},{"title":"Fentanyl | National Institute on Drug Abuse (NIDA)","displayLink":"nida.nih.gov","formattedUrl":"https://nida.nih.gov/research-topics/fentanyl"},{"title":"INTRODUCTION","displayLink":"archive.unu.edu","formattedUrl":"https://archive.unu.edu/env/govern/ElNIno/.../Introduction_txt.html"},{"title":"SOLUTION: Fen meno del ni o y la ni a - Studypool","displayLink":"www.studypool.com","formattedUrl":"https://www.studypool.com/documents/.../fen-meno-del-ni-o-y-la-ni-a-"},{"title":"List of Institutes and Centers | National Institutes of Health (NIH)","displayLink":"www.nih.gov","formattedUrl":"https://www.nih.gov/institutes-nih/list-institutes-centers"},{"title":"The environmental envelope of fires in the Colombian Caribbean","displayLink":"stri-sites.si.edu","formattedUrl":"https://stri-sites.si.edu/docs/.../Hoyos_et_al_2017_AppliedGeography.pdf"},{"title":"Dissipation of Micropollutants in a Rewetted Fen Peatland: A Field ...","displayLink":"www.mdpi.com","formattedUrl":"https://www.mdpi.com/2073-4441/9/6/449"},{"title":"University of Cambridge","displayLink":"www.cam.ac.uk","formattedUrl":"https://www.cam.ac.uk/"}]</t>
+  </si>
+  <si>
+    <t>Oscilaci�n del sur</t>
+  </si>
+  <si>
+    <t>Comunicaci�n</t>
+  </si>
+  <si>
+    <t>[{"title":"Publications - Levy Research Group","displayLink":"www.klevyresearch.org","formattedUrl":"http://www.klevyresearch.org/publications.html"},{"title":"A Phylogeographical Analysis across Three Biogeographical ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/20488425"},{"title":"Precipitaci?n y temperatura media mensual de cuatro estaciones ...","displayLink":"www.researchgate.net","formattedUrl":"https://www.researchgate.net/.../Figura-2-Precipitacin-y-temperatura-media-..."},{"title":"JSS: TC, 7, 1 (1979) lismos: Latinoam?rica y Espa?a. Philadelphia ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/27740868"},{"title":"Martínez-Sifuentes AR, Villanueva-Díaz J, Estrada-Ávalos J (2020 ...","displayLink":"iforest.sisef.org","formattedUrl":"https://iforest.sisef.org/pdf/?id=ifor3190-013"},{"title":"Nonlinear relationship between the weather phenomenon El ni~no ...","displayLink":"onlinelibrary.wiley.com","formattedUrl":"https://onlinelibrary.wiley.com/doi/pdf/10.1111/1467-8489.12394"},{"title":"Vista de Severidad y extensión de incendios mediante índice de ...","displayLink":"revistas.uned.ac.cr","formattedUrl":"https://revistas.uned.ac.cr/index.php/repertorio/article/view/3749/5230"},{"title":"Instituto del Mar del Perú - IMARPE - Plataforma del Estado Peruano","displayLink":"www.gob.pe","formattedUrl":"https://www.gob.pe/imarpe"},{"title":"diags/vignettes/refs.bib at master · flr/diags · GitHub","displayLink":"github.com","formattedUrl":"https://github.com/flr/diags/blob/master/vignettes/refs.bib"},{"title":"Seasonality of erosion and eolian particle transport in the coastal ...","displayLink":"www.andeangeology.cl","formattedUrl":"http://www.andeangeology.cl/index.php/revista1/article/view/V36n2.../html"}]</t>
   </si>
   <si>
     <t>Del ni?o</t>
   </si>
   <si>
-    <t>[{"title":"Venezuela's Desperation Spilling Into Neighboring Colombia - CBS ...","displayLink":"www.cbsnews.com","formattedUrl":"https://www.cbsnews.com/.../news/venezuelas-desperation-spilling-neighbor..."},{"title":"Atacan helicóptero del presidente de Colombia, sin víctimas | AP ...","displayLink":"apnews.com","formattedUrl":"https://apnews.com/article/noticias-84b7a351a36b7181787e1b5d73f89f6a"},{"title":"More US Humanitarian Aid For Venezuela Arrives In Colombia ...","displayLink":"www.cbsnews.com","formattedUrl":"https://www.cbsnews.com/.../news/more-us-humanitarian-aid-for-venezuela..."},{"title":"Qué hay detrás del insólito auge de estaciones de gasolina en ...","displayLink":"www.bbc.com","formattedUrl":"https://www.bbc.com/mundo/noticias-america-latina-63323077"},{"title":"Prohíben a enviados del CIDH visitar Venezuela; recabarán datos ...","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/article/venezuela-cidh-idLTAKBN1ZY29X/"},{"title":"Chivas se queda sin pan ni pedazo | MLSSoccer.com","displayLink":"www.mlssoccer.com","formattedUrl":"https://www.mlssoccer.com/news/chivas-se-queda-sin-pan-ni-pedazo"},{"title":"Los caminantes venezolanos | Human Rights Watch","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/es/news/2018/09/05/los-caminantes-venezolanos"},{"title":"Tibú, the Colombian town with the most coca in the world, but no ...","displayLink":"english.elpais.com","formattedUrl":"https://english.elpais.com/.../tibu-the-colombian-town-with-the-most-coca-i..."},{"title":"Exmilitares venezolanos en el exilio | Human Rights Watch","displayLink":"www.hrw.org","formattedUrl":"https://www.hrw.org/es/news/2019/05/.../exmilitares-venezolanos-en-el-exil..."},{"title":"Meet Alexandra, Nurse Manager at our Comuneros Clinic in Cúcuta ...","displayLink":"medglobal.org","formattedUrl":"https://medglobal.org/meet-alexandra-cardenas-nurse-manager-at-our-com..."}]</t>
+    <t>[{"title":"EU to investigate 'flood' of Chinese electric cars, weigh tariffs | Reuters","displayLink":"www.reuters.com","formattedUrl":"https://www.reuters.com/.../eu-launches-anti-subsidy-investigation-into-chin..."},{"title":"X-ray magnetic circular dichroism investigation of spin and orbital ...","displayLink":"ui.adsabs.harvard.edu","formattedUrl":"https://ui.adsabs.harvard.edu/abs/2008PhRvB..77a4402C/abstract"},{"title":"A model for the investigation of factors influencing haemorrhagic ...","displayLink":"www.ncbi.nlm.nih.gov","formattedUrl":"https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1554511/"},{"title":"Theoretical Investigation of the Deposition of Cu, Ag, and Au Atoms ...","displayLink":"pubs.acs.org","formattedUrl":"https://pubs.acs.org/doi/abs/10.1021/jp0704057"},{"title":"07/11/2023 21:40 Investigation of Ni@CoO core-shell nanoparticle ...","displayLink":"iris.unimore.it","formattedUrl":"https://iris.unimore.it/retrieve/.../Ni%40CoO%20manuscriptfinalrev2.pdf"},{"title":"View of Investigating potential icequakes at Llaima volcano, Chile","displayLink":"www.jvolcanica.org","formattedUrl":"http://www.jvolcanica.org/ojs/index.php/volcanica/article/view/56/66"},{"title":"Investigation of lunar metal particles","displayLink":"adsabs.harvard.edu","formattedUrl":"https://adsabs.harvard.edu/full/1970GeCAS...1..499G"},{"title":"Experimental and theoretical investigation of the order-disorder ...","displayLink":"www.cambridge.org","formattedUrl":"https://www.cambridge.org/...investigation.../55145643803279542AE260..."},{"title":"Senior ER Investigator, Corporate Employee Relations Central ...","displayLink":"www.amazon.jobs","formattedUrl":"https://www.amazon.jobs/.../senior-er-investigator-corporate-employee-relat..."},{"title":"Spin‐Resolved PES and IPES Investigation of the Graphene/Ni(111 ...","displayLink":"onlinelibrary.wiley.com","formattedUrl":"https://onlinelibrary.wiley.com/doi/abs/10.1002/pssb.201700415"}]</t>
   </si>
   <si>
     <t>El ni?o</t>
   </si>
   <si>
-    <t>fen�meno meteorol�gico</t>
-  </si>
-  <si>
-    <t>[{"title":"https://huggingface.co/ixa-ehu/ixambert-base-cased...","displayLink":"huggingface.co","formattedUrl":"https://huggingface.co/ixa-ehu/ixambert-base-cased/resolve/.../vocab.txt"},{"title":"https://worksheets.codalab.org/rest/bundles/0xadf9...","displayLink":"worksheets.codalab.org","formattedUrl":"https://worksheets.codalab.org/rest/bundles/.../glove.6B.100d.txt-vocab.txt"},{"title":"https://www.cs.toronto.edu/~rkiros/models/dictiona...","displayLink":"www.cs.toronto.edu","formattedUrl":"https://www.cs.toronto.edu/~rkiros/models/dictionary.txt"},{"title":"https://downey-n1.cs.northwestern.edu/downloads/OT...","displayLink":"downey-n1.cs.northwestern.edu","formattedUrl":"https://downey-n1.cs.northwestern.edu/downloads/.../all_entity_str.txt"},{"title":"https://downloads.cs.stanford.edu/nlp/data/jiwei/d...","displayLink":"downloads.cs.stanford.edu","formattedUrl":"https://downloads.cs.stanford.edu/nlp/data/jiwei/data/vocab_wiki.txt"}]</t>
+    <t>[{"title":"INVESTIGATING EL NIÑO USING REAL DATA","displayLink":"www.nnvl.noaa.gov","formattedUrl":"https://www.nnvl.noaa.gov/StoryMaps/DITC/.../ElNino_TeachersGuide.pdf"},{"title":"Investigating El Niño: Teacher Resources | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/el.../investigating-el-nino-teacher-resou..."},{"title":"El Niño: Pacific Wind and Current Changes Bring Warm, Wild Weather","displayLink":"earthobservatory.nasa.gov","formattedUrl":"https://earthobservatory.nasa.gov/features/ElNino"},{"title":"Investigating El Niño Using Data in the Classroom | NESDIS","displayLink":"dataintheclassroom.noaa.gov","formattedUrl":"https://dataintheclassroom.noaa.gov/el.../investigating-el-nino-using-data-th..."},{"title":"How will climate change change El Niño and La Niña? - NOAA ...","displayLink":"research.noaa.gov","formattedUrl":"https://research.noaa.gov/.../new-research-volume-explores-future-of-enso-..."},{"title":"El Niño &amp; La Niña (El Niño-Southern Oscillation) | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/enso"},{"title":"El Niño","displayLink":"www.nationalgeographic.org","formattedUrl":"https://www.nationalgeographic.org/encyclopedia/el-nino/"},{"title":"El Niño and La Niña: Frequently asked questions | NOAA Climate.gov","displayLink":"www.climate.gov","formattedUrl":"http://www.climate.gov/.../el-niño-and-la-niña-frequently-asked-questions"},{"title":"Investigation of the Reaction Thermal Effects in Al-Ni-FeOx ...","displayLink":"ieeexplore.ieee.org","formattedUrl":"https://ieeexplore.ieee.org/document/8656700"},{"title":"Investigation of the Mechanism for Ohmic Contact Formation in Ti/Al ...","displayLink":"pubs.acs.org","formattedUrl":"https://pubs.acs.org/doi/10.1021/acsami.9b09166"}]</t>
   </si>
   <si>
     <t>patr�n clim?tico</t>
   </si>
   <si>
-    <t>[{"title":"Colombian Christians Preached Social Justice. Practicing It Is Harder.","displayLink":"www.christianitytoday.com","formattedUrl":"https://www.christianitytoday.com/.../colombia-social-justice-integral-missio..."},{"title":"Toward a Common Agenda for the Andean Countries and the ...","displayLink":"www.cartercenter.org","formattedUrl":"https://www.cartercenter.org/.../news/peace.../andean-common-agenda-en.p..."},{"title":"Im/mobility in Coronatimes Blog - School of Geography","displayLink":"www.qmul.ac.uk","formattedUrl":"https://www.qmul.ac.uk/geog/research/immobility-in-coronatimes-blog/"},{"title":"Wikipedia:In the news/Candidates/December 2021 - Wikipedia","displayLink":"en.wikipedia.org","formattedUrl":"https://en.wikipedia.org/wiki/Wikipedia:In_the_news/.../December_2021"},{"title":"Ambassador Archives - U.S. Embassy in Costa Rica","displayLink":"cr.usembassy.gov","formattedUrl":"https://cr.usembassy.gov/category/ambassador/"},{"title":"Patron saints of places - Wikipedia","displayLink":"en.wikipedia.org","formattedUrl":"https://en.wikipedia.org/wiki/Patron_saints_of_places"},{"title":"TITLE Hearing on the Department of Education, Office of Civil Rights ...","displayLink":"files.eric.ed.gov","formattedUrl":"https://files.eric.ed.gov/fulltext/ED339264.pdf"},{"title":"2019 Colombian League Preview – COLFOOTBALL","displayLink":"colfootball.wordpress.com","formattedUrl":"https://colfootball.wordpress.com/2019/.../2019-colombian-league-preview/"},{"title":"News Room - auto-gas.net","displayLink":"auto-gas.net","formattedUrl":"https://auto-gas.net/news-room/"},{"title":"Latin America &amp; Caribbean in Review — AP Photos","displayLink":"apimagesblog.com","formattedUrl":"https://apimagesblog.com/blog/.../3/.../latin-america-amp-caribbean-in-revie..."}]</t>
+    <t>[{"title":"IRI – International Research Institute for Climate and Society ...","displayLink":"iri.columbia.edu","formattedUrl":"https://iri.columbia.edu/our-expertise/climate/forecasts/enso/current/"},{"title":"A Neutralizing Monoclonal Antibody for Hospitalized Patients with ...","displayLink":"www.nejm.org","formattedUrl":"https://www.nejm.org/doi/full/10.1056/NEJMoa2033130"},{"title":"Tixagevimab–cilgavimab for treatment of patients hospitalised with ...","displayLink":"www.thelancet.com","formattedUrl":"https://www.thelancet.com/journals/lanres/article/PIIS2213...6/fulltext"},{"title":"UNFCCC","displayLink":"unfccc.int","formattedUrl":"https://unfccc.int/"},{"title":"Capacity of Management Plans for Aquatic Invasive Species to ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/20183423"},{"title":"Special Report on Climate Change and Land — IPCC site","displayLink":"www.ipcc.ch","formattedUrl":"https://www.ipcc.ch/srccl/"},{"title":"Interacting Effects of Phenotypic Plasticity and Evolution on ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/27976427"},{"title":"Costa Rica | History, Map, Flag, Climate, Population, &amp; Facts ...","displayLink":"www.britannica.com","formattedUrl":"https://www.britannica.com/place/Costa-Rica"},{"title":"Current Practices and Future Opportunities for Policy on Climate ...","displayLink":"www.jstor.org","formattedUrl":"https://www.jstor.org/stable/20183425"},{"title":"Politics, Policy, Political News - POLITICO","displayLink":"www.politico.com","formattedUrl":"https://www.politico.com/"}]</t>
   </si>
   <si>
     <t>Atenci�n</t>
@@ -4988,16 +4994,16 @@
         <v>18</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>292</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="F126" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G126" s="0" t="s">
         <v>264</v>
@@ -5006,7 +5012,7 @@
         <v>264</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J126" s="0" t="s">
         <v>265</v>
@@ -5020,16 +5026,16 @@
         <v>18</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F127" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G127" s="0" t="s">
         <v>264</v>
@@ -5038,7 +5044,7 @@
         <v>264</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="J127" s="0" t="s">
         <v>265</v>
@@ -5055,13 +5061,13 @@
         <v>18</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>33</v>
+        <v>297</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="F128" s="0" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G128" s="0" t="s">
         <v>264</v>
@@ -5070,7 +5076,7 @@
         <v>264</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>36</v>
+        <v>298</v>
       </c>
       <c r="J128" s="0" t="s">
         <v>265</v>
@@ -5087,13 +5093,13 @@
         <v>18</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>295</v>
+        <v>33</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F129" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G129" s="0" t="s">
         <v>264</v>
@@ -5102,7 +5108,7 @@
         <v>264</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>296</v>
+        <v>36</v>
       </c>
       <c r="J129" s="0" t="s">
         <v>265</v>
@@ -5119,7 +5125,7 @@
         <v>18</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>247</v>
@@ -5134,7 +5140,7 @@
         <v>264</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="J130" s="0" t="s">
         <v>265</v>
@@ -5186,7 +5192,7 @@
         <v>49</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F132" s="0" t="s">
         <v>256</v>
@@ -5218,7 +5224,7 @@
         <v>53</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F133" s="0" t="s">
         <v>258</v>
@@ -5282,7 +5288,7 @@
         <v>59</v>
       </c>
       <c r="E135" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F135" s="0" t="s">
         <v>261</v>
@@ -5442,7 +5448,7 @@
         <v>289</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F140" s="0" t="s">
         <v>237</v>
@@ -5468,16 +5474,16 @@
         <v>18</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>18</v>
+        <v>248</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>292</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>303</v>
+        <v>249</v>
       </c>
       <c r="F141" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G141" s="0" t="s">
         <v>268</v>
@@ -5486,7 +5492,7 @@
         <v>268</v>
       </c>
       <c r="I141" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J141" s="0" t="s">
         <v>271</v>
@@ -5503,13 +5509,13 @@
         <v>18</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="F142" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G142" s="0" t="s">
         <v>268</v>
@@ -5518,7 +5524,7 @@
         <v>268</v>
       </c>
       <c r="I142" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="J142" s="0" t="s">
         <v>271</v>
@@ -5535,13 +5541,13 @@
         <v>18</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>33</v>
+        <v>297</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F143" s="0" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G143" s="0" t="s">
         <v>268</v>
@@ -5550,7 +5556,7 @@
         <v>268</v>
       </c>
       <c r="I143" s="0" t="s">
-        <v>36</v>
+        <v>298</v>
       </c>
       <c r="J143" s="0" t="s">
         <v>271</v>
@@ -5567,13 +5573,13 @@
         <v>18</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>295</v>
+        <v>33</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F144" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G144" s="0" t="s">
         <v>268</v>
@@ -5582,7 +5588,7 @@
         <v>268</v>
       </c>
       <c r="I144" s="0" t="s">
-        <v>296</v>
+        <v>36</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>271</v>
@@ -5599,10 +5605,10 @@
         <v>18</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F145" s="0" t="s">
         <v>252</v>
@@ -5614,7 +5620,7 @@
         <v>268</v>
       </c>
       <c r="I145" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="J145" s="0" t="s">
         <v>271</v>
@@ -5762,7 +5768,7 @@
         <v>59</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F150" s="0" t="s">
         <v>261</v>

</xml_diff>